<commit_message>
added test for conversion of arguments for the load flow calculator
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,45 +458,67 @@
         <v>0.54861111111111105</v>
       </c>
       <c r="E3" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="F3" s="3">
         <f>(E3-D3)*24*60</f>
-        <v>230.00000000000014</v>
+        <v>320.00000000000011</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="3"/>
+      <c r="A4">
+        <v>2014</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="F4" s="3">
+        <f>(E4-D4)*24*60</f>
+        <v>120.00000000000006</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="3">
-        <f>SUM(F2:F4)</f>
-        <v>375.00000000000011</v>
-      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2">
-        <f>F5/60</f>
-        <v>6.2500000000000018</v>
+        <v>6</v>
+      </c>
+      <c r="F6" s="3">
+        <f>SUM(F2:F5)</f>
+        <v>585.00000000000023</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2">
+        <f>F6/60</f>
+        <v>9.7500000000000036</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="2">
-        <f>F6/38.5</f>
-        <v>0.16233766233766239</v>
+      <c r="F8" s="2">
+        <f>F7/38.5</f>
+        <v>0.25324675324675333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for load flow calculator
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,45 +480,67 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="E4" s="1">
-        <v>0.875</v>
+        <v>0.84722222222222221</v>
       </c>
       <c r="F4" s="3">
         <f>(E4-D4)*24*60</f>
-        <v>120.00000000000006</v>
+        <v>80.000000000000028</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="3"/>
+      <c r="A5">
+        <v>2014</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="3">
+        <f>(E5-D5)*24*60</f>
+        <v>234.99999999999997</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="3">
-        <f>SUM(F2:F5)</f>
-        <v>585.00000000000023</v>
-      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="2">
-        <f>F6/60</f>
-        <v>9.7500000000000036</v>
+        <v>6</v>
+      </c>
+      <c r="F7" s="3">
+        <f>SUM(F2:F6)</f>
+        <v>780.00000000000011</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2">
+        <f>F7/60</f>
+        <v>13.000000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="2">
-        <f>F7/38.5</f>
-        <v>0.25324675324675333</v>
+      <c r="F9" s="2">
+        <f>F8/38.5</f>
+        <v>0.33766233766233772</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first try to implement the current iteration
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,45 +502,67 @@
         <v>0.33680555555555558</v>
       </c>
       <c r="E5" s="1">
-        <v>0.5</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="F5" s="3">
         <f>(E5-D5)*24*60</f>
-        <v>234.99999999999997</v>
+        <v>310</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="3"/>
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F6" s="3">
+        <f>(E6-D6)*24*60</f>
+        <v>255.00000000000006</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="3">
-        <f>SUM(F2:F6)</f>
-        <v>780.00000000000011</v>
-      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="2">
-        <f>F7/60</f>
-        <v>13.000000000000002</v>
+        <v>6</v>
+      </c>
+      <c r="F8" s="3">
+        <f>SUM(F2:F7)</f>
+        <v>1110.0000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2">
+        <f>F8/60</f>
+        <v>18.500000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="2">
-        <f>F8/38.5</f>
-        <v>0.33766233766233772</v>
+      <c r="F10" s="2">
+        <f>F9/38.5</f>
+        <v>0.48051948051948062</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug in calculation of currents
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,45 +524,67 @@
         <v>0.57291666666666663</v>
       </c>
       <c r="E6" s="1">
-        <v>0.75</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="F6" s="3">
         <f>(E6-D6)*24*60</f>
-        <v>255.00000000000006</v>
+        <v>60.000000000000107</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="3"/>
+      <c r="A7">
+        <v>2014</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F7" s="3">
+        <f>(E7-D7)*24*60</f>
+        <v>180</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="3">
-        <f>SUM(F2:F7)</f>
-        <v>1110.0000000000002</v>
-      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="2">
-        <f>F8/60</f>
-        <v>18.500000000000004</v>
+        <v>6</v>
+      </c>
+      <c r="F9" s="3">
+        <f>SUM(F2:F8)</f>
+        <v>1095.0000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="2">
+        <f>F9/60</f>
+        <v>18.250000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="2">
-        <f>F9/38.5</f>
-        <v>0.48051948051948062</v>
+      <c r="F11" s="2">
+        <f>F10/38.5</f>
+        <v>0.47402597402597413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extracted static function for creating the power series of the exponential function
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +439,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f>(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F9" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="1"/>
@@ -461,7 +461,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="F3" s="3">
-        <f>(E3-D3)*24*60</f>
+        <f t="shared" si="0"/>
         <v>320.00000000000011</v>
       </c>
       <c r="G3" s="1"/>
@@ -483,7 +483,7 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="F4" s="3">
-        <f>(E4-D4)*24*60</f>
+        <f t="shared" si="0"/>
         <v>80.000000000000028</v>
       </c>
       <c r="G4" s="1"/>
@@ -505,7 +505,7 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="F5" s="3">
-        <f>(E5-D5)*24*60</f>
+        <f t="shared" si="0"/>
         <v>310</v>
       </c>
       <c r="G5" s="1"/>
@@ -527,7 +527,7 @@
         <v>0.61458333333333337</v>
       </c>
       <c r="F6" s="3">
-        <f>(E6-D6)*24*60</f>
+        <f t="shared" si="0"/>
         <v>60.000000000000107</v>
       </c>
       <c r="G6" s="1"/>
@@ -549,42 +549,86 @@
         <v>0.75</v>
       </c>
       <c r="F7" s="3">
-        <f>(E7-D7)*24*60</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="3"/>
+      <c r="A8">
+        <v>2014</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>59.999999999999943</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="4" t="s">
-        <v>6</v>
+      <c r="A9">
+        <v>2014</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.5</v>
       </c>
       <c r="F9" s="3">
-        <f>SUM(F2:F8)</f>
-        <v>1095.0000000000002</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>60.000000000000028</v>
+      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="2">
-        <f>F9/60</f>
-        <v>18.250000000000004</v>
-      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3">
+        <f>SUM(F2:F10)</f>
+        <v>1215.0000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2">
+        <f>F11/60</f>
+        <v>20.250000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="2">
-        <f>F10/38.5</f>
-        <v>0.47402597402597413</v>
+      <c r="F13" s="2">
+        <f>F12/38.5</f>
+        <v>0.52597402597402609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for load flow calculation
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +439,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F9" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F10" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="1"/>
@@ -599,36 +599,58 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="3"/>
+      <c r="A10">
+        <v>2014</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.78125</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>175.00000000000003</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="3">
-        <f>SUM(F2:F10)</f>
-        <v>1215.0000000000002</v>
-      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="2">
-        <f>F11/60</f>
-        <v>20.250000000000004</v>
+        <v>6</v>
+      </c>
+      <c r="F12" s="3">
+        <f>SUM(F2:F11)</f>
+        <v>1390.0000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="2">
+        <f>F12/60</f>
+        <v>23.166666666666671</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="2">
-        <f>F12/38.5</f>
-        <v>0.52597402597402609</v>
+      <c r="F14" s="2">
+        <f>F13/38.5</f>
+        <v>0.6017316017316019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added functions for creating vectors and matrices to the generic calculators
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +439,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F10" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F12" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="1"/>
@@ -621,36 +621,80 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="3"/>
+      <c r="A11">
+        <v>2014</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>105.00000000000003</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="4" t="s">
-        <v>6</v>
+      <c r="A12">
+        <v>2014</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.54166666666666663</v>
       </c>
       <c r="F12" s="3">
-        <f>SUM(F2:F11)</f>
-        <v>1330.0000000000002</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="2">
-        <f>F12/60</f>
-        <v>22.166666666666671</v>
-      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="3">
+        <f>SUM(F2:F13)</f>
+        <v>1480.0000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="2">
+        <f>F14/60</f>
+        <v>24.666666666666671</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="2">
-        <f>F13/38.5</f>
-        <v>0.57575757575757591</v>
+      <c r="F16" s="2">
+        <f>F15/38.5</f>
+        <v>0.64069264069264087</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented indexer for the power series
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +439,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F12" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F13" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="1"/>
@@ -665,36 +665,58 @@
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="3"/>
+      <c r="A13">
+        <v>2014</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>149.99999999999994</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="3">
-        <f>SUM(F2:F13)</f>
-        <v>1480.0000000000002</v>
-      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="2">
-        <f>F14/60</f>
-        <v>24.666666666666671</v>
+        <v>6</v>
+      </c>
+      <c r="F15" s="3">
+        <f>SUM(F2:F14)</f>
+        <v>1630.0000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="2">
+        <f>F15/60</f>
+        <v>27.166666666666671</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="2">
-        <f>F15/38.5</f>
-        <v>0.64069264069264087</v>
+      <c r="F17" s="2">
+        <f>F16/38.5</f>
+        <v>0.70562770562770571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug in calculation of q-coefficients
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>sum [working weeks]</t>
+  </si>
+  <si>
+    <t>time spent [h]</t>
   </si>
 </sst>
 </file>
@@ -391,15 +394,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -421,6 +425,9 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -439,10 +446,13 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F13" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F14" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="2">
+        <f>F2/60</f>
+        <v>2.4166666666666661</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -464,7 +474,10 @@
         <f t="shared" si="0"/>
         <v>320.00000000000011</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G14" si="1">F3/60</f>
+        <v>5.3333333333333348</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -486,7 +499,10 @@
         <f t="shared" si="0"/>
         <v>80.000000000000028</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333337</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -508,7 +524,10 @@
         <f t="shared" si="0"/>
         <v>310</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="2">
+        <f t="shared" si="1"/>
+        <v>5.166666666666667</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -530,7 +549,10 @@
         <f t="shared" si="0"/>
         <v>60.000000000000107</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000018</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -552,7 +574,10 @@
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -574,7 +599,10 @@
         <f t="shared" si="0"/>
         <v>59.999999999999943</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.999999999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -596,7 +624,10 @@
         <f t="shared" si="0"/>
         <v>60.000000000000028</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0000000000000004</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -618,7 +649,10 @@
         <f t="shared" si="0"/>
         <v>115.00000000000007</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9166666666666679</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -640,7 +674,10 @@
         <f t="shared" si="0"/>
         <v>105.00000000000003</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>1.7500000000000004</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -662,7 +699,10 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -684,39 +724,66 @@
         <f t="shared" si="0"/>
         <v>75.000000000000057</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2500000000000009</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="1"/>
+      <c r="A14">
+        <v>2014</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>209.99999999999989</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>3.4999999999999982</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="3">
-        <f>SUM(F2:F14)</f>
-        <v>1555.0000000000002</v>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="2">
-        <f>F15/60</f>
-        <v>25.916666666666671</v>
+        <v>6</v>
+      </c>
+      <c r="F16" s="3">
+        <f>SUM(F2:F15)</f>
+        <v>1765</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="2">
+        <f>F16/60</f>
+        <v>29.416666666666668</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="2">
-        <f>F16/38.5</f>
-        <v>0.67316017316017329</v>
+      <c r="F18" s="2">
+        <f>F17/38.5</f>
+        <v>0.76406926406926412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extracted functions for calculating the different coefficients
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F15" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F16" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="2">
@@ -475,7 +475,7 @@
         <v>320.00000000000011</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G15" si="1">F3/60</f>
+        <f t="shared" ref="G3:G16" si="1">F3/60</f>
         <v>5.3333333333333348</v>
       </c>
     </row>
@@ -780,35 +780,60 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="4" t="s">
+      <c r="A16">
+        <v>2014</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="0"/>
+        <v>59.999999999999943</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.999999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="3">
-        <f>SUM(F2:F16)</f>
-        <v>1705.0000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="3">
+        <f>SUM(F2:F17)</f>
+        <v>1765.0000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="2">
-        <f>F17/60</f>
-        <v>28.416666666666671</v>
-      </c>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="2">
+        <f>F18/60</f>
+        <v>29.416666666666671</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="2">
-        <f>F18/38.5</f>
-        <v>0.73809523809523825</v>
+      <c r="F20" s="2">
+        <f>F19/38.5</f>
+        <v>0.76406926406926423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
introduced usage of pade approximants for HELM
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -82,7 +82,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -90,6 +90,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +447,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F16" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F17" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="2">
@@ -475,7 +476,7 @@
         <v>320.00000000000011</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G16" si="1">F3/60</f>
+        <f t="shared" ref="G3:G17" si="1">F3/60</f>
         <v>5.3333333333333348</v>
       </c>
     </row>
@@ -804,36 +805,61 @@
         <v>0.999999999999999</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E18" s="4" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>2014</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>22</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="0"/>
+        <v>30.000000000000053</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.50000000000000089</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="3">
-        <f>SUM(F2:F17)</f>
-        <v>1765.0000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="3">
+        <f>SUM(F2:F18)</f>
+        <v>1795.0000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="2">
-        <f>F18/60</f>
-        <v>29.416666666666671</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="2">
+        <f>F19/60</f>
+        <v>29.916666666666671</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="2">
-        <f>F19/38.5</f>
-        <v>0.76406926406926423</v>
+      <c r="F21" s="2">
+        <f>F20/38.5</f>
+        <v>0.77705627705627722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made stuff static where ever possible
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -82,7 +82,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -90,7 +90,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +446,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F17" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F18" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="2">
@@ -476,7 +475,7 @@
         <v>320.00000000000011</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G17" si="1">F3/60</f>
+        <f t="shared" ref="G3:G18" si="1">F3/60</f>
         <v>5.3333333333333348</v>
       </c>
     </row>
@@ -806,7 +805,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17">
         <v>2014</v>
       </c>
       <c r="B17">
@@ -831,35 +830,60 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="3"/>
+      <c r="A18">
+        <v>2014</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="0"/>
+        <v>255.00000000000006</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>4.2500000000000009</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="3">
-        <f>SUM(F2:F18)</f>
-        <v>1795.0000000000002</v>
-      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="2">
-        <f>F19/60</f>
-        <v>29.916666666666671</v>
+        <v>6</v>
+      </c>
+      <c r="F20" s="3">
+        <f>SUM(F2:F19)</f>
+        <v>2050.0000000000005</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="2">
+        <f>F20/60</f>
+        <v>34.166666666666671</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="2">
-        <f>F20/38.5</f>
-        <v>0.77705627705627722</v>
+      <c r="F22" s="2">
+        <f>F21/38.5</f>
+        <v>0.88744588744588759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first implementation of the epsilon algorithm
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -396,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,15 +893,15 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="E20" s="1">
-        <v>0.875</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="0"/>
-        <v>165.00000000000006</v>
+        <v>135</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="1"/>
-        <v>2.7500000000000009</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -915,7 +915,7 @@
       </c>
       <c r="F22" s="3">
         <f>SUM(F2:F21)</f>
-        <v>2205.0000000000005</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -924,7 +924,7 @@
       </c>
       <c r="F23" s="2">
         <f>F22/60</f>
-        <v>36.750000000000007</v>
+        <v>36.25</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -933,7 +933,7 @@
       </c>
       <c r="F24" s="2">
         <f>F23/38.5</f>
-        <v>0.9545454545454547</v>
+        <v>0.94155844155844159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug: epsilon algorithm considers the partial sums, not the elements
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F20" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F21" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="2">
@@ -475,7 +475,7 @@
         <v>320.00000000000011</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G20" si="1">F3/60</f>
+        <f t="shared" ref="G3:G21" si="1">F3/60</f>
         <v>5.3333333333333348</v>
       </c>
     </row>
@@ -905,35 +905,60 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
+      <c r="A21">
+        <v>2014</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.90625</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.9375</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" s="3">
-        <f>SUM(F2:F21)</f>
-        <v>2175</v>
-      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="2">
-        <f>F22/60</f>
-        <v>36.25</v>
+        <v>6</v>
+      </c>
+      <c r="F23" s="3">
+        <f>SUM(F2:F22)</f>
+        <v>2220</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="2">
+        <f>F23/60</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="2">
-        <f>F23/38.5</f>
-        <v>0.94155844155844159</v>
+      <c r="F25" s="2">
+        <f>F24/38.5</f>
+        <v>0.96103896103896103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simplified tests for the analytic continuations
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F21" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F22" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="2">
@@ -475,7 +475,7 @@
         <v>320.00000000000011</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G21" si="1">F3/60</f>
+        <f t="shared" ref="G3:G22" si="1">F3/60</f>
         <v>5.3333333333333348</v>
       </c>
     </row>
@@ -930,35 +930,60 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
+      <c r="A22">
+        <v>2014</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>24</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="0"/>
+        <v>120.00000000000006</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000009</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="3">
-        <f>SUM(F2:F22)</f>
-        <v>2260</v>
-      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="2">
-        <f>F23/60</f>
-        <v>37.666666666666664</v>
+        <v>6</v>
+      </c>
+      <c r="F24" s="3">
+        <f>SUM(F2:F23)</f>
+        <v>2380</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="2">
+        <f>F24/60</f>
+        <v>39.666666666666664</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="2">
-        <f>F24/38.5</f>
-        <v>0.97835497835497831</v>
+      <c r="F26" s="2">
+        <f>F25/38.5</f>
+        <v>1.0303030303030303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests for the epsilon algorithm
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F22" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F23" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="2">
@@ -475,7 +475,7 @@
         <v>320.00000000000011</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G22" si="1">F3/60</f>
+        <f t="shared" ref="G3:G23" si="1">F3/60</f>
         <v>5.3333333333333348</v>
       </c>
     </row>
@@ -955,35 +955,60 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="3"/>
+      <c r="A23">
+        <v>2014</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>24</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="0"/>
+        <v>120.00000000000006</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000009</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="3">
-        <f>SUM(F2:F23)</f>
-        <v>2380</v>
-      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="2">
-        <f>F24/60</f>
-        <v>39.666666666666664</v>
+        <v>6</v>
+      </c>
+      <c r="F25" s="3">
+        <f>SUM(F2:F24)</f>
+        <v>2500</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="2">
+        <f>F25/60</f>
+        <v>41.666666666666664</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="2">
-        <f>F25/38.5</f>
-        <v>1.0303030303030303</v>
+      <c r="F27" s="2">
+        <f>F26/38.5</f>
+        <v>1.0822510822510822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed internal function of HELM
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F23" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F24" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="2">
@@ -475,7 +475,7 @@
         <v>320.00000000000011</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G23" si="1">F3/60</f>
+        <f t="shared" ref="G3:G24" si="1">F3/60</f>
         <v>5.3333333333333348</v>
       </c>
     </row>
@@ -968,47 +968,72 @@
         <v>0.75</v>
       </c>
       <c r="E23" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2014</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>24</v>
+      </c>
+      <c r="D24" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>120.00000000000006</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="1"/>
-        <v>2.0000000000000009</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="0"/>
+        <v>119.99999999999989</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>1.999999999999998</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="3">
-        <f>SUM(F2:F24)</f>
-        <v>2500</v>
-      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="2">
-        <f>F25/60</f>
-        <v>41.666666666666664</v>
+        <v>6</v>
+      </c>
+      <c r="F26" s="3">
+        <f>SUM(F2:F25)</f>
+        <v>2590</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="2">
+        <f>F26/60</f>
+        <v>43.166666666666664</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="2">
-        <f>F26/38.5</f>
-        <v>1.0822510822510822</v>
+      <c r="F28" s="2">
+        <f>F27/38.5</f>
+        <v>1.1212121212121211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added param to indicate voltage collapse
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F24" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F25" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="2">
@@ -475,7 +475,7 @@
         <v>320.00000000000011</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G24" si="1">F3/60</f>
+        <f t="shared" ref="G3:G25" si="1">F3/60</f>
         <v>5.3333333333333348</v>
       </c>
     </row>
@@ -1005,35 +1005,60 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="3"/>
+      <c r="A25">
+        <v>2014</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="1"/>
+        <v>2.25</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="3">
-        <f>SUM(F2:F25)</f>
-        <v>2620</v>
-      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="2">
-        <f>F26/60</f>
-        <v>43.666666666666664</v>
+        <v>6</v>
+      </c>
+      <c r="F27" s="3">
+        <f>SUM(F2:F26)</f>
+        <v>2755</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="2">
+        <f>F27/60</f>
+        <v>45.916666666666664</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="2">
-        <f>F27/38.5</f>
-        <v>1.1341991341991342</v>
+      <c r="F29" s="2">
+        <f>F28/38.5</f>
+        <v>1.1926406926406925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed useless constraint on the maximum number of coefficients for HELM
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
         <v>0.53125</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F25" si="0">(E2-D2)*24*60</f>
+        <f t="shared" ref="F2:F26" si="0">(E2-D2)*24*60</f>
         <v>144.99999999999997</v>
       </c>
       <c r="G2" s="2">
@@ -475,7 +475,7 @@
         <v>320.00000000000011</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G25" si="1">F3/60</f>
+        <f t="shared" ref="G3:G26" si="1">F3/60</f>
         <v>5.3333333333333348</v>
       </c>
     </row>
@@ -1030,35 +1030,60 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="3"/>
+      <c r="A26">
+        <v>2014</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="0"/>
+        <v>255.00000000000006</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="1"/>
+        <v>4.2500000000000009</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="3">
-        <f>SUM(F2:F26)</f>
-        <v>2755</v>
-      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="2">
-        <f>F27/60</f>
-        <v>45.916666666666664</v>
+        <v>6</v>
+      </c>
+      <c r="F28" s="3">
+        <f>SUM(F2:F27)</f>
+        <v>3010</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="2">
+        <f>F28/60</f>
+        <v>50.166666666666664</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="2">
-        <f>F28/38.5</f>
-        <v>1.1926406926406925</v>
+      <c r="F30" s="2">
+        <f>F29/38.5</f>
+        <v>1.303030303030303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved detection of voltage collapse
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -396,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,18 +1096,38 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F29" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28" si="3">F28/60</f>
+        <f t="shared" ref="G28:G29" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="3"/>
+      <c r="A29">
+        <v>2014</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.34375</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="2"/>
+        <v>284.99999999999994</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="3"/>
+        <v>4.7499999999999991</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
@@ -1120,7 +1140,7 @@
       </c>
       <c r="F31" s="3">
         <f>SUM(F2:F30)</f>
-        <v>3275</v>
+        <v>3560</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1129,7 +1149,7 @@
       </c>
       <c r="F32" s="2">
         <f>F31/60</f>
-        <v>54.583333333333336</v>
+        <v>59.333333333333336</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
@@ -1138,7 +1158,7 @@
       </c>
       <c r="F33" s="2">
         <f>F32/38.5</f>
-        <v>1.4177489177489178</v>
+        <v>1.5411255411255411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed feature that for certain nodes the calculation is stopped earlier
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F30" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F31" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G30" si="3">F28/60</f>
+        <f t="shared" ref="G28:G31" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1155,35 +1155,60 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
+      <c r="A31">
+        <v>2014</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>27</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="2"/>
+        <v>120.00000000000006</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="3"/>
+        <v>2.0000000000000009</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E32" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F32" s="3">
-        <f>SUM(F2:F31)</f>
-        <v>3630</v>
-      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E33" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="2">
-        <f>F32/60</f>
-        <v>60.5</v>
+        <v>6</v>
+      </c>
+      <c r="F33" s="3">
+        <f>SUM(F2:F32)</f>
+        <v>3750</v>
       </c>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="2">
+        <f>F33/60</f>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="2">
-        <f>F33/38.5</f>
-        <v>1.5714285714285714</v>
+      <c r="F35" s="2">
+        <f>F34/38.5</f>
+        <v>1.6233766233766234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added structure for newton-raphson method
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F31" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F32" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G31" si="3">F28/60</f>
+        <f t="shared" ref="G28:G32" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1180,35 +1180,60 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33" s="4" t="s">
+      <c r="A32">
+        <v>2014</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="3">
-        <f>SUM(F2:F32)</f>
-        <v>3705</v>
-      </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="4" t="s">
+      <c r="F34" s="3">
+        <f>SUM(F2:F33)</f>
+        <v>3795</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="2">
-        <f>F33/60</f>
-        <v>61.75</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E35" s="4" t="s">
+      <c r="F35" s="2">
+        <f>F34/60</f>
+        <v>63.25</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="2">
-        <f>F34/38.5</f>
-        <v>1.6038961038961039</v>
+      <c r="F36" s="2">
+        <f>F35/38.5</f>
+        <v>1.6428571428571428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
detected wrong calcluation of voltage changes in the fast decoupled load flow method
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F32" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F33" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G32" si="3">F28/60</f>
+        <f t="shared" ref="G28:G33" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1204,36 +1204,61 @@
         <v>1.2500000000000009</v>
       </c>
     </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="4" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2014</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" si="2"/>
+        <v>195.00000000000011</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="3"/>
+        <v>3.2500000000000018</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="3">
-        <f>SUM(F2:F33)</f>
-        <v>3780</v>
-      </c>
-    </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E35" s="4" t="s">
+      <c r="F35" s="3">
+        <f>SUM(F2:F34)</f>
+        <v>3975</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E36" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="2">
-        <f>F34/60</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E36" s="4" t="s">
+      <c r="F36" s="2">
+        <f>F35/60</f>
+        <v>66.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="2">
-        <f>F35/38.5</f>
-        <v>1.6363636363636365</v>
+      <c r="F37" s="2">
+        <f>F36/38.5</f>
+        <v>1.7207792207792207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved internal interface for jacobi matrix based methods
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F33" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F35" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G33" si="3">F28/60</f>
+        <f t="shared" ref="G28:G35" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1230,35 +1230,85 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="3"/>
+      <c r="A34">
+        <v>2014</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="2"/>
+        <v>10.000000000000124</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="3"/>
+        <v>0.16666666666666874</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E35" s="4" t="s">
-        <v>6</v>
+      <c r="A35">
+        <v>2014</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.5</v>
       </c>
       <c r="F35" s="3">
-        <f>SUM(F2:F34)</f>
-        <v>3975</v>
+        <f t="shared" si="2"/>
+        <v>114.99999999999999</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="3"/>
+        <v>1.9166666666666665</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="2">
-        <f>F35/60</f>
-        <v>66.25</v>
-      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="3">
+        <f>SUM(F2:F36)</f>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="2">
+        <f>F37/60</f>
+        <v>68.333333333333329</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E39" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="2">
-        <f>F36/38.5</f>
-        <v>1.7207792207792207</v>
+      <c r="F39" s="2">
+        <f>F38/38.5</f>
+        <v>1.7748917748917747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests for fast decoupled load flow method
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,15 +1268,15 @@
         <v>0.4201388888888889</v>
       </c>
       <c r="E35" s="1">
-        <v>0.5</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="2"/>
-        <v>114.99999999999999</v>
+        <v>99.999999999999972</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" si="3"/>
-        <v>1.9166666666666665</v>
+        <v>1.6666666666666663</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="F37" s="3">
         <f>SUM(F2:F36)</f>
-        <v>4100</v>
+        <v>4085</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1299,7 +1299,7 @@
       </c>
       <c r="F38" s="2">
         <f>F37/60</f>
-        <v>68.333333333333329</v>
+        <v>68.083333333333329</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="F39" s="2">
         <f>F38/38.5</f>
-        <v>1.7748917748917747</v>
+        <v>1.7683982683982682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for fast decoupled load flow method
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F36" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F37" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G36" si="3">F28/60</f>
+        <f t="shared" ref="G28:G37" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1305,35 +1305,60 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="3"/>
+      <c r="A37">
+        <v>2014</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F37" s="3">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E38" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" s="3">
-        <f>SUM(F2:F37)</f>
-        <v>4280</v>
-      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="2">
-        <f>F38/60</f>
-        <v>71.333333333333329</v>
+        <v>6</v>
+      </c>
+      <c r="F39" s="3">
+        <f>SUM(F2:F38)</f>
+        <v>4370</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="2">
+        <f>F39/60</f>
+        <v>72.833333333333329</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F40" s="2">
-        <f>F39/38.5</f>
-        <v>1.8528138528138527</v>
+      <c r="F41" s="2">
+        <f>F40/38.5</f>
+        <v>1.8917748917748916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for FDLF
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F37" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F38" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G37" si="3">F28/60</f>
+        <f t="shared" ref="G28:G38" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1318,47 +1318,72 @@
         <v>0.6875</v>
       </c>
       <c r="E37" s="1">
-        <v>0.75</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>59.999999999999943</v>
       </c>
       <c r="G37" s="2">
         <f t="shared" si="3"/>
-        <v>1.5</v>
+        <v>0.999999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="3"/>
+      <c r="A38">
+        <v>2014</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="F38" s="3">
+        <f t="shared" si="2"/>
+        <v>40.000000000000178</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666963</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E39" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="3">
-        <f>SUM(F2:F38)</f>
-        <v>4370</v>
-      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E40" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="2">
-        <f>F39/60</f>
-        <v>72.833333333333329</v>
+        <v>6</v>
+      </c>
+      <c r="F40" s="3">
+        <f>SUM(F2:F39)</f>
+        <v>4380</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="2">
+        <f>F40/60</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="2">
-        <f>F40/38.5</f>
-        <v>1.8917748917748916</v>
+      <c r="F42" s="2">
+        <f>F41/38.5</f>
+        <v>1.8961038961038961</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ui for comparison of methods
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F39" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F40" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G39" si="3">F28/60</f>
+        <f t="shared" ref="G28:G40" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1368,47 +1368,72 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="E39" s="1">
-        <v>0.54166666666666663</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="F39" s="3">
         <f t="shared" si="2"/>
-        <v>74.999999999999972</v>
+        <v>90.000000000000085</v>
       </c>
       <c r="G39" s="2">
         <f t="shared" si="3"/>
-        <v>1.2499999999999996</v>
+        <v>1.5000000000000013</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="3"/>
+      <c r="A40">
+        <v>2014</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" si="2"/>
+        <v>210.00000000000006</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="3"/>
+        <v>3.5000000000000009</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E41" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="3">
-        <f>SUM(F2:F40)</f>
-        <v>4440</v>
-      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="2">
-        <f>F41/60</f>
-        <v>74</v>
+        <v>6</v>
+      </c>
+      <c r="F42" s="3">
+        <f>SUM(F2:F41)</f>
+        <v>4665</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="2">
+        <f>F42/60</f>
+        <v>77.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E44" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="2">
-        <f>F42/38.5</f>
-        <v>1.9220779220779221</v>
+      <c r="F44" s="2">
+        <f>F43/38.5</f>
+        <v>2.0194805194805197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented seperation of PQ- and PV-buses
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,15 +1443,15 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="E42" s="1">
-        <v>0.91666666666666663</v>
+        <v>0.9375</v>
       </c>
       <c r="F42" s="3">
         <f t="shared" si="2"/>
-        <v>99.999999999999972</v>
+        <v>130.00000000000003</v>
       </c>
       <c r="G42" s="2">
         <f t="shared" si="3"/>
-        <v>1.6666666666666663</v>
+        <v>2.166666666666667</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="F44" s="3">
         <f>SUM(F2:F43)</f>
-        <v>4730</v>
+        <v>4760</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="F45" s="2">
         <f>F44/60</f>
-        <v>78.833333333333329</v>
+        <v>79.333333333333329</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="F46" s="2">
         <f>F45/38.5</f>
-        <v>2.0476190476190474</v>
+        <v>2.0606060606060606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test with one PV-bus
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F42" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F43" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G42" si="3">F28/60</f>
+        <f t="shared" ref="G28:G43" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1455,35 +1455,60 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="3"/>
+      <c r="A43">
+        <v>2014</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="2"/>
+        <v>164.99999999999997</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="3"/>
+        <v>2.7499999999999996</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E44" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F44" s="3">
-        <f>SUM(F2:F43)</f>
-        <v>4760</v>
-      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F45" s="2">
-        <f>F44/60</f>
-        <v>79.333333333333329</v>
+        <v>6</v>
+      </c>
+      <c r="F45" s="3">
+        <f>SUM(F2:F44)</f>
+        <v>4925</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="2">
+        <f>F45/60</f>
+        <v>82.083333333333329</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E47" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F46" s="2">
-        <f>F45/38.5</f>
-        <v>2.0606060606060606</v>
+      <c r="F47" s="2">
+        <f>F46/38.5</f>
+        <v>2.1320346320346317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved tests for HELM
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F43" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F44" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G43" si="3">F28/60</f>
+        <f t="shared" ref="G28:G44" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1462,53 +1462,78 @@
         <v>3</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D43" s="1">
         <v>0.38541666666666669</v>
       </c>
       <c r="E43" s="1">
-        <v>0.5</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="F43" s="3">
         <f t="shared" si="2"/>
-        <v>164.99999999999997</v>
+        <v>149.99999999999994</v>
       </c>
       <c r="G43" s="2">
         <f t="shared" si="3"/>
-        <v>2.7499999999999996</v>
+        <v>2.4999999999999991</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="3"/>
+      <c r="A44">
+        <v>2014</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="F44" s="3">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F45" s="3">
-        <f>SUM(F2:F44)</f>
-        <v>4925</v>
-      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E46" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="2">
-        <f>F45/60</f>
-        <v>82.083333333333329</v>
+        <v>6</v>
+      </c>
+      <c r="F46" s="3">
+        <f>SUM(F2:F45)</f>
+        <v>4955</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="2">
+        <f>F46/60</f>
+        <v>82.583333333333329</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E48" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F47" s="2">
-        <f>F46/38.5</f>
-        <v>2.1320346320346317</v>
+      <c r="F48" s="2">
+        <f>F47/38.5</f>
+        <v>2.1450216450216448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved tests for newton raphson
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F44" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F45" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G44" si="3">F28/60</f>
+        <f t="shared" ref="G28:G45" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1493,46 +1493,71 @@
         <v>0.53125</v>
       </c>
       <c r="E44" s="1">
-        <v>0.5625</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="F44" s="3">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>14.999999999999947</v>
       </c>
       <c r="G44" s="2">
         <f t="shared" si="3"/>
-        <v>0.75</v>
+        <v>0.24999999999999911</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="3"/>
+      <c r="A45">
+        <v>2014</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F45" s="3">
+        <f t="shared" si="2"/>
+        <v>29.999999999999893</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="3"/>
+        <v>0.49999999999999822</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E46" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F46" s="3">
-        <f>SUM(F2:F45)</f>
-        <v>4955</v>
-      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E47" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" s="2">
-        <f>F46/60</f>
-        <v>82.583333333333329</v>
+        <v>6</v>
+      </c>
+      <c r="F47" s="3">
+        <f>SUM(F2:F46)</f>
+        <v>4955</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="2">
+        <f>F47/60</f>
+        <v>82.583333333333329</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E49" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F48" s="2">
-        <f>F47/38.5</f>
+      <c r="F49" s="2">
+        <f>F48/38.5</f>
         <v>2.1450216450216448</v>
       </c>
     </row>

</xml_diff>

<commit_message>
extracted function for reducing the admittance matrix by known voltages
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F45" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F46" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G45" si="3">F28/60</f>
+        <f t="shared" ref="G28:G46" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1530,35 +1530,60 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="3"/>
+      <c r="A46">
+        <v>2014</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.84375</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F46" s="3">
+        <f t="shared" si="2"/>
+        <v>104.99999999999994</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="3"/>
+        <v>1.7499999999999991</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E47" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F47" s="3">
-        <f>SUM(F2:F46)</f>
-        <v>4955</v>
-      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E48" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="2">
-        <f>F47/60</f>
-        <v>82.583333333333329</v>
+        <v>6</v>
+      </c>
+      <c r="F48" s="3">
+        <f>SUM(F2:F47)</f>
+        <v>5060</v>
       </c>
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="2">
+        <f>F48/60</f>
+        <v>84.333333333333329</v>
+      </c>
+    </row>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E50" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F49" s="2">
-        <f>F48/38.5</f>
-        <v>2.1450216450216448</v>
+      <c r="F50" s="2">
+        <f>F49/38.5</f>
+        <v>2.1904761904761902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bound all algorithm settings which were left
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F46" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F47" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G46" si="3">F28/60</f>
+        <f t="shared" ref="G28:G47" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1555,35 +1555,60 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="3"/>
+      <c r="A47">
+        <v>2014</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F47" s="3">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333335</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E48" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F48" s="3">
-        <f>SUM(F2:F47)</f>
-        <v>5150</v>
-      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="2">
-        <f>F48/60</f>
-        <v>85.833333333333329</v>
+        <v>6</v>
+      </c>
+      <c r="F49" s="3">
+        <f>SUM(F2:F48)</f>
+        <v>5350</v>
       </c>
     </row>
     <row r="50" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="2">
+        <f>F49/60</f>
+        <v>89.166666666666671</v>
+      </c>
+    </row>
+    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E51" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F50" s="2">
-        <f>F49/38.5</f>
-        <v>2.2294372294372291</v>
+      <c r="F51" s="2">
+        <f>F50/38.5</f>
+        <v>2.3160173160173163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added data validation for all fields
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F47" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F48" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G47" si="3">F28/60</f>
+        <f t="shared" ref="G28:G48" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1568,47 +1568,72 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="E47" s="1">
-        <v>0.5</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="F47" s="3">
         <f t="shared" si="2"/>
-        <v>200</v>
+        <v>184.99999999999997</v>
       </c>
       <c r="G47" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333335</v>
+        <v>3.083333333333333</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E49" s="4" t="s">
+      <c r="A48">
+        <v>2014</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="2"/>
+        <v>329.99999999999994</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="3"/>
+        <v>5.4999999999999991</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E50" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F49" s="3">
-        <f>SUM(F2:F48)</f>
-        <v>5350</v>
-      </c>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E50" s="4" t="s">
+      <c r="F50" s="3">
+        <f>SUM(F2:F49)</f>
+        <v>5665</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E51" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F50" s="2">
-        <f>F49/60</f>
-        <v>89.166666666666671</v>
-      </c>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E51" s="4" t="s">
+      <c r="F51" s="2">
+        <f>F50/60</f>
+        <v>94.416666666666671</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E52" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F51" s="2">
-        <f>F50/38.5</f>
-        <v>2.3160173160173163</v>
+      <c r="F52" s="2">
+        <f>F51/38.5</f>
+        <v>2.4523809523809526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved calculation of results into own thread
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F48" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F49" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G48" si="3">F28/60</f>
+        <f t="shared" ref="G28:G49" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1562,7 +1562,7 @@
         <v>3</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D47" s="1">
         <v>0.3611111111111111</v>
@@ -1587,53 +1587,78 @@
         <v>3</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D48" s="1">
         <v>0.52083333333333337</v>
       </c>
       <c r="E48" s="1">
-        <v>0.75</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="F48" s="3">
         <f t="shared" si="2"/>
-        <v>329.99999999999994</v>
+        <v>360</v>
       </c>
       <c r="G48" s="2">
         <f t="shared" si="3"/>
-        <v>5.4999999999999991</v>
-      </c>
-    </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E50" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F50" s="3">
-        <f>SUM(F2:F49)</f>
-        <v>5665</v>
-      </c>
-    </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2014</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="F49" s="3">
+        <f t="shared" si="2"/>
+        <v>74.999999999999886</v>
+      </c>
+      <c r="G49" s="2">
+        <f t="shared" si="3"/>
+        <v>1.249999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="3">
+        <f>SUM(F2:F50)</f>
+        <v>5770</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E52" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="2">
-        <f>F50/60</f>
-        <v>94.416666666666671</v>
-      </c>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E52" s="4" t="s">
+      <c r="F52" s="2">
+        <f>F51/60</f>
+        <v>96.166666666666671</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E53" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F52" s="2">
-        <f>F51/38.5</f>
-        <v>2.4523809523809526</v>
+      <c r="F53" s="2">
+        <f>F52/38.5</f>
+        <v>2.497835497835498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved storage of calculation results
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F49" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F50" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G49" si="3">F28/60</f>
+        <f t="shared" ref="G28:G50" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1630,35 +1630,60 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="3"/>
+      <c r="A50">
+        <v>2014</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F50" s="3">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="G50" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E51" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F51" s="3">
-        <f>SUM(F2:F50)</f>
-        <v>5770</v>
-      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="3"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E52" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F52" s="2">
-        <f>F51/60</f>
-        <v>96.166666666666671</v>
+        <v>6</v>
+      </c>
+      <c r="F52" s="3">
+        <f>SUM(F2:F51)</f>
+        <v>6010</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" s="2">
+        <f>F52/60</f>
+        <v>100.16666666666667</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E54" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F53" s="2">
-        <f>F52/38.5</f>
-        <v>2.497835497835498</v>
+      <c r="F54" s="2">
+        <f>F53/38.5</f>
+        <v>2.6017316017316019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for newton raphson method
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,15 +1643,15 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E50" s="1">
-        <v>0.5</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="F50" s="3">
         <f t="shared" si="2"/>
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="G50" s="2">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1665,7 +1665,7 @@
       </c>
       <c r="F52" s="3">
         <f>SUM(F2:F51)</f>
-        <v>6010</v>
+        <v>6070</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="F53" s="2">
         <f>F52/60</f>
-        <v>100.16666666666667</v>
+        <v>101.16666666666667</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="F54" s="2">
         <f>F53/38.5</f>
-        <v>2.6017316017316019</v>
+        <v>2.6277056277056277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for FromPolarCoordinates with negative magnitude
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F50" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F51" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G50" si="3">F28/60</f>
+        <f t="shared" ref="G28:G51" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1655,35 +1655,60 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="3"/>
+      <c r="A51">
+        <v>2014</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <v>6</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="F51" s="3">
+        <f t="shared" si="2"/>
+        <v>29.999999999999893</v>
+      </c>
+      <c r="G51" s="2">
+        <f t="shared" si="3"/>
+        <v>0.49999999999999822</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E52" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F52" s="3">
-        <f>SUM(F2:F51)</f>
-        <v>6070</v>
-      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E53" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F53" s="2">
-        <f>F52/60</f>
-        <v>101.16666666666667</v>
+        <v>6</v>
+      </c>
+      <c r="F53" s="3">
+        <f>SUM(F2:F52)</f>
+        <v>6100</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="2">
+        <f>F53/60</f>
+        <v>101.66666666666667</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E55" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F54" s="2">
-        <f>F53/38.5</f>
-        <v>2.6277056277056277</v>
+      <c r="F55" s="2">
+        <f>F54/38.5</f>
+        <v>2.6406926406926408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented PV-bus for FDLF
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F52" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F53" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G52" si="3">F28/60</f>
+        <f t="shared" ref="G28:G53" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1693,47 +1693,72 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="E52" s="1">
-        <v>0.75</v>
+        <v>0.6875</v>
       </c>
       <c r="F52" s="3">
         <f t="shared" si="2"/>
-        <v>210.00000000000006</v>
+        <v>120.00000000000006</v>
       </c>
       <c r="G52" s="2">
         <f t="shared" si="3"/>
-        <v>3.5000000000000009</v>
+        <v>2.0000000000000009</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="3"/>
+      <c r="A53">
+        <v>2014</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="F53" s="3">
+        <f t="shared" si="2"/>
+        <v>60.000000000000107</v>
+      </c>
+      <c r="G53" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0000000000000018</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E54" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F54" s="3">
-        <f>SUM(F2:F53)</f>
-        <v>6315</v>
-      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E55" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F55" s="2">
-        <f>F54/60</f>
-        <v>105.25</v>
+        <v>6</v>
+      </c>
+      <c r="F55" s="3">
+        <f>SUM(F2:F54)</f>
+        <v>6285</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="2">
+        <f>F55/60</f>
+        <v>104.75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E57" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F56" s="2">
-        <f>F55/38.5</f>
-        <v>2.7337662337662336</v>
+      <c r="F57" s="2">
+        <f>F56/38.5</f>
+        <v>2.720779220779221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added voltage magnitudes for PV-buses as param
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F53" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F54" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G53" si="3">F28/60</f>
+        <f t="shared" ref="G28:G54" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1718,47 +1718,72 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="E53" s="1">
-        <v>0.77083333333333337</v>
+        <v>0.78125</v>
       </c>
       <c r="F53" s="3">
         <f t="shared" si="2"/>
-        <v>60.000000000000107</v>
+        <v>75.000000000000057</v>
       </c>
       <c r="G53" s="2">
         <f t="shared" si="3"/>
-        <v>1.0000000000000018</v>
+        <v>1.2500000000000009</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="3"/>
+      <c r="A54">
+        <v>2014</v>
+      </c>
+      <c r="B54">
+        <v>5</v>
+      </c>
+      <c r="C54">
+        <v>6</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F54" s="3">
+        <f t="shared" si="2"/>
+        <v>119.99999999999989</v>
+      </c>
+      <c r="G54" s="2">
+        <f t="shared" si="3"/>
+        <v>1.999999999999998</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E55" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F55" s="3">
-        <f>SUM(F2:F54)</f>
-        <v>6285</v>
-      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E56" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F56" s="2">
-        <f>F55/60</f>
-        <v>104.75</v>
+        <v>6</v>
+      </c>
+      <c r="F56" s="3">
+        <f>SUM(F2:F55)</f>
+        <v>6420</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" s="2">
+        <f>F56/60</f>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E58" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F57" s="2">
-        <f>F56/38.5</f>
-        <v>2.720779220779221</v>
+      <c r="F58" s="2">
+        <f>F57/38.5</f>
+        <v>2.779220779220779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests for load flow calculators
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F55" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F56" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G55" si="3">F28/60</f>
+        <f t="shared" ref="G28:G56" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1780,35 +1780,60 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="3"/>
+      <c r="A56">
+        <v>2014</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56">
+        <v>10</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0.34375</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F56" s="3">
+        <f t="shared" si="2"/>
+        <v>225</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="3"/>
+        <v>3.75</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E57" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F57" s="3">
-        <f>SUM(F2:F56)</f>
-        <v>6530</v>
-      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F58" s="2">
-        <f>F57/60</f>
-        <v>108.83333333333333</v>
+        <v>6</v>
+      </c>
+      <c r="F58" s="3">
+        <f>SUM(F2:F57)</f>
+        <v>6755</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F59" s="2">
+        <f>F58/60</f>
+        <v>112.58333333333333</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E60" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F59" s="2">
-        <f>F58/38.5</f>
-        <v>2.8268398268398269</v>
+      <c r="F60" s="2">
+        <f>F59/38.5</f>
+        <v>2.9242424242424243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prepared implementation of PV-buses in HELM
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F56" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F57" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G56" si="3">F28/60</f>
+        <f t="shared" ref="G28:G57" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1793,47 +1793,72 @@
         <v>0.34375</v>
       </c>
       <c r="E56" s="1">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="F56" s="3">
+        <f t="shared" si="2"/>
+        <v>114.99999999999999</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="3"/>
+        <v>1.9166666666666665</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2014</v>
+      </c>
+      <c r="B57">
+        <v>3</v>
+      </c>
+      <c r="C57">
+        <v>10</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E57" s="1">
         <v>0.5</v>
       </c>
-      <c r="F56" s="3">
-        <f t="shared" si="2"/>
-        <v>225</v>
-      </c>
-      <c r="G56" s="2">
-        <f t="shared" si="3"/>
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="3"/>
+      <c r="F57" s="3">
+        <f t="shared" si="2"/>
+        <v>74.999999999999972</v>
+      </c>
+      <c r="G57" s="2">
+        <f t="shared" si="3"/>
+        <v>1.2499999999999996</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E58" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F58" s="3">
-        <f>SUM(F2:F57)</f>
-        <v>6755</v>
-      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E59" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F59" s="2">
-        <f>F58/60</f>
-        <v>112.58333333333333</v>
+        <v>6</v>
+      </c>
+      <c r="F59" s="3">
+        <f>SUM(F2:F58)</f>
+        <v>6720</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="2">
+        <f>F59/60</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E61" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F60" s="2">
-        <f>F59/38.5</f>
-        <v>2.9242424242424243</v>
+      <c r="F61" s="2">
+        <f>F60/38.5</f>
+        <v>2.9090909090909092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first implementation of PV-buses for HELM
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1835,29 +1835,34 @@
       <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E59" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F59" s="3">
-        <f>SUM(F2:F58)</f>
-        <v>6720</v>
-      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E60" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F60" s="2">
-        <f>F59/60</f>
-        <v>112</v>
+        <v>6</v>
+      </c>
+      <c r="F60" s="3">
+        <f>SUM(F2:F59)</f>
+        <v>6720</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E61" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" s="2">
+        <f>F60/60</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E62" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F61" s="2">
-        <f>F60/38.5</f>
+      <c r="F62" s="2">
+        <f>F61/38.5</f>
         <v>2.9090909090909092</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added infrastructure for library in C++
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F57" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F59" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G57" si="3">F28/60</f>
+        <f t="shared" ref="G28:G59" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1830,40 +1830,85 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="3"/>
+      <c r="A58">
+        <v>2014</v>
+      </c>
+      <c r="B58">
+        <v>3</v>
+      </c>
+      <c r="C58">
+        <v>11</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F58" s="3">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="G58" s="2">
+        <f t="shared" si="3"/>
+        <v>2.25</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="3"/>
+      <c r="A59">
+        <v>2014</v>
+      </c>
+      <c r="B59">
+        <v>3</v>
+      </c>
+      <c r="C59">
+        <v>11</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F59" s="3">
+        <f t="shared" si="2"/>
+        <v>169.99999999999989</v>
+      </c>
+      <c r="G59" s="2">
+        <f t="shared" si="3"/>
+        <v>2.8333333333333313</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E60" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F60" s="3">
-        <f>SUM(F2:F59)</f>
-        <v>6810</v>
-      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="3"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E61" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F61" s="2">
-        <f>F60/60</f>
-        <v>113.5</v>
+        <v>6</v>
+      </c>
+      <c r="F61" s="3">
+        <f>SUM(F2:F60)</f>
+        <v>7115</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E62" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F62" s="2">
+        <f>F61/60</f>
+        <v>118.58333333333333</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E63" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F62" s="2">
-        <f>F61/38.5</f>
-        <v>2.948051948051948</v>
+      <c r="F63" s="2">
+        <f>F62/38.5</f>
+        <v>3.0800865800865798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented hand-over of data to the library
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F59" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F63" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G59" si="3">F28/60</f>
+        <f t="shared" ref="G28:G63" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1868,47 +1868,147 @@
         <v>0.79861111111111116</v>
       </c>
       <c r="E59" s="1">
-        <v>0.91666666666666663</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="F59" s="3">
         <f t="shared" si="2"/>
-        <v>169.99999999999989</v>
+        <v>129.99999999999986</v>
       </c>
       <c r="G59" s="2">
         <f t="shared" si="3"/>
-        <v>2.8333333333333313</v>
+        <v>2.1666666666666643</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="3"/>
+      <c r="A60">
+        <v>2014</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <v>11</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0.96875</v>
+      </c>
+      <c r="F60" s="3">
+        <f t="shared" si="2"/>
+        <v>225</v>
+      </c>
+      <c r="G60" s="2">
+        <f t="shared" si="3"/>
+        <v>3.75</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E61" s="4" t="s">
+      <c r="A61">
+        <v>2014</v>
+      </c>
+      <c r="B61">
+        <v>3</v>
+      </c>
+      <c r="C61">
+        <v>12</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F61" s="3">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="G61" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2014</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="C62">
+        <v>12</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F62" s="3">
+        <f t="shared" si="2"/>
+        <v>45.000000000000078</v>
+      </c>
+      <c r="G62" s="2">
+        <f t="shared" si="3"/>
+        <v>0.75000000000000133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2014</v>
+      </c>
+      <c r="B63">
+        <v>3</v>
+      </c>
+      <c r="C63">
+        <v>12</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F63" s="3">
+        <f t="shared" si="2"/>
+        <v>159.99999999999991</v>
+      </c>
+      <c r="G63" s="2">
+        <f t="shared" si="3"/>
+        <v>2.6666666666666652</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E65" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F61" s="3">
-        <f>SUM(F2:F60)</f>
-        <v>7115</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E62" s="4" t="s">
+      <c r="F65" s="3">
+        <f>SUM(F2:F64)</f>
+        <v>7595</v>
+      </c>
+    </row>
+    <row r="66" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E66" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F62" s="2">
-        <f>F61/60</f>
-        <v>118.58333333333333</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E63" s="4" t="s">
+      <c r="F66" s="2">
+        <f>F65/60</f>
+        <v>126.58333333333333</v>
+      </c>
+    </row>
+    <row r="67" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E67" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F63" s="2">
-        <f>F62/38.5</f>
-        <v>3.0800865800865798</v>
+      <c r="F67" s="2">
+        <f>F66/38.5</f>
+        <v>3.2878787878787876</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QR-decomposition is also handed over to the library
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F63" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F64" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G63" si="3">F28/60</f>
+        <f t="shared" ref="G28:G64" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -1968,47 +1968,72 @@
         <v>0.63888888888888895</v>
       </c>
       <c r="E63" s="1">
-        <v>0.75</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="F63" s="3">
         <f t="shared" si="2"/>
-        <v>159.99999999999991</v>
+        <v>189.99999999999997</v>
       </c>
       <c r="G63" s="2">
         <f t="shared" si="3"/>
-        <v>2.6666666666666652</v>
+        <v>3.1666666666666661</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E65" s="4" t="s">
+      <c r="A64">
+        <v>2014</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64">
+        <v>12</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="F64" s="3">
+        <f t="shared" si="2"/>
+        <v>120.00000000000006</v>
+      </c>
+      <c r="G64" s="2">
+        <f t="shared" si="3"/>
+        <v>2.0000000000000009</v>
+      </c>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E66" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F65" s="3">
-        <f>SUM(F2:F64)</f>
-        <v>7595</v>
-      </c>
-    </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E66" s="4" t="s">
+      <c r="F66" s="3">
+        <f>SUM(F2:F65)</f>
+        <v>7745</v>
+      </c>
+    </row>
+    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E67" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F66" s="2">
-        <f>F65/60</f>
-        <v>126.58333333333333</v>
-      </c>
-    </row>
-    <row r="67" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E67" s="4" t="s">
+      <c r="F67" s="2">
+        <f>F66/60</f>
+        <v>129.08333333333334</v>
+      </c>
+    </row>
+    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E68" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F67" s="2">
-        <f>F66/38.5</f>
-        <v>3.2878787878787876</v>
+      <c r="F68" s="2">
+        <f>F67/38.5</f>
+        <v>3.3528138528138531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated ignore settings for intelli-sense file
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,15 +1993,15 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="E64" s="1">
-        <v>0.875</v>
+        <v>0.8125</v>
       </c>
       <c r="F64" s="3">
         <f t="shared" si="2"/>
-        <v>120.00000000000006</v>
+        <v>30.000000000000053</v>
       </c>
       <c r="G64" s="2">
         <f t="shared" si="3"/>
-        <v>2.0000000000000009</v>
+        <v>0.50000000000000089</v>
       </c>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.25">
@@ -2015,7 +2015,7 @@
       </c>
       <c r="F66" s="3">
         <f>SUM(F2:F65)</f>
-        <v>7745</v>
+        <v>7655</v>
       </c>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.25">
@@ -2024,7 +2024,7 @@
       </c>
       <c r="F67" s="2">
         <f>F66/60</f>
-        <v>129.08333333333334</v>
+        <v>127.58333333333333</v>
       </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.25">
@@ -2033,7 +2033,7 @@
       </c>
       <c r="F68" s="2">
         <f>F67/38.5</f>
-        <v>3.3528138528138531</v>
+        <v>3.3138528138528138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first try to implement HELM in the library
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F64" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F65" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G64" si="3">F28/60</f>
+        <f t="shared" ref="G28:G65" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2004,36 +2004,61 @@
         <v>0.50000000000000089</v>
       </c>
     </row>
-    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E66" s="4" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2014</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <v>13</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="F65" s="3">
+        <f t="shared" si="2"/>
+        <v>150.00000000000011</v>
+      </c>
+      <c r="G65" s="2">
+        <f t="shared" si="3"/>
+        <v>2.5000000000000018</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E67" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F66" s="3">
-        <f>SUM(F2:F65)</f>
-        <v>7655</v>
-      </c>
-    </row>
-    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E67" s="4" t="s">
+      <c r="F67" s="3">
+        <f>SUM(F2:F66)</f>
+        <v>7805</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E68" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F67" s="2">
-        <f>F66/60</f>
-        <v>127.58333333333333</v>
-      </c>
-    </row>
-    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E68" s="4" t="s">
+      <c r="F68" s="2">
+        <f>F67/60</f>
+        <v>130.08333333333334</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E69" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F68" s="2">
-        <f>F67/38.5</f>
-        <v>3.3138528138528138</v>
+      <c r="F69" s="2">
+        <f>F68/38.5</f>
+        <v>3.3787878787878789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests for HELM-Coefficients
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F65" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F66" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G65" si="3">F28/60</f>
+        <f t="shared" ref="G28:G66" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2030,35 +2030,60 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="3"/>
+      <c r="A66">
+        <v>2014</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66">
+        <v>13</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0.78125</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="F66" s="3">
+        <f t="shared" si="2"/>
+        <v>25.000000000000071</v>
+      </c>
+      <c r="G66" s="2">
+        <f t="shared" si="3"/>
+        <v>0.41666666666666785</v>
+      </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E67" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F67" s="3">
-        <f>SUM(F2:F66)</f>
-        <v>7805</v>
-      </c>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="3"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E68" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F68" s="2">
-        <f>F67/60</f>
-        <v>130.08333333333334</v>
+        <v>6</v>
+      </c>
+      <c r="F68" s="3">
+        <f>SUM(F2:F67)</f>
+        <v>7830</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E69" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="2">
+        <f>F68/60</f>
+        <v>130.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E70" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F69" s="2">
-        <f>F68/38.5</f>
-        <v>3.3787878787878789</v>
+      <c r="F70" s="2">
+        <f>F69/38.5</f>
+        <v>3.3896103896103895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests with a real coefficient series for the epsilon-algorithm and the viskovatov algorithm
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F66" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F68" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G66" si="3">F28/60</f>
+        <f t="shared" ref="G28:G68" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2055,35 +2055,85 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="3"/>
+      <c r="A67">
+        <v>2014</v>
+      </c>
+      <c r="B67">
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <v>15</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="E67" s="1">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="F67" s="3">
+        <f t="shared" si="2"/>
+        <v>59.999999999999943</v>
+      </c>
+      <c r="G67" s="2">
+        <f t="shared" si="3"/>
+        <v>0.999999999999999</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E68" s="4" t="s">
-        <v>6</v>
+      <c r="A68">
+        <v>2014</v>
+      </c>
+      <c r="B68">
+        <v>3</v>
+      </c>
+      <c r="C68">
+        <v>15</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="E68" s="1">
+        <v>0.75</v>
       </c>
       <c r="F68" s="3">
-        <f>SUM(F2:F67)</f>
-        <v>7830</v>
+        <f t="shared" si="2"/>
+        <v>225</v>
+      </c>
+      <c r="G68" s="2">
+        <f t="shared" si="3"/>
+        <v>3.75</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E69" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F69" s="2">
-        <f>F68/60</f>
-        <v>130.5</v>
-      </c>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E70" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="3">
+        <f>SUM(F2:F69)</f>
+        <v>8115</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E71" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" s="2">
+        <f>F70/60</f>
+        <v>135.25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E72" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F70" s="2">
-        <f>F69/38.5</f>
-        <v>3.3896103896103895</v>
+      <c r="F72" s="2">
+        <f>F71/38.5</f>
+        <v>3.5129870129870131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented selection of result with smallest power error in HELM
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F68" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F69" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G68" si="3">F28/60</f>
+        <f t="shared" ref="G28:G69" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2093,47 +2093,72 @@
         <v>0.59375</v>
       </c>
       <c r="E68" s="1">
-        <v>0.75</v>
+        <v>0.80555555555555547</v>
       </c>
       <c r="F68" s="3">
         <f t="shared" si="2"/>
-        <v>225</v>
+        <v>304.99999999999989</v>
       </c>
       <c r="G68" s="2">
         <f t="shared" si="3"/>
-        <v>3.75</v>
+        <v>5.0833333333333313</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="3"/>
+      <c r="A69">
+        <v>2014</v>
+      </c>
+      <c r="B69">
+        <v>3</v>
+      </c>
+      <c r="C69">
+        <v>16</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="E69" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F69" s="3">
+        <f t="shared" si="2"/>
+        <v>194.99999999999994</v>
+      </c>
+      <c r="G69" s="2">
+        <f t="shared" si="3"/>
+        <v>3.2499999999999991</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E70" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F70" s="3">
-        <f>SUM(F2:F69)</f>
-        <v>8115</v>
-      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="3"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E71" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F71" s="2">
-        <f>F70/60</f>
-        <v>135.25</v>
+        <v>6</v>
+      </c>
+      <c r="F71" s="3">
+        <f>SUM(F2:F70)</f>
+        <v>8390</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E72" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72" s="2">
+        <f>F71/60</f>
+        <v>139.83333333333334</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E73" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F72" s="2">
-        <f>F71/38.5</f>
-        <v>3.5129870129870131</v>
+      <c r="F73" s="2">
+        <f>F72/38.5</f>
+        <v>3.6320346320346322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switched over to use eigen instead of boost-ublas
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F69" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F70" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G69" si="3">F28/60</f>
+        <f t="shared" ref="G28:G70" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2118,47 +2118,72 @@
         <v>0.40625</v>
       </c>
       <c r="E69" s="1">
-        <v>0.54166666666666663</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="F69" s="3">
         <f t="shared" si="2"/>
-        <v>194.99999999999994</v>
+        <v>210.00000000000006</v>
       </c>
       <c r="G69" s="2">
         <f t="shared" si="3"/>
-        <v>3.2499999999999991</v>
+        <v>3.5000000000000009</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="3"/>
+      <c r="A70">
+        <v>2014</v>
+      </c>
+      <c r="B70">
+        <v>3</v>
+      </c>
+      <c r="C70">
+        <v>16</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="E70" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F70" s="3">
+        <f t="shared" si="2"/>
+        <v>260.00000000000006</v>
+      </c>
+      <c r="G70" s="2">
+        <f t="shared" si="3"/>
+        <v>4.3333333333333339</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E71" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F71" s="3">
-        <f>SUM(F2:F70)</f>
-        <v>8390</v>
-      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="3"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E72" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F72" s="2">
-        <f>F71/60</f>
-        <v>139.83333333333334</v>
+        <v>6</v>
+      </c>
+      <c r="F72" s="3">
+        <f>SUM(F2:F71)</f>
+        <v>8665</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E73" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="2">
+        <f>F72/60</f>
+        <v>144.41666666666666</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E74" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F73" s="2">
-        <f>F72/38.5</f>
-        <v>3.6320346320346322</v>
+      <c r="F74" s="2">
+        <f>F73/38.5</f>
+        <v>3.7510822510822508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added MPIR for multi precision
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F70" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F72" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G70" si="3">F28/60</f>
+        <f t="shared" ref="G28:G72" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2143,47 +2143,97 @@
         <v>0.56944444444444442</v>
       </c>
       <c r="E70" s="1">
-        <v>0.75</v>
+        <v>0.6875</v>
       </c>
       <c r="F70" s="3">
         <f t="shared" si="2"/>
-        <v>260.00000000000006</v>
+        <v>170.00000000000003</v>
       </c>
       <c r="G70" s="2">
         <f t="shared" si="3"/>
-        <v>4.3333333333333339</v>
+        <v>2.8333333333333339</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="3"/>
+      <c r="A71">
+        <v>2014</v>
+      </c>
+      <c r="B71">
+        <v>3</v>
+      </c>
+      <c r="C71">
+        <v>16</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="E71" s="1">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="F71" s="3">
+        <f t="shared" si="2"/>
+        <v>69.999999999999915</v>
+      </c>
+      <c r="G71" s="2">
+        <f t="shared" si="3"/>
+        <v>1.1666666666666652</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E72" s="4" t="s">
-        <v>6</v>
+      <c r="A72">
+        <v>2014</v>
+      </c>
+      <c r="B72">
+        <v>3</v>
+      </c>
+      <c r="C72">
+        <v>17</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="E72" s="1">
+        <v>0.45833333333333331</v>
       </c>
       <c r="F72" s="3">
-        <f>SUM(F2:F71)</f>
-        <v>8665</v>
+        <f t="shared" si="2"/>
+        <v>94.999999999999986</v>
+      </c>
+      <c r="G72" s="2">
+        <f t="shared" si="3"/>
+        <v>1.583333333333333</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E73" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F73" s="2">
-        <f>F72/60</f>
-        <v>144.41666666666666</v>
-      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="3"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E74" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F74" s="3">
+        <f>SUM(F2:F73)</f>
+        <v>8740</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E75" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" s="2">
+        <f>F74/60</f>
+        <v>145.66666666666666</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E76" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F74" s="2">
-        <f>F73/38.5</f>
-        <v>3.7510822510822508</v>
+      <c r="F76" s="2">
+        <f>F75/38.5</f>
+        <v>3.7835497835497831</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started to implement wrapper for multi precision data type
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F72" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F73" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G72" si="3">F28/60</f>
+        <f t="shared" ref="G28:G73" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2193,47 +2193,72 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="E72" s="1">
-        <v>0.45833333333333331</v>
+        <v>0.46180555555555558</v>
       </c>
       <c r="F72" s="3">
         <f t="shared" si="2"/>
-        <v>94.999999999999986</v>
+        <v>100.00000000000004</v>
       </c>
       <c r="G72" s="2">
         <f t="shared" si="3"/>
-        <v>1.583333333333333</v>
+        <v>1.6666666666666674</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="3"/>
+      <c r="A73">
+        <v>2014</v>
+      </c>
+      <c r="B73">
+        <v>3</v>
+      </c>
+      <c r="C73">
+        <v>17</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="E73" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="F73" s="3">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="G73" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E74" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F74" s="3">
-        <f>SUM(F2:F73)</f>
-        <v>8740</v>
-      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="3"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E75" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F75" s="2">
-        <f>F74/60</f>
-        <v>145.66666666666666</v>
+        <v>6</v>
+      </c>
+      <c r="F75" s="3">
+        <f>SUM(F2:F74)</f>
+        <v>8835</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E76" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" s="2">
+        <f>F75/60</f>
+        <v>147.25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E77" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F76" s="2">
-        <f>F75/38.5</f>
-        <v>3.7835497835497831</v>
+      <c r="F77" s="2">
+        <f>F76/38.5</f>
+        <v>3.8246753246753249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replaced std::complex with custom complex class
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+      <selection activeCell="K73" sqref="K73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2218,15 +2218,15 @@
         <v>0.5625</v>
       </c>
       <c r="E73" s="1">
-        <v>0.625</v>
+        <v>0.62152777777777779</v>
       </c>
       <c r="F73" s="3">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>85.000000000000014</v>
       </c>
       <c r="G73" s="2">
         <f t="shared" si="3"/>
-        <v>1.5</v>
+        <v>1.416666666666667</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2240,7 +2240,7 @@
       </c>
       <c r="F75" s="3">
         <f>SUM(F2:F74)</f>
-        <v>8835</v>
+        <v>8830</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2249,7 +2249,7 @@
       </c>
       <c r="F76" s="2">
         <f>F75/60</f>
-        <v>147.25</v>
+        <v>147.16666666666666</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="F77" s="2">
         <f>F76/38.5</f>
-        <v>3.8246753246753249</v>
+        <v>3.8225108225108224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented necessary operators to get eigen working with custom datatypes
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="K73" sqref="K73"/>
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F73" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F75" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G73" si="3">F28/60</f>
+        <f t="shared" ref="G28:G75" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2230,35 +2230,85 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="3"/>
+      <c r="A74">
+        <v>2014</v>
+      </c>
+      <c r="B74">
+        <v>3</v>
+      </c>
+      <c r="C74">
+        <v>17</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F74" s="3">
+        <f t="shared" si="2"/>
+        <v>119.99999999999989</v>
+      </c>
+      <c r="G74" s="2">
+        <f t="shared" si="3"/>
+        <v>1.999999999999998</v>
+      </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E75" s="4" t="s">
-        <v>6</v>
+      <c r="A75">
+        <v>2014</v>
+      </c>
+      <c r="B75">
+        <v>3</v>
+      </c>
+      <c r="C75">
+        <v>17</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0.91666666666666663</v>
       </c>
       <c r="F75" s="3">
-        <f>SUM(F2:F74)</f>
-        <v>8830</v>
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="G75" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E76" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F76" s="2">
-        <f>F75/60</f>
-        <v>147.16666666666666</v>
-      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="3"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E77" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="3">
+        <f>SUM(F2:F76)</f>
+        <v>9040</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E78" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F78" s="2">
+        <f>F77/60</f>
+        <v>150.66666666666666</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E79" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F77" s="2">
-        <f>F76/38.5</f>
-        <v>3.8225108225108224</v>
+      <c r="F79" s="2">
+        <f>F78/38.5</f>
+        <v>3.9134199134199132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added framework for unit tests in the c++ library
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F75" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F76" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G75" si="3">F28/60</f>
+        <f t="shared" ref="G28:G76" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2268,47 +2268,72 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="E75" s="1">
-        <v>0.91666666666666663</v>
+        <v>0.93055555555555547</v>
       </c>
       <c r="F75" s="3">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>109.99999999999993</v>
       </c>
       <c r="G75" s="2">
         <f t="shared" si="3"/>
-        <v>1.5</v>
+        <v>1.8333333333333321</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="3"/>
+      <c r="A76">
+        <v>2014</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76">
+        <v>18</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F76" s="3">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="G76" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E77" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F77" s="3">
-        <f>SUM(F2:F76)</f>
-        <v>9040</v>
-      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="3"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E78" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F78" s="2">
-        <f>F77/60</f>
-        <v>150.66666666666666</v>
+        <v>6</v>
+      </c>
+      <c r="F78" s="3">
+        <f>SUM(F2:F77)</f>
+        <v>9240</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F79" s="2">
+        <f>F78/60</f>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E80" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F79" s="2">
-        <f>F78/38.5</f>
-        <v>3.9134199134199132</v>
+      <c r="F80" s="2">
+        <f>F79/38.5</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed temporary file from version control
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="J80" sqref="J80"/>
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F76" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F77" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G76" si="3">F28/60</f>
+        <f t="shared" ref="G28:G77" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2293,47 +2293,72 @@
         <v>0.375</v>
       </c>
       <c r="E76" s="1">
-        <v>0.5</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="F76" s="3">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>210.00000000000006</v>
       </c>
       <c r="G76" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>3.5000000000000009</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="3"/>
+      <c r="A77">
+        <v>2014</v>
+      </c>
+      <c r="B77">
+        <v>3</v>
+      </c>
+      <c r="C77">
+        <v>18</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E77" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="F77" s="3">
+        <f t="shared" si="2"/>
+        <v>120.00000000000006</v>
+      </c>
+      <c r="G77" s="2">
+        <f t="shared" si="3"/>
+        <v>2.0000000000000009</v>
+      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E78" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F78" s="3">
-        <f>SUM(F2:F77)</f>
-        <v>9240</v>
-      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="3"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E79" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F79" s="2">
-        <f>F78/60</f>
-        <v>154</v>
+        <v>6</v>
+      </c>
+      <c r="F79" s="3">
+        <f>SUM(F2:F78)</f>
+        <v>9390</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E80" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" s="2">
+        <f>F79/60</f>
+        <v>156.5</v>
+      </c>
+    </row>
+    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E81" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F80" s="2">
-        <f>F79/38.5</f>
-        <v>4</v>
+      <c r="F81" s="2">
+        <f>F80/38.5</f>
+        <v>4.0649350649350646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved performance of helm implementation
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F77" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F78" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G77" si="3">F28/60</f>
+        <f t="shared" ref="G28:G78" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2330,35 +2330,60 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="3"/>
+      <c r="A78">
+        <v>2014</v>
+      </c>
+      <c r="B78">
+        <v>3</v>
+      </c>
+      <c r="C78">
+        <v>19</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F78" s="3">
+        <f t="shared" si="2"/>
+        <v>194.99999999999994</v>
+      </c>
+      <c r="G78" s="2">
+        <f t="shared" si="3"/>
+        <v>3.2499999999999991</v>
+      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E79" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F79" s="3">
-        <f>SUM(F2:F78)</f>
-        <v>9390</v>
-      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="3"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E80" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F80" s="2">
-        <f>F79/60</f>
-        <v>156.5</v>
+        <v>6</v>
+      </c>
+      <c r="F80" s="3">
+        <f>SUM(F2:F79)</f>
+        <v>9585</v>
       </c>
     </row>
     <row r="81" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E81" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81" s="2">
+        <f>F80/60</f>
+        <v>159.75</v>
+      </c>
+    </row>
+    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E82" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F81" s="2">
-        <f>F80/38.5</f>
-        <v>4.0649350649350646</v>
+      <c r="F82" s="2">
+        <f>F81/38.5</f>
+        <v>4.1493506493506498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
selected best result based on power error in the C# implementation of HELM
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="N85" sqref="N85"/>
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2393,15 +2393,15 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="E80" s="1">
-        <v>0.51041666666666663</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="F80" s="3">
         <f t="shared" si="2"/>
-        <v>74.999999999999972</v>
+        <v>90.000000000000085</v>
       </c>
       <c r="G80" s="2">
         <f t="shared" si="3"/>
-        <v>1.2499999999999996</v>
+        <v>1.5000000000000013</v>
       </c>
     </row>
     <row r="81" spans="4:6" x14ac:dyDescent="0.25">
@@ -2415,7 +2415,7 @@
       </c>
       <c r="F82" s="3">
         <f>SUM(F2:F81)</f>
-        <v>9745</v>
+        <v>9760</v>
       </c>
     </row>
     <row r="83" spans="4:6" x14ac:dyDescent="0.25">
@@ -2424,7 +2424,7 @@
       </c>
       <c r="F83" s="2">
         <f>F82/60</f>
-        <v>162.41666666666666</v>
+        <v>162.66666666666666</v>
       </c>
     </row>
     <row r="84" spans="4:6" x14ac:dyDescent="0.25">
@@ -2433,7 +2433,7 @@
       </c>
       <c r="F84" s="2">
         <f>F83/38.5</f>
-        <v>4.2186147186147185</v>
+        <v>4.225108225108225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added high accuracy helm to the gui
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F80" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F81" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G80" si="3">F28/60</f>
+        <f t="shared" ref="G28:G81" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2404,36 +2404,61 @@
         <v>1.5000000000000013</v>
       </c>
     </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="3"/>
-    </row>
-    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E82" s="4" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2014</v>
+      </c>
+      <c r="B81">
+        <v>3</v>
+      </c>
+      <c r="C81">
+        <v>20</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="E81" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F81" s="3">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="G81" s="2">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E83" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F82" s="3">
-        <f>SUM(F2:F81)</f>
-        <v>9760</v>
-      </c>
-    </row>
-    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E83" s="4" t="s">
+      <c r="F83" s="3">
+        <f>SUM(F2:F82)</f>
+        <v>9805</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E84" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F83" s="2">
-        <f>F82/60</f>
-        <v>162.66666666666666</v>
-      </c>
-    </row>
-    <row r="84" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E84" s="4" t="s">
+      <c r="F84" s="2">
+        <f>F83/60</f>
+        <v>163.41666666666666</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E85" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F84" s="2">
-        <f>F83/38.5</f>
-        <v>4.225108225108225</v>
+      <c r="F85" s="2">
+        <f>F84/38.5</f>
+        <v>4.2445887445887447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replaced direct usage of inverse coefficients
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F82" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F83" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G82" si="3">F28/60</f>
+        <f t="shared" ref="G28:G83" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2443,47 +2443,72 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="E82" s="1">
-        <v>0.8125</v>
+        <v>0.875</v>
       </c>
       <c r="F82" s="3">
         <f t="shared" si="2"/>
-        <v>14.999999999999947</v>
+        <v>104.99999999999994</v>
       </c>
       <c r="G82" s="2">
         <f t="shared" si="3"/>
-        <v>0.24999999999999911</v>
+        <v>1.7499999999999991</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="3"/>
+      <c r="A83">
+        <v>2014</v>
+      </c>
+      <c r="B83">
+        <v>3</v>
+      </c>
+      <c r="C83">
+        <v>21</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E83" s="1">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="F83" s="3">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="G83" s="2">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E84" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F84" s="3">
-        <f>SUM(F2:F83)</f>
-        <v>9820</v>
-      </c>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="3"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E85" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F85" s="2">
-        <f>F84/60</f>
-        <v>163.66666666666666</v>
+        <v>6</v>
+      </c>
+      <c r="F85" s="3">
+        <f>SUM(F2:F84)</f>
+        <v>9955</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E86" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F86" s="2">
+        <f>F85/60</f>
+        <v>165.91666666666666</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E87" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F86" s="2">
-        <f>F85/38.5</f>
-        <v>4.2510822510822512</v>
+      <c r="F87" s="2">
+        <f>F86/38.5</f>
+        <v>4.3095238095238093</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved calculation of the actual voltages into the coefficient storage
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F84" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F85" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G84" si="3">F28/60</f>
+        <f t="shared" ref="G28:G85" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2505,35 +2505,60 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="3"/>
+      <c r="A85">
+        <v>2014</v>
+      </c>
+      <c r="B85">
+        <v>3</v>
+      </c>
+      <c r="C85">
+        <v>21</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="E85" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F85" s="3">
+        <f t="shared" si="2"/>
+        <v>159.99999999999991</v>
+      </c>
+      <c r="G85" s="2">
+        <f t="shared" si="3"/>
+        <v>2.6666666666666652</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E86" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F86" s="3">
-        <f>SUM(F2:F85)</f>
-        <v>10015</v>
-      </c>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="3"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E87" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F87" s="2">
-        <f>F86/60</f>
-        <v>166.91666666666666</v>
+        <v>6</v>
+      </c>
+      <c r="F87" s="3">
+        <f>SUM(F2:F86)</f>
+        <v>10175</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E88" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F88" s="2">
+        <f>F87/60</f>
+        <v>169.58333333333334</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E89" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F88" s="2">
-        <f>F87/38.5</f>
-        <v>4.3354978354978355</v>
+      <c r="F89" s="2">
+        <f>F88/38.5</f>
+        <v>4.4047619047619051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented calculation of combined coefficients
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F85" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F86" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G85" si="3">F28/60</f>
+        <f t="shared" ref="G28:G86" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2518,47 +2518,72 @@
         <v>0.63888888888888895</v>
       </c>
       <c r="E85" s="1">
-        <v>0.75</v>
+        <v>0.8125</v>
       </c>
       <c r="F85" s="3">
         <f t="shared" si="2"/>
-        <v>159.99999999999991</v>
+        <v>249.99999999999991</v>
       </c>
       <c r="G85" s="2">
         <f t="shared" si="3"/>
-        <v>2.6666666666666652</v>
+        <v>4.1666666666666652</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="3"/>
+      <c r="A86">
+        <v>2014</v>
+      </c>
+      <c r="B86">
+        <v>3</v>
+      </c>
+      <c r="C86">
+        <v>21</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E86" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F86" s="3">
+        <f t="shared" si="2"/>
+        <v>119.99999999999989</v>
+      </c>
+      <c r="G86" s="2">
+        <f t="shared" si="3"/>
+        <v>1.999999999999998</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E87" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F87" s="3">
-        <f>SUM(F2:F86)</f>
-        <v>10175</v>
-      </c>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="3"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E88" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F88" s="2">
-        <f>F87/60</f>
-        <v>169.58333333333334</v>
+        <v>6</v>
+      </c>
+      <c r="F88" s="3">
+        <f>SUM(F2:F87)</f>
+        <v>10385</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E89" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F89" s="2">
+        <f>F88/60</f>
+        <v>173.08333333333334</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E90" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F89" s="2">
-        <f>F88/38.5</f>
-        <v>4.4047619047619051</v>
+      <c r="F90" s="2">
+        <f>F89/38.5</f>
+        <v>4.4956709956709959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replaced C#-HELM-implementation in the comparison gui
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F86" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F87" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G86" si="3">F28/60</f>
+        <f t="shared" ref="G28:G87" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2543,47 +2543,72 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E86" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="F86" s="3">
+        <f t="shared" si="2"/>
+        <v>59.999999999999943</v>
+      </c>
+      <c r="G86" s="2">
+        <f t="shared" si="3"/>
+        <v>0.999999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>2014</v>
+      </c>
+      <c r="B87">
+        <v>3</v>
+      </c>
+      <c r="C87">
+        <v>21</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E87" s="1">
         <v>0.91666666666666663</v>
       </c>
-      <c r="F86" s="3">
-        <f t="shared" si="2"/>
-        <v>119.99999999999989</v>
-      </c>
-      <c r="G86" s="2">
-        <f t="shared" si="3"/>
-        <v>1.999999999999998</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="3"/>
+      <c r="F87" s="3">
+        <f t="shared" si="2"/>
+        <v>40.000000000000014</v>
+      </c>
+      <c r="G87" s="2">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666685</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E88" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F88" s="3">
-        <f>SUM(F2:F87)</f>
-        <v>10385</v>
-      </c>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="3"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E89" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F89" s="2">
-        <f>F88/60</f>
-        <v>173.08333333333334</v>
+        <v>6</v>
+      </c>
+      <c r="F89" s="3">
+        <f>SUM(F2:F88)</f>
+        <v>10365</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E90" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F90" s="2">
+        <f>F89/60</f>
+        <v>172.75</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E91" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F90" s="2">
-        <f>F89/38.5</f>
-        <v>4.4956709956709959</v>
+      <c r="F91" s="2">
+        <f>F90/38.5</f>
+        <v>4.4870129870129869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for coefficients of HELM
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F87" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F91" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G87" si="3">F28/60</f>
+        <f t="shared" ref="G28:G91" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2568,47 +2568,147 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="E87" s="1">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="F87" s="3">
+        <f t="shared" si="2"/>
+        <v>55.000000000000128</v>
+      </c>
+      <c r="G87" s="2">
+        <f t="shared" si="3"/>
+        <v>0.91666666666666885</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2014</v>
+      </c>
+      <c r="B88">
+        <v>3</v>
+      </c>
+      <c r="C88">
+        <v>23</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="F88" s="3">
+        <f t="shared" si="2"/>
+        <v>30.000000000000053</v>
+      </c>
+      <c r="G88" s="2">
+        <f t="shared" si="3"/>
+        <v>0.50000000000000089</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>2014</v>
+      </c>
+      <c r="B89">
+        <v>3</v>
+      </c>
+      <c r="C89">
+        <v>24</v>
+      </c>
+      <c r="D89" s="1">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="E89" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F89" s="3">
+        <f t="shared" si="2"/>
+        <v>49.999999999999986</v>
+      </c>
+      <c r="G89" s="2">
+        <f t="shared" si="3"/>
+        <v>0.83333333333333315</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2014</v>
+      </c>
+      <c r="B90">
+        <v>3</v>
+      </c>
+      <c r="C90">
+        <v>24</v>
+      </c>
+      <c r="D90" s="1">
+        <v>0.71180555555555547</v>
+      </c>
+      <c r="E90" s="1">
+        <v>0.78125</v>
+      </c>
+      <c r="F90" s="3">
+        <f t="shared" si="2"/>
+        <v>100.00000000000013</v>
+      </c>
+      <c r="G90" s="2">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666687</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>2014</v>
+      </c>
+      <c r="B91">
+        <v>3</v>
+      </c>
+      <c r="C91">
+        <v>24</v>
+      </c>
+      <c r="D91" s="1">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="E91" s="1">
         <v>0.91666666666666663</v>
       </c>
-      <c r="F87" s="3">
-        <f t="shared" si="2"/>
-        <v>40.000000000000014</v>
-      </c>
-      <c r="G87" s="2">
-        <f t="shared" si="3"/>
-        <v>0.66666666666666685</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="3"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E89" s="4" t="s">
+      <c r="F91" s="3">
+        <f t="shared" si="2"/>
+        <v>130.00000000000003</v>
+      </c>
+      <c r="G91" s="2">
+        <f t="shared" si="3"/>
+        <v>2.166666666666667</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="3"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E93" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F89" s="3">
-        <f>SUM(F2:F88)</f>
-        <v>10365</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E90" s="4" t="s">
+      <c r="F93" s="3">
+        <f>SUM(F2:F92)</f>
+        <v>10690</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E94" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F90" s="2">
-        <f>F89/60</f>
-        <v>172.75</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E91" s="4" t="s">
+      <c r="F94" s="2">
+        <f>F93/60</f>
+        <v>178.16666666666666</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E95" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F91" s="2">
-        <f>F90/38.5</f>
-        <v>4.4870129870129869</v>
+      <c r="F95" s="2">
+        <f>F94/38.5</f>
+        <v>4.6277056277056277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added check if result of experiment is correct
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F92" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F93" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G92" si="3">F28/60</f>
+        <f t="shared" ref="G28:G93" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2693,47 +2693,72 @@
         <v>0.38194444444444442</v>
       </c>
       <c r="E92" s="1">
-        <v>0.44791666666666669</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="F92" s="3">
         <f t="shared" si="2"/>
-        <v>95.000000000000057</v>
+        <v>60.000000000000028</v>
       </c>
       <c r="G92" s="2">
         <f t="shared" si="3"/>
-        <v>1.5833333333333344</v>
+        <v>1.0000000000000004</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="3"/>
+      <c r="A93">
+        <v>2014</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
+      </c>
+      <c r="C93">
+        <v>25</v>
+      </c>
+      <c r="D93" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E93" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F93" s="3">
+        <f t="shared" si="2"/>
+        <v>89.999999999999915</v>
+      </c>
+      <c r="G93" s="2">
+        <f t="shared" si="3"/>
+        <v>1.4999999999999987</v>
+      </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E94" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F94" s="3">
-        <f>SUM(F2:F93)</f>
-        <v>10785</v>
-      </c>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="3"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E95" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F95" s="2">
-        <f>F94/60</f>
-        <v>179.75</v>
+        <v>6</v>
+      </c>
+      <c r="F95" s="3">
+        <f>SUM(F2:F94)</f>
+        <v>10840</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E96" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F96" s="2">
+        <f>F95/60</f>
+        <v>180.66666666666666</v>
+      </c>
+    </row>
+    <row r="97" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E97" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F96" s="2">
-        <f>F95/38.5</f>
-        <v>4.6688311688311686</v>
+      <c r="F97" s="2">
+        <f>F96/38.5</f>
+        <v>4.6926406926406923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved readabiliy of formula in the experiment
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F93" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F94" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G93" si="3">F28/60</f>
+        <f t="shared" ref="G28:G94" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2718,47 +2718,72 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="E93" s="1">
-        <v>0.54166666666666663</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="F93" s="3">
         <f t="shared" si="2"/>
-        <v>89.999999999999915</v>
+        <v>134.99999999999991</v>
       </c>
       <c r="G93" s="2">
         <f t="shared" si="3"/>
-        <v>1.4999999999999987</v>
+        <v>2.2499999999999987</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="3"/>
+      <c r="A94">
+        <v>2014</v>
+      </c>
+      <c r="B94">
+        <v>3</v>
+      </c>
+      <c r="C94">
+        <v>25</v>
+      </c>
+      <c r="D94" s="1">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="E94" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F94" s="3">
+        <f t="shared" si="2"/>
+        <v>200.00000000000009</v>
+      </c>
+      <c r="G94" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333348</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E95" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F95" s="3">
-        <f>SUM(F2:F94)</f>
-        <v>10840</v>
-      </c>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="3"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E96" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F96" s="2">
-        <f>F95/60</f>
-        <v>180.66666666666666</v>
+        <v>6</v>
+      </c>
+      <c r="F96" s="3">
+        <f>SUM(F2:F95)</f>
+        <v>11085</v>
       </c>
     </row>
     <row r="97" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E97" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F97" s="2">
+        <f>F96/60</f>
+        <v>184.75</v>
+      </c>
+    </row>
+    <row r="98" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E98" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F97" s="2">
-        <f>F96/38.5</f>
-        <v>4.6926406926406923</v>
+      <c r="F98" s="2">
+        <f>F97/38.5</f>
+        <v>4.7987012987012987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed second coefficient of HELM
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -2743,15 +2743,15 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="E94" s="1">
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F94" s="3">
         <f t="shared" si="2"/>
-        <v>200.00000000000009</v>
+        <v>80.000000000000028</v>
       </c>
       <c r="G94" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333348</v>
+        <v>1.3333333333333337</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="F96" s="3">
         <f>SUM(F2:F95)</f>
-        <v>11085</v>
+        <v>10965</v>
       </c>
     </row>
     <row r="97" spans="5:6" x14ac:dyDescent="0.25">
@@ -2774,7 +2774,7 @@
       </c>
       <c r="F97" s="2">
         <f>F96/60</f>
-        <v>184.75</v>
+        <v>182.75</v>
       </c>
     </row>
     <row r="98" spans="5:6" x14ac:dyDescent="0.25">
@@ -2783,7 +2783,7 @@
       </c>
       <c r="F98" s="2">
         <f>F97/38.5</f>
-        <v>4.7987012987012987</v>
+        <v>4.7467532467532472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed coefficients for HELM in some cases
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,15 +2793,15 @@
         <v>0.69791666666666663</v>
       </c>
       <c r="E96" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F96" s="3">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="G96" s="2">
+        <f t="shared" si="3"/>
         <v>0.75</v>
-      </c>
-      <c r="F96" s="3">
-        <f t="shared" si="2"/>
-        <v>75.000000000000057</v>
-      </c>
-      <c r="G96" s="2">
-        <f t="shared" si="3"/>
-        <v>1.2500000000000009</v>
       </c>
     </row>
     <row r="97" spans="4:6" x14ac:dyDescent="0.25">
@@ -2815,7 +2815,7 @@
       </c>
       <c r="F98" s="3">
         <f>SUM(F2:F97)</f>
-        <v>11130</v>
+        <v>11100</v>
       </c>
     </row>
     <row r="99" spans="4:6" x14ac:dyDescent="0.25">
@@ -2824,7 +2824,7 @@
       </c>
       <c r="F99" s="2">
         <f>F98/60</f>
-        <v>185.5</v>
+        <v>185</v>
       </c>
     </row>
     <row r="100" spans="4:6" x14ac:dyDescent="0.25">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="F100" s="2">
         <f>F99/38.5</f>
-        <v>4.8181818181818183</v>
+        <v>4.8051948051948052</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for Complex
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,15 +2818,15 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="E97" s="1">
-        <v>0.5</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="F97" s="3">
         <f t="shared" si="2"/>
-        <v>150.00000000000003</v>
+        <v>209.99999999999997</v>
       </c>
       <c r="G97" s="2">
         <f t="shared" si="3"/>
-        <v>2.5000000000000004</v>
+        <v>3.4999999999999996</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -2840,7 +2840,7 @@
       </c>
       <c r="F99" s="3">
         <f>SUM(F2:F98)</f>
-        <v>11250</v>
+        <v>11310</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -2849,7 +2849,7 @@
       </c>
       <c r="F100" s="2">
         <f>F99/60</f>
-        <v>187.5</v>
+        <v>188.5</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -2858,7 +2858,7 @@
       </c>
       <c r="F101" s="2">
         <f>F100/38.5</f>
-        <v>4.8701298701298699</v>
+        <v>4.8961038961038961</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increased count of coefficients for one test
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+      <selection activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F97" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F99" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G97" si="3">F28/60</f>
+        <f t="shared" ref="G28:G99" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2830,35 +2830,85 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="3"/>
+      <c r="A98">
+        <v>2014</v>
+      </c>
+      <c r="B98">
+        <v>3</v>
+      </c>
+      <c r="C98">
+        <v>27</v>
+      </c>
+      <c r="D98" s="1">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="E98" s="1">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="F98" s="3">
+        <f t="shared" si="2"/>
+        <v>145.00000000000011</v>
+      </c>
+      <c r="G98" s="2">
+        <f t="shared" si="3"/>
+        <v>2.4166666666666687</v>
+      </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E99" s="4" t="s">
-        <v>6</v>
+      <c r="A99">
+        <v>2014</v>
+      </c>
+      <c r="B99">
+        <v>3</v>
+      </c>
+      <c r="C99">
+        <v>28</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="E99" s="1">
+        <v>0.40625</v>
       </c>
       <c r="F99" s="3">
-        <f>SUM(F2:F98)</f>
-        <v>11310</v>
+        <f t="shared" si="2"/>
+        <v>84.999999999999943</v>
+      </c>
+      <c r="G99" s="2">
+        <f t="shared" si="3"/>
+        <v>1.4166666666666656</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E100" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F100" s="2">
-        <f>F99/60</f>
-        <v>188.5</v>
-      </c>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="3"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E101" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F101" s="3">
+        <f>SUM(F2:F100)</f>
+        <v>11540</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E102" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F102" s="2">
+        <f>F101/60</f>
+        <v>192.33333333333334</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E103" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F101" s="2">
-        <f>F100/38.5</f>
-        <v>4.8961038961038961</v>
+      <c r="F103" s="2">
+        <f>F102/38.5</f>
+        <v>4.9956709956709959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for update of analytic continuation
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:G103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="F99" sqref="F99"/>
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2868,15 +2868,15 @@
         <v>0.34722222222222227</v>
       </c>
       <c r="E99" s="1">
-        <v>0.40625</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="F99" s="3">
         <f t="shared" si="2"/>
-        <v>84.999999999999943</v>
+        <v>69.999999999999915</v>
       </c>
       <c r="G99" s="2">
         <f t="shared" si="3"/>
-        <v>1.4166666666666656</v>
+        <v>1.1666666666666652</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -2890,7 +2890,7 @@
       </c>
       <c r="F101" s="3">
         <f>SUM(F2:F100)</f>
-        <v>11540</v>
+        <v>11525</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -2899,7 +2899,7 @@
       </c>
       <c r="F102" s="2">
         <f>F101/60</f>
-        <v>192.33333333333334</v>
+        <v>192.08333333333334</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -2908,7 +2908,7 @@
       </c>
       <c r="F103" s="2">
         <f>F102/38.5</f>
-        <v>4.9956709956709959</v>
+        <v>4.9891774891774894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved performance of HELM through reduction of redundancy in analytic continuation
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G103"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100"/>
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F99" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F101" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G99" si="3">F28/60</f>
+        <f t="shared" ref="G28:G101" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2880,35 +2880,85 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="3"/>
+      <c r="A100">
+        <v>2014</v>
+      </c>
+      <c r="B100">
+        <v>3</v>
+      </c>
+      <c r="C100">
+        <v>29</v>
+      </c>
+      <c r="D100" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="F100" s="3">
+        <f t="shared" si="2"/>
+        <v>30.000000000000053</v>
+      </c>
+      <c r="G100" s="2">
+        <f t="shared" si="3"/>
+        <v>0.50000000000000089</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E101" s="4" t="s">
-        <v>6</v>
+      <c r="A101">
+        <v>2014</v>
+      </c>
+      <c r="B101">
+        <v>3</v>
+      </c>
+      <c r="C101">
+        <v>29</v>
+      </c>
+      <c r="D101" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E101" s="1">
+        <v>0.79166666666666663</v>
       </c>
       <c r="F101" s="3">
-        <f>SUM(F2:F100)</f>
-        <v>11525</v>
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="G101" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E102" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F102" s="2">
-        <f>F101/60</f>
-        <v>192.08333333333334</v>
-      </c>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="3"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E103" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F103" s="3">
+        <f>SUM(F2:F102)</f>
+        <v>11735</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E104" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F104" s="2">
+        <f>F103/60</f>
+        <v>195.58333333333334</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E105" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F103" s="2">
-        <f>F102/38.5</f>
-        <v>4.9891774891774894</v>
+      <c r="F105" s="2">
+        <f>F104/38.5</f>
+        <v>5.0800865800865802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prepared usage of dense QR-decomposition
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F101" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F102" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G101" si="3">F28/60</f>
+        <f t="shared" ref="G28:G102" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2930,35 +2930,60 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="3"/>
+      <c r="A102">
+        <v>2014</v>
+      </c>
+      <c r="B102">
+        <v>3</v>
+      </c>
+      <c r="C102">
+        <v>29</v>
+      </c>
+      <c r="D102" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E102" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="F102" s="3">
+        <f t="shared" si="2"/>
+        <v>59.999999999999943</v>
+      </c>
+      <c r="G102" s="2">
+        <f t="shared" si="3"/>
+        <v>0.999999999999999</v>
+      </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E103" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F103" s="3">
-        <f>SUM(F2:F102)</f>
-        <v>11735</v>
-      </c>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="3"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E104" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F104" s="2">
-        <f>F103/60</f>
-        <v>195.58333333333334</v>
+        <v>6</v>
+      </c>
+      <c r="F104" s="3">
+        <f>SUM(F2:F103)</f>
+        <v>11795</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E105" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F105" s="2">
+        <f>F104/60</f>
+        <v>196.58333333333334</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E106" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F105" s="2">
-        <f>F104/38.5</f>
-        <v>5.0800865800865802</v>
+      <c r="F106" s="2">
+        <f>F105/38.5</f>
+        <v>5.1060606060606064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added data grid for node voltages
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103"/>
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F102" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F103" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G102" si="3">F28/60</f>
+        <f t="shared" ref="G28:G103" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2955,35 +2955,60 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
-      <c r="F103" s="3"/>
+      <c r="A103">
+        <v>2014</v>
+      </c>
+      <c r="B103">
+        <v>3</v>
+      </c>
+      <c r="C103">
+        <v>30</v>
+      </c>
+      <c r="D103" s="1">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="E103" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F103" s="3">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="G103" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E104" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F104" s="3">
-        <f>SUM(F2:F103)</f>
-        <v>11885</v>
-      </c>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="3"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E105" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F105" s="2">
-        <f>F104/60</f>
-        <v>198.08333333333334</v>
+        <v>6</v>
+      </c>
+      <c r="F105" s="3">
+        <f>SUM(F2:F104)</f>
+        <v>11975</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E106" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F106" s="2">
+        <f>F105/60</f>
+        <v>199.58333333333334</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E107" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F106" s="2">
-        <f>F105/38.5</f>
-        <v>5.1450216450216448</v>
+      <c r="F107" s="2">
+        <f>F106/38.5</f>
+        <v>5.1839826839826841</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added difference in voltage magnitude for PV-buses to the total relative error
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2968,15 +2968,15 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="E103" s="1">
-        <v>0.91666666666666663</v>
+        <v>0.92013888888888884</v>
       </c>
       <c r="F103" s="3">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>94.999999999999986</v>
       </c>
       <c r="G103" s="2">
         <f t="shared" si="3"/>
-        <v>1.5</v>
+        <v>1.583333333333333</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="F105" s="3">
         <f>SUM(F2:F104)</f>
-        <v>11975</v>
+        <v>11980</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -2999,7 +2999,7 @@
       </c>
       <c r="F106" s="2">
         <f>F105/60</f>
-        <v>199.58333333333334</v>
+        <v>199.66666666666666</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="F107" s="2">
         <f>F106/38.5</f>
-        <v>5.1839826839826841</v>
+        <v>5.1861471861471857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented possibility to select the bit precision in the comparison-gui
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F103" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F105" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G103" si="3">F28/60</f>
+        <f t="shared" ref="G28:G105" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2980,35 +2980,85 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="3"/>
+      <c r="A104">
+        <v>2014</v>
+      </c>
+      <c r="B104">
+        <v>3</v>
+      </c>
+      <c r="C104">
+        <v>31</v>
+      </c>
+      <c r="D104" s="1">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E104" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F104" s="3">
+        <f t="shared" si="2"/>
+        <v>225.00000000000009</v>
+      </c>
+      <c r="G104" s="2">
+        <f t="shared" si="3"/>
+        <v>3.7500000000000013</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E105" s="4" t="s">
-        <v>6</v>
+      <c r="A105">
+        <v>2014</v>
+      </c>
+      <c r="B105">
+        <v>3</v>
+      </c>
+      <c r="C105">
+        <v>31</v>
+      </c>
+      <c r="D105" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="E105" s="1">
+        <v>0.66666666666666663</v>
       </c>
       <c r="F105" s="3">
-        <f>SUM(F2:F104)</f>
-        <v>11980</v>
+        <f t="shared" si="2"/>
+        <v>104.99999999999994</v>
+      </c>
+      <c r="G105" s="2">
+        <f t="shared" si="3"/>
+        <v>1.7499999999999991</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E106" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F106" s="2">
-        <f>F105/60</f>
-        <v>199.66666666666666</v>
-      </c>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="3"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E107" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F107" s="3">
+        <f>SUM(F2:F106)</f>
+        <v>12310</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E108" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F108" s="2">
+        <f>F107/60</f>
+        <v>205.16666666666666</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E109" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F107" s="2">
-        <f>F106/38.5</f>
-        <v>5.1861471861471857</v>
+      <c r="F109" s="2">
+        <f>F108/38.5</f>
+        <v>5.329004329004329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increased precision for test
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F105" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F106" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G105" si="3">F28/60</f>
+        <f t="shared" ref="G28:G106" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -3018,47 +3018,72 @@
         <v>0.59375</v>
       </c>
       <c r="E105" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.64930555555555558</v>
       </c>
       <c r="F105" s="3">
         <f t="shared" si="2"/>
-        <v>104.99999999999994</v>
+        <v>80.000000000000028</v>
       </c>
       <c r="G105" s="2">
         <f t="shared" si="3"/>
-        <v>1.7499999999999991</v>
+        <v>1.3333333333333337</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
-      <c r="F106" s="3"/>
+      <c r="A106">
+        <v>2014</v>
+      </c>
+      <c r="B106">
+        <v>3</v>
+      </c>
+      <c r="C106">
+        <v>31</v>
+      </c>
+      <c r="D106" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="E106" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F106" s="3">
+        <f t="shared" si="2"/>
+        <v>74.999999999999886</v>
+      </c>
+      <c r="G106" s="2">
+        <f t="shared" si="3"/>
+        <v>1.249999999999998</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E107" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F107" s="3">
-        <f>SUM(F2:F106)</f>
-        <v>12310</v>
-      </c>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="3"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E108" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F108" s="2">
-        <f>F107/60</f>
-        <v>205.16666666666666</v>
+        <v>6</v>
+      </c>
+      <c r="F108" s="3">
+        <f>SUM(F2:F107)</f>
+        <v>12360</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E109" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F109" s="2">
+        <f>F108/60</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E110" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F109" s="2">
-        <f>F108/38.5</f>
-        <v>5.329004329004329</v>
+      <c r="F110" s="2">
+        <f>F109/38.5</f>
+        <v>5.3506493506493502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added node potential method for initial voltages in FDLF and newton raphson
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -3043,15 +3043,15 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="E106" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.78472222222222221</v>
       </c>
       <c r="F106" s="3">
         <f t="shared" si="2"/>
-        <v>74.999999999999886</v>
+        <v>64.999999999999929</v>
       </c>
       <c r="G106" s="2">
         <f t="shared" si="3"/>
-        <v>1.249999999999998</v>
+        <v>1.0833333333333321</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3065,7 +3065,7 @@
       </c>
       <c r="F108" s="3">
         <f>SUM(F2:F107)</f>
-        <v>12360</v>
+        <v>12350</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -3074,7 +3074,7 @@
       </c>
       <c r="F109" s="2">
         <f>F108/60</f>
-        <v>206</v>
+        <v>205.83333333333334</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3083,7 +3083,7 @@
       </c>
       <c r="F110" s="2">
         <f>F109/38.5</f>
-        <v>5.3506493506493502</v>
+        <v>5.3463203463203461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added example with one PV- and one PQ-bus
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F106" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F108" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G106" si="3">F28/60</f>
+        <f t="shared" ref="G28:G108" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -3055,35 +3055,85 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
-      <c r="F107" s="3"/>
+      <c r="A107">
+        <v>2014</v>
+      </c>
+      <c r="B107">
+        <v>3</v>
+      </c>
+      <c r="C107">
+        <v>31</v>
+      </c>
+      <c r="D107" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="E107" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="F107" s="3">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="G107" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E108" s="4" t="s">
-        <v>6</v>
+      <c r="A108">
+        <v>2014</v>
+      </c>
+      <c r="B108">
+        <v>4</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="D108" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0.64583333333333337</v>
       </c>
       <c r="F108" s="3">
-        <f>SUM(F2:F107)</f>
-        <v>12350</v>
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="G108" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E109" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F109" s="2">
-        <f>F108/60</f>
-        <v>205.83333333333334</v>
-      </c>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="3"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E110" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F110" s="3">
+        <f>SUM(F2:F109)</f>
+        <v>12530</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E111" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F111" s="2">
+        <f>F110/60</f>
+        <v>208.83333333333334</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E112" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F110" s="2">
-        <f>F109/38.5</f>
-        <v>5.3463203463203461</v>
+      <c r="F112" s="2">
+        <f>F111/38.5</f>
+        <v>5.4242424242424248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests for load flow calculators with one PV- and one PQ-bus
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F108" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F109" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G108" si="3">F28/60</f>
+        <f t="shared" ref="G28:G109" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -3093,47 +3093,72 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E108" s="1">
-        <v>0.64583333333333337</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="F108" s="3">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>29.999999999999893</v>
       </c>
       <c r="G108" s="2">
         <f t="shared" si="3"/>
-        <v>1.5</v>
+        <v>0.49999999999999822</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
-      <c r="F109" s="3"/>
+      <c r="A109">
+        <v>2014</v>
+      </c>
+      <c r="B109">
+        <v>4</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="E109" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F109" s="3">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="G109" s="2">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E110" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F110" s="3">
-        <f>SUM(F2:F109)</f>
-        <v>12530</v>
-      </c>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="3"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E111" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F111" s="2">
-        <f>F110/60</f>
-        <v>208.83333333333334</v>
+        <v>6</v>
+      </c>
+      <c r="F111" s="3">
+        <f>SUM(F2:F110)</f>
+        <v>12515</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E112" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F112" s="2">
+        <f>F111/60</f>
+        <v>208.58333333333334</v>
+      </c>
+    </row>
+    <row r="113" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E113" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F112" s="2">
-        <f>F111/38.5</f>
-        <v>5.4242424242424248</v>
+      <c r="F113" s="2">
+        <f>F112/38.5</f>
+        <v>5.4177489177489182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added structure for test on HELM coefficients
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F109" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F111" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G109" si="3">F28/60</f>
+        <f t="shared" ref="G28:G111" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -2804,7 +2804,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2014</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>3.4999999999999996</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2014</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>2.4166666666666687</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2014</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>1.1666666666666652</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2014</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>0.50000000000000089</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2014</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2014</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>2.4999999999999991</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2014</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>1.583333333333333</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2014</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>3.7500000000000013</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2014</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>1.3333333333333337</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2014</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>1.0833333333333321</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2014</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -3103,8 +3103,9 @@
         <f t="shared" si="3"/>
         <v>0.49999999999999822</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H108" s="2"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2014</v>
       </c>
@@ -3118,47 +3119,97 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="E109" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.78125</v>
       </c>
       <c r="F109" s="3">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>30.000000000000053</v>
       </c>
       <c r="G109" s="2">
         <f t="shared" si="3"/>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="3"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E111" s="4" t="s">
-        <v>6</v>
+        <v>0.50000000000000089</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>2014</v>
+      </c>
+      <c r="B110">
+        <v>4</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E110" s="1">
+        <v>0.84375</v>
+      </c>
+      <c r="F110" s="3">
+        <f t="shared" si="2"/>
+        <v>14.999999999999947</v>
+      </c>
+      <c r="G110" s="2">
+        <f t="shared" si="3"/>
+        <v>0.24999999999999911</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>2014</v>
+      </c>
+      <c r="B111">
+        <v>4</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="E111" s="1">
+        <v>0.91666666666666663</v>
       </c>
       <c r="F111" s="3">
-        <f>SUM(F2:F110)</f>
-        <v>12515</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E112" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F112" s="2">
-        <f>F111/60</f>
-        <v>208.58333333333334</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>59.999999999999943</v>
+      </c>
+      <c r="G111" s="2">
+        <f t="shared" si="3"/>
+        <v>0.999999999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="3"/>
     </row>
     <row r="113" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E113" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F113" s="3">
+        <f>SUM(F2:F112)</f>
+        <v>12575</v>
+      </c>
+    </row>
+    <row r="114" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E114" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F114" s="2">
+        <f>F113/60</f>
+        <v>209.58333333333334</v>
+      </c>
+    </row>
+    <row r="115" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E115" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F113" s="2">
-        <f>F112/38.5</f>
-        <v>5.4177489177489182</v>
+      <c r="F115" s="2">
+        <f>F114/38.5</f>
+        <v>5.4437229437229444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added experiment with PQ- and PV-bus
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+      <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F111" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F115" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G111" si="3">F28/60</f>
+        <f t="shared" ref="G28:G115" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -3138,7 +3138,7 @@
         <v>4</v>
       </c>
       <c r="C110">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D110" s="1">
         <v>0.83333333333333337</v>
@@ -3163,53 +3163,153 @@
         <v>4</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D111" s="1">
         <v>0.875</v>
       </c>
       <c r="E111" s="1">
+        <v>0.9375</v>
+      </c>
+      <c r="F111" s="3">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="G111" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>2014</v>
+      </c>
+      <c r="B112">
+        <v>4</v>
+      </c>
+      <c r="C112">
+        <v>3</v>
+      </c>
+      <c r="D112" s="1">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="E112" s="1">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="F112" s="3">
+        <f t="shared" si="2"/>
+        <v>25.000000000000071</v>
+      </c>
+      <c r="G112" s="2">
+        <f t="shared" si="3"/>
+        <v>0.41666666666666785</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>2014</v>
+      </c>
+      <c r="B113">
+        <v>4</v>
+      </c>
+      <c r="C113">
+        <v>3</v>
+      </c>
+      <c r="D113" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E113" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F113" s="3">
+        <f t="shared" si="2"/>
+        <v>60.000000000000107</v>
+      </c>
+      <c r="G113" s="2">
+        <f t="shared" si="3"/>
+        <v>1.0000000000000018</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>2014</v>
+      </c>
+      <c r="B114">
+        <v>4</v>
+      </c>
+      <c r="C114">
+        <v>4</v>
+      </c>
+      <c r="D114" s="1">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="E114" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F114" s="3">
+        <f t="shared" si="2"/>
+        <v>159.99999999999991</v>
+      </c>
+      <c r="G114" s="2">
+        <f t="shared" si="3"/>
+        <v>2.6666666666666652</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>2014</v>
+      </c>
+      <c r="B115">
+        <v>4</v>
+      </c>
+      <c r="C115">
+        <v>4</v>
+      </c>
+      <c r="D115" s="1">
+        <v>0.84375</v>
+      </c>
+      <c r="E115" s="1">
         <v>0.91666666666666663</v>
       </c>
-      <c r="F111" s="3">
-        <f t="shared" si="2"/>
-        <v>59.999999999999943</v>
-      </c>
-      <c r="G111" s="2">
-        <f t="shared" si="3"/>
-        <v>0.999999999999999</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="3"/>
-    </row>
-    <row r="113" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E113" s="4" t="s">
+      <c r="F115" s="3">
+        <f t="shared" si="2"/>
+        <v>104.99999999999994</v>
+      </c>
+      <c r="G115" s="2">
+        <f t="shared" si="3"/>
+        <v>1.7499999999999991</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="3"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E117" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F113" s="3">
-        <f>SUM(F2:F112)</f>
-        <v>12575</v>
-      </c>
-    </row>
-    <row r="114" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E114" s="4" t="s">
+      <c r="F117" s="3">
+        <f>SUM(F2:F116)</f>
+        <v>12955</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E118" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F114" s="2">
-        <f>F113/60</f>
-        <v>209.58333333333334</v>
-      </c>
-    </row>
-    <row r="115" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E115" s="4" t="s">
+      <c r="F118" s="2">
+        <f>F117/60</f>
+        <v>215.91666666666666</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E119" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F115" s="2">
-        <f>F114/38.5</f>
-        <v>5.4437229437229444</v>
+      <c r="F119" s="2">
+        <f>F118/38.5</f>
+        <v>5.608225108225108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
defined interface for power net on multiple voltage levels
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H119"/>
+  <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E115" sqref="E115"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="J113" sqref="J113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F115" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F118" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G115" si="3">F28/60</f>
+        <f t="shared" ref="G28:G118" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -3281,35 +3281,110 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
-      <c r="F116" s="3"/>
+      <c r="A116">
+        <v>2014</v>
+      </c>
+      <c r="B116">
+        <v>4</v>
+      </c>
+      <c r="C116">
+        <v>5</v>
+      </c>
+      <c r="D116" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E116" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="F116" s="3">
+        <f t="shared" si="2"/>
+        <v>195.00000000000003</v>
+      </c>
+      <c r="G116" s="2">
+        <f t="shared" si="3"/>
+        <v>3.2500000000000004</v>
+      </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E117" s="4" t="s">
+      <c r="A117">
+        <v>2014</v>
+      </c>
+      <c r="B117">
+        <v>4</v>
+      </c>
+      <c r="C117">
+        <v>5</v>
+      </c>
+      <c r="D117" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E117" s="1">
+        <v>0.65625</v>
+      </c>
+      <c r="F117" s="3">
+        <f t="shared" si="2"/>
+        <v>165.00000000000006</v>
+      </c>
+      <c r="G117" s="2">
+        <f t="shared" si="3"/>
+        <v>2.7500000000000009</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>2014</v>
+      </c>
+      <c r="B118">
+        <v>4</v>
+      </c>
+      <c r="C118">
+        <v>7</v>
+      </c>
+      <c r="D118" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="E118" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F118" s="3">
+        <f t="shared" si="2"/>
+        <v>30.000000000000053</v>
+      </c>
+      <c r="G118" s="2">
+        <f t="shared" si="3"/>
+        <v>0.50000000000000089</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="3"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E120" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F117" s="3">
-        <f>SUM(F2:F116)</f>
-        <v>12955</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E118" s="4" t="s">
+      <c r="F120" s="3">
+        <f>SUM(F2:F119)</f>
+        <v>13345</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E121" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F118" s="2">
-        <f>F117/60</f>
-        <v>215.91666666666666</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E119" s="4" t="s">
+      <c r="F121" s="2">
+        <f>F120/60</f>
+        <v>222.41666666666666</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E122" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F119" s="2">
-        <f>F118/38.5</f>
-        <v>5.608225108225108</v>
+      <c r="F122" s="2">
+        <f>F121/38.5</f>
+        <v>5.7770562770562766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests for Node
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,9 +394,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H123"/>
+  <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
       <selection activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F119" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F120" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G119" si="3">F28/60</f>
+        <f t="shared" ref="G28:G120" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -3381,35 +3381,60 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
-      <c r="F120" s="3"/>
+      <c r="A120">
+        <v>2014</v>
+      </c>
+      <c r="B120">
+        <v>4</v>
+      </c>
+      <c r="C120">
+        <v>9</v>
+      </c>
+      <c r="D120" s="1">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="E120" s="1">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="F120" s="3">
+        <f t="shared" si="2"/>
+        <v>50.000000000000142</v>
+      </c>
+      <c r="G120" s="2">
+        <f t="shared" si="3"/>
+        <v>0.8333333333333357</v>
+      </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E121" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F121" s="3">
-        <f>SUM(F2:F120)</f>
-        <v>13405</v>
-      </c>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="3"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E122" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F122" s="2">
-        <f>F121/60</f>
-        <v>223.41666666666666</v>
+        <v>6</v>
+      </c>
+      <c r="F122" s="3">
+        <f>SUM(F2:F121)</f>
+        <v>13455</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E123" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F123" s="2">
+        <f>F122/60</f>
+        <v>224.25</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E124" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F123" s="2">
-        <f>F122/38.5</f>
-        <v>5.8030303030303028</v>
+      <c r="F124" s="2">
+        <f>F123/38.5</f>
+        <v>5.8246753246753249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented check for floating nodes
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:H125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="H121" sqref="H121"/>
+      <selection activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3419,15 +3419,15 @@
         <v>0.63541666666666663</v>
       </c>
       <c r="E121" s="1">
-        <v>0.75</v>
+        <v>0.74305555555555547</v>
       </c>
       <c r="F121" s="3">
         <f t="shared" si="2"/>
-        <v>165.00000000000006</v>
+        <v>154.99999999999994</v>
       </c>
       <c r="G121" s="2">
         <f t="shared" si="3"/>
-        <v>2.7500000000000009</v>
+        <v>2.5833333333333326</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -3441,7 +3441,7 @@
       </c>
       <c r="F123" s="3">
         <f>SUM(F2:F122)</f>
-        <v>13620</v>
+        <v>13610</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -3450,7 +3450,7 @@
       </c>
       <c r="F124" s="2">
         <f>F123/60</f>
-        <v>227</v>
+        <v>226.83333333333334</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -3459,7 +3459,7 @@
       </c>
       <c r="F125" s="2">
         <f>F124/38.5</f>
-        <v>5.8961038961038961</v>
+        <v>5.891774891774892</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented basics for calculator for multiple voltage levels
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H126"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="H117" sqref="H117"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="O114" sqref="O114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F122" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F123" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G122" si="3">F28/60</f>
+        <f t="shared" ref="G28:G123" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -3444,47 +3444,72 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="E122" s="1">
-        <v>0.91666666666666663</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="F122" s="3">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>240.00000000000011</v>
       </c>
       <c r="G122" s="2">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4.0000000000000018</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D123" s="1"/>
-      <c r="E123" s="1"/>
-      <c r="F123" s="3"/>
+      <c r="A123">
+        <v>2014</v>
+      </c>
+      <c r="B123">
+        <v>4</v>
+      </c>
+      <c r="C123">
+        <v>11</v>
+      </c>
+      <c r="D123" s="1">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="E123" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F123" s="3">
+        <f t="shared" si="2"/>
+        <v>40.000000000000014</v>
+      </c>
+      <c r="G123" s="2">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666685</v>
+      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E124" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F124" s="3">
-        <f>SUM(F2:F123)</f>
-        <v>13790</v>
-      </c>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+      <c r="F124" s="3"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E125" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F125" s="2">
-        <f>F124/60</f>
-        <v>229.83333333333334</v>
+        <v>6</v>
+      </c>
+      <c r="F125" s="3">
+        <f>SUM(F2:F124)</f>
+        <v>13890</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E126" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F126" s="2">
+        <f>F125/60</f>
+        <v>231.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E127" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F126" s="2">
-        <f>F125/38.5</f>
-        <v>5.9696969696969697</v>
+      <c r="F127" s="2">
+        <f>F126/38.5</f>
+        <v>6.0129870129870131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed scaling of power in load
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H128"/>
+  <dimension ref="A1:H129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="K123" sqref="K123"/>
+      <selection activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F124" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F125" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G124" si="3">F28/60</f>
+        <f t="shared" ref="G28:G125" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -3506,35 +3506,60 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D125" s="1"/>
-      <c r="E125" s="1"/>
-      <c r="F125" s="3"/>
+      <c r="A125">
+        <v>2014</v>
+      </c>
+      <c r="B125">
+        <v>4</v>
+      </c>
+      <c r="C125">
+        <v>14</v>
+      </c>
+      <c r="D125" s="1">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E125" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F125" s="3">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="G125" s="2">
+        <f t="shared" si="3"/>
+        <v>2.6666666666666665</v>
+      </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E126" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F126" s="3">
-        <f>SUM(F2:F125)</f>
-        <v>13965</v>
-      </c>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="3"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E127" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F127" s="2">
-        <f>F126/60</f>
-        <v>232.75</v>
+        <v>6</v>
+      </c>
+      <c r="F127" s="3">
+        <f>SUM(F2:F126)</f>
+        <v>14125</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E128" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F128" s="2">
+        <f>F127/60</f>
+        <v>235.41666666666666</v>
+      </c>
+    </row>
+    <row r="129" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E129" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F128" s="2">
-        <f>F127/38.5</f>
-        <v>6.0454545454545459</v>
+      <c r="F129" s="2">
+        <f>F128/38.5</f>
+        <v>6.1147186147186146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented input impedance calculation for feed in
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -396,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F125" sqref="F125"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3519,15 +3519,15 @@
         <v>0.3888888888888889</v>
       </c>
       <c r="E125" s="1">
-        <v>0.5</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="F125" s="3">
         <f t="shared" si="2"/>
-        <v>160</v>
+        <v>130.00000000000003</v>
       </c>
       <c r="G125" s="2">
         <f t="shared" si="3"/>
-        <v>2.6666666666666665</v>
+        <v>2.166666666666667</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -3541,7 +3541,7 @@
       </c>
       <c r="F127" s="3">
         <f>SUM(F2:F126)</f>
-        <v>14125</v>
+        <v>14095</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -3550,7 +3550,7 @@
       </c>
       <c r="F128" s="2">
         <f>F127/60</f>
-        <v>235.41666666666666</v>
+        <v>234.91666666666666</v>
       </c>
     </row>
     <row r="129" spans="5:6" x14ac:dyDescent="0.25">
@@ -3559,7 +3559,7 @@
       </c>
       <c r="F129" s="2">
         <f>F128/38.5</f>
-        <v>6.1147186147186146</v>
+        <v>6.1017316017316015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added interface for objects with internal nodes
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H129"/>
+  <dimension ref="A1:H130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E126" sqref="E126"/>
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F125" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F126" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G125" si="3">F28/60</f>
+        <f t="shared" ref="G28:G126" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -3531,35 +3531,60 @@
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D126" s="1"/>
-      <c r="E126" s="1"/>
-      <c r="F126" s="3"/>
+      <c r="A126">
+        <v>2014</v>
+      </c>
+      <c r="B126">
+        <v>4</v>
+      </c>
+      <c r="C126">
+        <v>15</v>
+      </c>
+      <c r="D126" s="1">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E126" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F126" s="3">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="G126" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E127" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F127" s="3">
-        <f>SUM(F2:F126)</f>
-        <v>14095</v>
-      </c>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="3"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E128" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F128" s="2">
-        <f>F127/60</f>
-        <v>234.91666666666666</v>
+        <v>6</v>
+      </c>
+      <c r="F128" s="3">
+        <f>SUM(F2:F127)</f>
+        <v>14185</v>
       </c>
     </row>
     <row r="129" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E129" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F129" s="2">
+        <f>F128/60</f>
+        <v>236.41666666666666</v>
+      </c>
+    </row>
+    <row r="130" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E130" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F129" s="2">
-        <f>F128/38.5</f>
-        <v>6.1017316017316015</v>
+      <c r="F130" s="2">
+        <f>F129/38.5</f>
+        <v>6.1406926406926408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented derived internal pq node
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:H131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="K127" sqref="K127"/>
+      <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3569,15 +3569,15 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="E127" s="1">
-        <v>0.69444444444444453</v>
+        <v>0.6875</v>
       </c>
       <c r="F127" s="3">
         <f t="shared" si="2"/>
-        <v>70.000000000000071</v>
+        <v>59.999999999999943</v>
       </c>
       <c r="G127" s="2">
         <f t="shared" si="3"/>
-        <v>1.1666666666666679</v>
+        <v>0.999999999999999</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -3591,7 +3591,7 @@
       </c>
       <c r="F129" s="3">
         <f>SUM(F2:F128)</f>
-        <v>14255</v>
+        <v>14245</v>
       </c>
     </row>
     <row r="130" spans="5:6" x14ac:dyDescent="0.25">
@@ -3600,7 +3600,7 @@
       </c>
       <c r="F130" s="2">
         <f>F129/60</f>
-        <v>237.58333333333334</v>
+        <v>237.41666666666666</v>
       </c>
     </row>
     <row r="131" spans="5:6" x14ac:dyDescent="0.25">
@@ -3609,7 +3609,7 @@
       </c>
       <c r="F131" s="2">
         <f>F130/38.5</f>
-        <v>6.170995670995671</v>
+        <v>6.1666666666666661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented derived internal slack node
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H131"/>
+  <dimension ref="A1:H132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+      <selection activeCell="H128" sqref="H128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F127" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F128" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G127" si="3">F28/60</f>
+        <f t="shared" ref="G28:G128" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -3581,35 +3581,60 @@
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D128" s="1"/>
-      <c r="E128" s="1"/>
-      <c r="F128" s="3"/>
-    </row>
-    <row r="129" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E129" s="4" t="s">
+      <c r="A128">
+        <v>2014</v>
+      </c>
+      <c r="B128">
+        <v>4</v>
+      </c>
+      <c r="C128">
+        <v>15</v>
+      </c>
+      <c r="D128" s="1">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="E128" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F128" s="3">
+        <f t="shared" si="2"/>
+        <v>105.00000000000011</v>
+      </c>
+      <c r="G128" s="2">
+        <f t="shared" si="3"/>
+        <v>1.750000000000002</v>
+      </c>
+    </row>
+    <row r="129" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="3"/>
+    </row>
+    <row r="130" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E130" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F129" s="3">
-        <f>SUM(F2:F128)</f>
-        <v>14245</v>
-      </c>
-    </row>
-    <row r="130" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E130" s="4" t="s">
+      <c r="F130" s="3">
+        <f>SUM(F2:F129)</f>
+        <v>14350</v>
+      </c>
+    </row>
+    <row r="131" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E131" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F130" s="2">
-        <f>F129/60</f>
-        <v>237.41666666666666</v>
-      </c>
-    </row>
-    <row r="131" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E131" s="4" t="s">
+      <c r="F131" s="2">
+        <f>F130/60</f>
+        <v>239.16666666666666</v>
+      </c>
+    </row>
+    <row r="132" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E132" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F131" s="2">
-        <f>F130/38.5</f>
-        <v>6.1666666666666661</v>
+      <c r="F132" s="2">
+        <f>F131/38.5</f>
+        <v>6.2121212121212119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented calculation of length impedance and shunt admittance of a line in the most general form
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:H132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="H128" sqref="H128"/>
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3594,15 +3594,15 @@
         <v>0.88541666666666663</v>
       </c>
       <c r="E128" s="1">
-        <v>0.95833333333333337</v>
+        <v>0.95138888888888884</v>
       </c>
       <c r="F128" s="3">
         <f t="shared" si="2"/>
-        <v>105.00000000000011</v>
+        <v>94.999999999999986</v>
       </c>
       <c r="G128" s="2">
         <f t="shared" si="3"/>
-        <v>1.750000000000002</v>
+        <v>1.583333333333333</v>
       </c>
     </row>
     <row r="129" spans="4:6" x14ac:dyDescent="0.25">
@@ -3616,7 +3616,7 @@
       </c>
       <c r="F130" s="3">
         <f>SUM(F2:F129)</f>
-        <v>14350</v>
+        <v>14340</v>
       </c>
     </row>
     <row r="131" spans="4:6" x14ac:dyDescent="0.25">
@@ -3625,7 +3625,7 @@
       </c>
       <c r="F131" s="2">
         <f>F130/60</f>
-        <v>239.16666666666666</v>
+        <v>239</v>
       </c>
     </row>
     <row r="132" spans="4:6" x14ac:dyDescent="0.25">
@@ -3634,7 +3634,7 @@
       </c>
       <c r="F132" s="2">
         <f>F131/38.5</f>
-        <v>6.2121212121212119</v>
+        <v>6.2077922077922079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for Line
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H132"/>
+  <dimension ref="A1:H133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E129" sqref="E129"/>
+      <selection activeCell="H131" sqref="H131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F128" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F129" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G128" si="3">F28/60</f>
+        <f t="shared" ref="G28:G129" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -3605,36 +3605,61 @@
         <v>1.583333333333333</v>
       </c>
     </row>
-    <row r="129" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D129" s="1"/>
-      <c r="E129" s="1"/>
-      <c r="F129" s="3"/>
-    </row>
-    <row r="130" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E130" s="4" t="s">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>2014</v>
+      </c>
+      <c r="B129">
+        <v>4</v>
+      </c>
+      <c r="C129">
+        <v>16</v>
+      </c>
+      <c r="D129" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E129" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="F129" s="3">
+        <f t="shared" si="2"/>
+        <v>15.000000000000027</v>
+      </c>
+      <c r="G129" s="2">
+        <f t="shared" si="3"/>
+        <v>0.25000000000000044</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D130" s="1"/>
+      <c r="E130" s="1"/>
+      <c r="F130" s="3"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E131" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F130" s="3">
-        <f>SUM(F2:F129)</f>
-        <v>14340</v>
-      </c>
-    </row>
-    <row r="131" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E131" s="4" t="s">
+      <c r="F131" s="3">
+        <f>SUM(F2:F130)</f>
+        <v>14355</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E132" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F131" s="2">
-        <f>F130/60</f>
-        <v>239</v>
-      </c>
-    </row>
-    <row r="132" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E132" s="4" t="s">
+      <c r="F132" s="2">
+        <f>F131/60</f>
+        <v>239.25</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E133" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F132" s="2">
-        <f>F131/38.5</f>
-        <v>6.2077922077922079</v>
+      <c r="F133" s="2">
+        <f>F132/38.5</f>
+        <v>6.2142857142857144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved filling of admittance matrix into the power net
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H133"/>
+  <dimension ref="A1:H134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="H131" sqref="H131"/>
+      <selection activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,11 +1096,11 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28:F129" si="2">(E28-D28)*24*60</f>
+        <f t="shared" ref="F28:F130" si="2">(E28-D28)*24*60</f>
         <v>230.00000000000014</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" ref="G28:G129" si="3">F28/60</f>
+        <f t="shared" ref="G28:G130" si="3">F28/60</f>
         <v>3.8333333333333357</v>
       </c>
     </row>
@@ -3631,35 +3631,60 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D130" s="1"/>
-      <c r="E130" s="1"/>
-      <c r="F130" s="3"/>
+      <c r="A130">
+        <v>2014</v>
+      </c>
+      <c r="B130">
+        <v>4</v>
+      </c>
+      <c r="C130">
+        <v>16</v>
+      </c>
+      <c r="D130" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="E130" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F130" s="3">
+        <f t="shared" si="2"/>
+        <v>75.000000000000057</v>
+      </c>
+      <c r="G130" s="2">
+        <f t="shared" si="3"/>
+        <v>1.2500000000000009</v>
+      </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E131" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F131" s="3">
-        <f>SUM(F2:F130)</f>
-        <v>14355</v>
-      </c>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="3"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E132" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F132" s="2">
-        <f>F131/60</f>
-        <v>239.25</v>
+        <v>6</v>
+      </c>
+      <c r="F132" s="3">
+        <f>SUM(F2:F131)</f>
+        <v>14430</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E133" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F133" s="2">
+        <f>F132/60</f>
+        <v>240.5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E134" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F133" s="2">
-        <f>F132/38.5</f>
-        <v>6.2142857142857144</v>
+      <c r="F134" s="2">
+        <f>F133/38.5</f>
+        <v>6.2467532467532472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added voltage to node
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>time spent [h]</t>
-  </si>
-  <si>
-    <t>2ß14</t>
   </si>
 </sst>
 </file>
@@ -397,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H135"/>
+  <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3684,8 +3681,8 @@
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>10</v>
+      <c r="A132">
+        <v>2014</v>
       </c>
       <c r="B132">
         <v>7</v>
@@ -3696,41 +3693,73 @@
       <c r="D132" s="1">
         <v>0.84375</v>
       </c>
-      <c r="E132" s="1"/>
+      <c r="E132" s="1">
+        <v>0.92708333333333337</v>
+      </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132" si="4">(E132-D132)*24*60</f>
-        <v>-1215</v>
+        <f t="shared" ref="F132:F133" si="4">(E132-D132)*24*60</f>
+        <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132" si="5">F132/60</f>
-        <v>-20.25</v>
+        <f t="shared" ref="G132:G133" si="5">F132/60</f>
+        <v>2.0000000000000009</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E133" s="4" t="s">
-        <v>6</v>
+      <c r="A133">
+        <v>2014</v>
+      </c>
+      <c r="B133">
+        <v>7</v>
+      </c>
+      <c r="C133">
+        <v>12</v>
+      </c>
+      <c r="D133" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="E133" s="1">
+        <v>0.5</v>
       </c>
       <c r="F133" s="3">
-        <f>SUM(F2:F132)</f>
-        <v>13255</v>
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="G133" s="2">
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E134" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F134" s="2">
-        <f>F133/60</f>
-        <v>220.91666666666666</v>
-      </c>
+      <c r="D134" s="1"/>
+      <c r="E134" s="1"/>
+      <c r="F134" s="3"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E135" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F135" s="3">
+        <f>SUM(F2:F133)</f>
+        <v>14770</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E136" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F136" s="2">
+        <f>F135/60</f>
+        <v>246.16666666666666</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E137" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F135" s="2">
-        <f>F134/38.5</f>
-        <v>5.7380952380952381</v>
+      <c r="F137" s="2">
+        <f>F136/38.5</f>
+        <v>6.3939393939393936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added necessary parameter for transformer
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7650"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="11250" windowHeight="7575"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H137"/>
+  <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="F133" sqref="F133"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F133" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F134" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G133" si="5">F132/60</f>
+        <f t="shared" ref="G132:G134" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -3719,47 +3719,72 @@
         <v>0.375</v>
       </c>
       <c r="E133" s="1">
-        <v>0.5</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="F133" s="3">
         <f t="shared" si="4"/>
-        <v>180</v>
+        <v>239.99999999999994</v>
       </c>
       <c r="G133" s="2">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>3.9999999999999991</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D134" s="1"/>
-      <c r="E134" s="1"/>
-      <c r="F134" s="3"/>
+      <c r="A134">
+        <v>2014</v>
+      </c>
+      <c r="B134">
+        <v>7</v>
+      </c>
+      <c r="C134">
+        <v>12</v>
+      </c>
+      <c r="D134" s="1">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="E134" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F134" s="3">
+        <f t="shared" si="4"/>
+        <v>194.99999999999994</v>
+      </c>
+      <c r="G134" s="2">
+        <f t="shared" si="5"/>
+        <v>3.2499999999999991</v>
+      </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E135" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F135" s="3">
-        <f>SUM(F2:F133)</f>
-        <v>14770</v>
-      </c>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+      <c r="F135" s="3"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E136" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F136" s="2">
-        <f>F135/60</f>
-        <v>246.16666666666666</v>
+        <v>6</v>
+      </c>
+      <c r="F136" s="3">
+        <f>SUM(F2:F134)</f>
+        <v>15025</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E137" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F137" s="2">
+        <f>F136/60</f>
+        <v>250.41666666666666</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E138" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F137" s="2">
-        <f>F136/38.5</f>
-        <v>6.3939393939393936</v>
+      <c r="F138" s="2">
+        <f>F137/38.5</f>
+        <v>6.5043290043290041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test with transformer
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H138"/>
+  <dimension ref="A1:H139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="E135" sqref="E135"/>
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F134" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F135" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G134" si="5">F132/60</f>
+        <f t="shared" ref="G132:G135" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -3756,34 +3756,59 @@
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D135" s="1"/>
-      <c r="E135" s="1"/>
-      <c r="F135" s="3"/>
+      <c r="A135">
+        <v>2014</v>
+      </c>
+      <c r="B135">
+        <v>7</v>
+      </c>
+      <c r="C135">
+        <v>12</v>
+      </c>
+      <c r="D135" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="E135" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="F135" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G135" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E136" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F136" s="3">
-        <f>SUM(F2:F134)</f>
-        <v>15025</v>
-      </c>
+      <c r="D136" s="1"/>
+      <c r="E136" s="1"/>
+      <c r="F136" s="3"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E137" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F137" s="2">
-        <f>F136/60</f>
-        <v>250.41666666666666</v>
+        <v>6</v>
+      </c>
+      <c r="F137" s="3">
+        <f>SUM(F2:F135)</f>
+        <v>15025</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E138" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F138" s="2">
+        <f>F137/60</f>
+        <v>250.41666666666666</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E139" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F138" s="2">
-        <f>F137/38.5</f>
+      <c r="F139" s="2">
+        <f>F138/38.5</f>
         <v>6.5043290043290041</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed tests for ideal transformers
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -3769,15 +3769,15 @@
         <v>0.875</v>
       </c>
       <c r="E135" s="1">
-        <v>0.875</v>
+        <v>0.94791666666666663</v>
       </c>
       <c r="F135" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>104.99999999999994</v>
       </c>
       <c r="G135" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.7499999999999991</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -3791,7 +3791,7 @@
       </c>
       <c r="F137" s="3">
         <f>SUM(F2:F135)</f>
-        <v>15025</v>
+        <v>15130</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -3800,7 +3800,7 @@
       </c>
       <c r="F138" s="2">
         <f>F137/60</f>
-        <v>250.41666666666666</v>
+        <v>252.16666666666666</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -3809,7 +3809,7 @@
       </c>
       <c r="F139" s="2">
         <f>F138/38.5</f>
-        <v>6.5043290043290041</v>
+        <v>6.5497835497835499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed check on condition of admittance matrix
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H139"/>
+  <dimension ref="A1:H141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136"/>
+      <selection activeCell="E138" sqref="E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F135" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F137" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G135" si="5">F132/60</f>
+        <f t="shared" ref="G132:G137" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -3781,35 +3781,85 @@
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D136" s="1"/>
-      <c r="E136" s="1"/>
-      <c r="F136" s="3"/>
+      <c r="A136">
+        <v>2014</v>
+      </c>
+      <c r="B136">
+        <v>7</v>
+      </c>
+      <c r="C136">
+        <v>12</v>
+      </c>
+      <c r="D136" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E136" s="1">
+        <v>1</v>
+      </c>
+      <c r="F136" s="3">
+        <f t="shared" si="4"/>
+        <v>59.999999999999943</v>
+      </c>
+      <c r="G136" s="2">
+        <f t="shared" si="5"/>
+        <v>0.999999999999999</v>
+      </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E137" s="4" t="s">
-        <v>6</v>
+      <c r="A137">
+        <v>2014</v>
+      </c>
+      <c r="B137">
+        <v>7</v>
+      </c>
+      <c r="C137">
+        <v>13</v>
+      </c>
+      <c r="D137" s="1">
+        <v>0</v>
+      </c>
+      <c r="E137" s="1">
+        <v>0</v>
       </c>
       <c r="F137" s="3">
-        <f>SUM(F2:F135)</f>
-        <v>15130</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G137" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E138" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F138" s="2">
-        <f>F137/60</f>
-        <v>252.16666666666666</v>
-      </c>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
+      <c r="F138" s="3"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E139" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F139" s="3">
+        <f>SUM(F2:F137)</f>
+        <v>15190</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E140" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F140" s="2">
+        <f>F139/60</f>
+        <v>253.16666666666666</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E141" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F139" s="2">
-        <f>F138/38.5</f>
-        <v>6.5497835497835499</v>
+      <c r="F141" s="2">
+        <f>F140/38.5</f>
+        <v>6.5757575757575752</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added factor in transformer for ideal transformer
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H141"/>
+  <dimension ref="A1:H142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
       <selection activeCell="E138" sqref="E138"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F137" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F138" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G137" si="5">F132/60</f>
+        <f t="shared" ref="G132:G138" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -3819,47 +3819,72 @@
         <v>0</v>
       </c>
       <c r="E137" s="1">
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="F137" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G137" s="2">
         <f t="shared" si="5"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>2014</v>
+      </c>
+      <c r="B138">
+        <v>7</v>
+      </c>
+      <c r="C138">
+        <v>13</v>
+      </c>
+      <c r="D138" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E138" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F138" s="3">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D138" s="1"/>
-      <c r="E138" s="1"/>
-      <c r="F138" s="3"/>
+      <c r="G138" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E139" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F139" s="3">
-        <f>SUM(F2:F137)</f>
-        <v>15190</v>
-      </c>
+      <c r="D139" s="1"/>
+      <c r="E139" s="1"/>
+      <c r="F139" s="3"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E140" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F140" s="2">
-        <f>F139/60</f>
-        <v>253.16666666666666</v>
+        <v>6</v>
+      </c>
+      <c r="F140" s="3">
+        <f>SUM(F2:F138)</f>
+        <v>15205</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E141" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F141" s="2">
+        <f>F140/60</f>
+        <v>253.41666666666666</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E142" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F141" s="2">
-        <f>F140/38.5</f>
-        <v>6.5757575757575752</v>
+      <c r="F142" s="2">
+        <f>F141/38.5</f>
+        <v>6.5822510822510818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed slack voltage of ground node
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -396,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="E138" sqref="E138"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="E139" sqref="E139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3844,15 +3844,15 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E138" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="F138" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="G138" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="F140" s="3">
         <f>SUM(F2:F138)</f>
-        <v>15205</v>
+        <v>15445</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -3875,7 +3875,7 @@
       </c>
       <c r="F141" s="2">
         <f>F140/60</f>
-        <v>253.41666666666666</v>
+        <v>257.41666666666669</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -3884,7 +3884,7 @@
       </c>
       <c r="F142" s="2">
         <f>F141/38.5</f>
-        <v>6.5822510822510818</v>
+        <v>6.6861471861471866</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for admittance matrix
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H142"/>
+  <dimension ref="A1:H144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="E139" sqref="E139"/>
+      <selection activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F138" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F140" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G138" si="5">F132/60</f>
+        <f t="shared" ref="G132:G140" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -3856,35 +3856,85 @@
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D139" s="1"/>
-      <c r="E139" s="1"/>
-      <c r="F139" s="3"/>
+      <c r="A139">
+        <v>2014</v>
+      </c>
+      <c r="B139">
+        <v>7</v>
+      </c>
+      <c r="C139">
+        <v>13</v>
+      </c>
+      <c r="D139" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="E139" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F139" s="3">
+        <f t="shared" si="4"/>
+        <v>270</v>
+      </c>
+      <c r="G139" s="2">
+        <f t="shared" si="5"/>
+        <v>4.5</v>
+      </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E140" s="4" t="s">
-        <v>6</v>
+      <c r="A140">
+        <v>2014</v>
+      </c>
+      <c r="B140">
+        <v>7</v>
+      </c>
+      <c r="C140">
+        <v>13</v>
+      </c>
+      <c r="D140" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E140" s="1">
+        <v>0.83333333333333337</v>
       </c>
       <c r="F140" s="3">
-        <f>SUM(F2:F138)</f>
-        <v>15445</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G140" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E141" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F141" s="2">
-        <f>F140/60</f>
-        <v>257.41666666666669</v>
-      </c>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1"/>
+      <c r="F141" s="3"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E142" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F142" s="3">
+        <f>SUM(F2:F140)</f>
+        <v>15715</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E143" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F143" s="2">
+        <f>F142/60</f>
+        <v>261.91666666666669</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E144" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F142" s="2">
-        <f>F141/38.5</f>
-        <v>6.6861471861471866</v>
+      <c r="F144" s="2">
+        <f>F143/38.5</f>
+        <v>6.8030303030303036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed test for ideal transformer
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H144"/>
+  <dimension ref="A1:H145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141"/>
+      <selection activeCell="H143" sqref="H143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F140" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F141" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G140" si="5">F132/60</f>
+        <f t="shared" ref="G132:G141" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -3906,34 +3906,59 @@
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D141" s="1"/>
-      <c r="E141" s="1"/>
-      <c r="F141" s="3"/>
+      <c r="A141">
+        <v>2014</v>
+      </c>
+      <c r="B141">
+        <v>7</v>
+      </c>
+      <c r="C141">
+        <v>14</v>
+      </c>
+      <c r="D141" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E141" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F141" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G141" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E142" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F142" s="3">
-        <f>SUM(F2:F140)</f>
-        <v>15820</v>
-      </c>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1"/>
+      <c r="F142" s="3"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E143" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F143" s="2">
-        <f>F142/60</f>
-        <v>263.66666666666669</v>
+        <v>6</v>
+      </c>
+      <c r="F143" s="3">
+        <f>SUM(F2:F141)</f>
+        <v>15820</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E144" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F144" s="2">
+        <f>F143/60</f>
+        <v>263.66666666666669</v>
+      </c>
+    </row>
+    <row r="145" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E145" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F144" s="2">
-        <f>F143/38.5</f>
+      <c r="F145" s="2">
+        <f>F144/38.5</f>
         <v>6.8484848484848486</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replaced plane matrix with admittance matrix in the power net
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H146"/>
+  <dimension ref="A1:H147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="F142" sqref="F142"/>
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F142" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F143" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G142" si="5">F132/60</f>
+        <f t="shared" ref="G132:G143" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -3944,47 +3944,72 @@
         <v>0.5</v>
       </c>
       <c r="E142" s="1">
-        <v>0.54166666666666663</v>
+        <v>0.5625</v>
       </c>
       <c r="F142" s="3">
         <f t="shared" si="4"/>
-        <v>59.999999999999943</v>
+        <v>90</v>
       </c>
       <c r="G142" s="2">
         <f t="shared" si="5"/>
-        <v>0.999999999999999</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D143" s="1"/>
-      <c r="E143" s="1"/>
-      <c r="F143" s="3"/>
+      <c r="A143">
+        <v>2014</v>
+      </c>
+      <c r="B143">
+        <v>7</v>
+      </c>
+      <c r="C143">
+        <v>21</v>
+      </c>
+      <c r="D143" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E143" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F143" s="3">
+        <f t="shared" si="4"/>
+        <v>210.00000000000006</v>
+      </c>
+      <c r="G143" s="2">
+        <f t="shared" si="5"/>
+        <v>3.5000000000000009</v>
+      </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E144" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F144" s="3">
-        <f>SUM(F2:F142)</f>
-        <v>15985</v>
-      </c>
+      <c r="D144" s="1"/>
+      <c r="E144" s="1"/>
+      <c r="F144" s="3"/>
     </row>
     <row r="145" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E145" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F145" s="2">
-        <f>F144/60</f>
-        <v>266.41666666666669</v>
+        <v>6</v>
+      </c>
+      <c r="F145" s="3">
+        <f>SUM(F2:F143)</f>
+        <v>16225</v>
       </c>
     </row>
     <row r="146" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E146" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F146" s="2">
+        <f>F145/60</f>
+        <v>270.41666666666669</v>
+      </c>
+    </row>
+    <row r="147" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E147" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F146" s="2">
-        <f>F145/38.5</f>
-        <v>6.9199134199134207</v>
+      <c r="F147" s="2">
+        <f>F146/38.5</f>
+        <v>7.0238095238095246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug in detection of convergence
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H148"/>
+  <dimension ref="A1:H149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="F144" sqref="F144"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="F145" sqref="F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F143" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F145" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G143" si="5">F132/60</f>
+        <f t="shared" ref="G132:G145" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -3993,39 +3993,73 @@
       <c r="D144" s="1">
         <v>0.76388888888888884</v>
       </c>
-      <c r="E144" s="1"/>
-      <c r="F144" s="3"/>
-    </row>
-    <row r="145" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D145" s="1"/>
-      <c r="E145" s="1"/>
-      <c r="F145" s="3"/>
-    </row>
-    <row r="146" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E146" s="4" t="s">
+      <c r="E144" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F144" s="3">
+        <f t="shared" si="4"/>
+        <v>40.000000000000014</v>
+      </c>
+      <c r="G144" s="2">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666685</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>2014</v>
+      </c>
+      <c r="B145">
+        <v>7</v>
+      </c>
+      <c r="C145">
+        <v>21</v>
+      </c>
+      <c r="D145" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E145" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="F145" s="3">
+        <f t="shared" si="4"/>
+        <v>59.999999999999943</v>
+      </c>
+      <c r="G145" s="2">
+        <f t="shared" si="5"/>
+        <v>0.999999999999999</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D146" s="1"/>
+      <c r="E146" s="1"/>
+      <c r="F146" s="3"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E147" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F146" s="3">
-        <f>SUM(F2:F143)</f>
-        <v>16165</v>
-      </c>
-    </row>
-    <row r="147" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E147" s="4" t="s">
+      <c r="F147" s="3">
+        <f>SUM(F2:F145)</f>
+        <v>16265</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E148" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F147" s="2">
-        <f>F146/60</f>
-        <v>269.41666666666669</v>
-      </c>
-    </row>
-    <row r="148" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E148" s="4" t="s">
+      <c r="F148" s="2">
+        <f>F147/60</f>
+        <v>271.08333333333331</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E149" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F148" s="2">
-        <f>F147/38.5</f>
-        <v>6.9978354978354984</v>
+      <c r="F149" s="2">
+        <f>F148/38.5</f>
+        <v>7.0411255411255409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests for power net
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H150"/>
+  <dimension ref="A1:H151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="F146" sqref="F146"/>
+      <selection activeCell="F147" sqref="F147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F146" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F147" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G146" si="5">F132/60</f>
+        <f t="shared" ref="G132:G147" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4056,35 +4056,60 @@
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D147" s="1"/>
-      <c r="E147" s="1"/>
-      <c r="F147" s="3"/>
+      <c r="A147">
+        <v>2014</v>
+      </c>
+      <c r="B147">
+        <v>7</v>
+      </c>
+      <c r="C147">
+        <v>22</v>
+      </c>
+      <c r="D147" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="E147" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F147" s="3">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="G147" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E148" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F148" s="3">
-        <f>SUM(F2:F146)</f>
-        <v>16340</v>
-      </c>
+      <c r="D148" s="1"/>
+      <c r="E148" s="1"/>
+      <c r="F148" s="3"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E149" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F149" s="2">
-        <f>F148/60</f>
-        <v>272.33333333333331</v>
+        <v>6</v>
+      </c>
+      <c r="F149" s="3">
+        <f>SUM(F2:F147)</f>
+        <v>16430</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E150" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F150" s="2">
+        <f>F149/60</f>
+        <v>273.83333333333331</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E151" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F150" s="2">
-        <f>F149/38.5</f>
-        <v>7.0735930735930728</v>
+      <c r="F151" s="2">
+        <f>F150/38.5</f>
+        <v>7.1125541125541121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added length to the line
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H152"/>
+  <dimension ref="A1:H153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="F148" sqref="F148"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F148" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F149" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G148" si="5">F132/60</f>
+        <f t="shared" ref="G132:G149" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4106,35 +4106,60 @@
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D149" s="1"/>
-      <c r="E149" s="1"/>
-      <c r="F149" s="3"/>
+      <c r="A149">
+        <v>2014</v>
+      </c>
+      <c r="B149">
+        <v>7</v>
+      </c>
+      <c r="C149">
+        <v>23</v>
+      </c>
+      <c r="D149" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E149" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F149" s="3">
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="G149" s="2">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E150" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F150" s="3">
-        <f>SUM(F2:F148)</f>
-        <v>16505</v>
-      </c>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1"/>
+      <c r="F150" s="3"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E151" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F151" s="2">
-        <f>F150/60</f>
-        <v>275.08333333333331</v>
+        <v>6</v>
+      </c>
+      <c r="F151" s="3">
+        <f>SUM(F2:F149)</f>
+        <v>16685</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E152" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F152" s="2">
+        <f>F151/60</f>
+        <v>278.08333333333331</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E153" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F152" s="2">
-        <f>F151/38.5</f>
-        <v>7.1450216450216448</v>
+      <c r="F153" s="2">
+        <f>F152/38.5</f>
+        <v>7.2229437229437226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved script from ETH
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H154"/>
+  <dimension ref="A1:H155"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="F150" sqref="F150"/>
+      <selection activeCell="F151" sqref="F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F150" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F151" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G150" si="5">F132/60</f>
+        <f t="shared" ref="G132:G151" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4156,35 +4156,60 @@
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D151" s="1"/>
-      <c r="E151" s="1"/>
-      <c r="F151" s="3"/>
+      <c r="A151">
+        <v>2014</v>
+      </c>
+      <c r="B151">
+        <v>7</v>
+      </c>
+      <c r="C151">
+        <v>24</v>
+      </c>
+      <c r="D151" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E151" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F151" s="3">
+        <f t="shared" si="4"/>
+        <v>149.99999999999994</v>
+      </c>
+      <c r="G151" s="2">
+        <f t="shared" si="5"/>
+        <v>2.4999999999999991</v>
+      </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E152" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F152" s="3">
-        <f>SUM(F2:F150)</f>
-        <v>16865</v>
-      </c>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="3"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E153" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F153" s="2">
-        <f>F152/60</f>
-        <v>281.08333333333331</v>
+        <v>6</v>
+      </c>
+      <c r="F153" s="3">
+        <f>SUM(F2:F151)</f>
+        <v>17015</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E154" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F154" s="2">
+        <f>F153/60</f>
+        <v>283.58333333333331</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E155" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F154" s="2">
-        <f>F153/38.5</f>
-        <v>7.3008658008658003</v>
+      <c r="F155" s="2">
+        <f>F154/38.5</f>
+        <v>7.3658008658008649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented binding of transformers
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:H155"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="F151" sqref="F151"/>
+      <selection activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4169,15 +4169,15 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="E151" s="1">
-        <v>0.75</v>
+        <v>0.76041666666666663</v>
       </c>
       <c r="F151" s="3">
         <f t="shared" si="4"/>
-        <v>149.99999999999994</v>
+        <v>164.99999999999989</v>
       </c>
       <c r="G151" s="2">
         <f t="shared" si="5"/>
-        <v>2.4999999999999991</v>
+        <v>2.7499999999999982</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
       </c>
       <c r="F153" s="3">
         <f>SUM(F2:F151)</f>
-        <v>17015</v>
+        <v>17030</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -4200,7 +4200,7 @@
       </c>
       <c r="F154" s="2">
         <f>F153/60</f>
-        <v>283.58333333333331</v>
+        <v>283.83333333333331</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -4209,7 +4209,7 @@
       </c>
       <c r="F155" s="2">
         <f>F154/38.5</f>
-        <v>7.3658008658008649</v>
+        <v>7.3722943722943715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried to implement binding of selected node
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H155"/>
+  <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="E152" sqref="E152"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="F152" sqref="F152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F151" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F152" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G151" si="5">F132/60</f>
+        <f t="shared" ref="G132:G152" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4181,35 +4181,60 @@
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D152" s="1"/>
-      <c r="E152" s="1"/>
-      <c r="F152" s="3"/>
+      <c r="A152">
+        <v>2014</v>
+      </c>
+      <c r="B152">
+        <v>7</v>
+      </c>
+      <c r="C152">
+        <v>24</v>
+      </c>
+      <c r="D152" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="E152" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F152" s="3">
+        <f t="shared" si="4"/>
+        <v>60.000000000000107</v>
+      </c>
+      <c r="G152" s="2">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000018</v>
+      </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E153" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F153" s="3">
-        <f>SUM(F2:F151)</f>
-        <v>17030</v>
-      </c>
+      <c r="D153" s="1"/>
+      <c r="E153" s="1"/>
+      <c r="F153" s="3"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E154" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F154" s="2">
-        <f>F153/60</f>
-        <v>283.83333333333331</v>
+        <v>6</v>
+      </c>
+      <c r="F154" s="3">
+        <f>SUM(F2:F152)</f>
+        <v>17090</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E155" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F155" s="2">
+        <f>F154/60</f>
+        <v>284.83333333333331</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E156" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F155" s="2">
-        <f>F154/38.5</f>
-        <v>7.3722943722943715</v>
+      <c r="F156" s="2">
+        <f>F155/38.5</f>
+        <v>7.3982683982683977</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replaced Complex as the real and imaginary part can not be set seperate
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H156"/>
+  <dimension ref="A1:H160"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="F152" sqref="F152"/>
+      <selection activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F152" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F156" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G152" si="5">F132/60</f>
+        <f t="shared" ref="G132:G156" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4206,35 +4206,135 @@
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D153" s="1"/>
-      <c r="E153" s="1"/>
-      <c r="F153" s="3"/>
+      <c r="A153">
+        <v>2014</v>
+      </c>
+      <c r="B153">
+        <v>7</v>
+      </c>
+      <c r="C153">
+        <v>25</v>
+      </c>
+      <c r="D153" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E153" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F153" s="3">
+        <f t="shared" si="4"/>
+        <v>59.999999999999943</v>
+      </c>
+      <c r="G153" s="2">
+        <f t="shared" si="5"/>
+        <v>0.999999999999999</v>
+      </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E154" s="4" t="s">
+      <c r="A154">
+        <v>2014</v>
+      </c>
+      <c r="B154">
+        <v>7</v>
+      </c>
+      <c r="C154">
+        <v>25</v>
+      </c>
+      <c r="D154" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E154" s="1">
+        <v>0.71875</v>
+      </c>
+      <c r="F154" s="3">
+        <f t="shared" si="4"/>
+        <v>30.000000000000053</v>
+      </c>
+      <c r="G154" s="2">
+        <f t="shared" si="5"/>
+        <v>0.50000000000000089</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>2014</v>
+      </c>
+      <c r="B155">
+        <v>7</v>
+      </c>
+      <c r="C155">
+        <v>26</v>
+      </c>
+      <c r="D155" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="E155" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F155" s="3">
+        <f t="shared" si="4"/>
+        <v>60.000000000000028</v>
+      </c>
+      <c r="G155" s="2">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000004</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>2014</v>
+      </c>
+      <c r="B156">
+        <v>7</v>
+      </c>
+      <c r="C156">
+        <v>26</v>
+      </c>
+      <c r="D156" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E156" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F156" s="3">
+        <f t="shared" si="4"/>
+        <v>60.000000000000028</v>
+      </c>
+      <c r="G156" s="2">
+        <f t="shared" si="5"/>
+        <v>1.0000000000000004</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D157" s="1"/>
+      <c r="E157" s="1"/>
+      <c r="F157" s="3"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E158" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F154" s="3">
-        <f>SUM(F2:F152)</f>
-        <v>17090</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E155" s="4" t="s">
+      <c r="F158" s="3">
+        <f>SUM(F2:F156)</f>
+        <v>17300</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E159" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F155" s="2">
-        <f>F154/60</f>
-        <v>284.83333333333331</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E156" s="4" t="s">
+      <c r="F159" s="2">
+        <f>F158/60</f>
+        <v>288.33333333333331</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E160" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F156" s="2">
-        <f>F155/38.5</f>
-        <v>7.3982683982683977</v>
+      <c r="F160" s="2">
+        <f>F159/38.5</f>
+        <v>7.4891774891774885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented item source for nodes
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H161"/>
+  <dimension ref="A1:H162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="E157" sqref="E157"/>
+      <selection activeCell="F158" sqref="F158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F156" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F158" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G156" si="5">F132/60</f>
+        <f t="shared" ref="G132:G158" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4306,40 +4306,85 @@
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D157" s="1"/>
-      <c r="E157" s="1"/>
-      <c r="F157" s="3"/>
+      <c r="A157">
+        <v>2014</v>
+      </c>
+      <c r="B157">
+        <v>7</v>
+      </c>
+      <c r="C157">
+        <v>26</v>
+      </c>
+      <c r="D157" s="1">
+        <v>0.84375</v>
+      </c>
+      <c r="E157" s="1">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="F157" s="3">
+        <f t="shared" si="4"/>
+        <v>120.00000000000006</v>
+      </c>
+      <c r="G157" s="2">
+        <f t="shared" si="5"/>
+        <v>2.0000000000000009</v>
+      </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D158" s="1"/>
-      <c r="E158" s="1"/>
-      <c r="F158" s="3"/>
+      <c r="A158">
+        <v>2014</v>
+      </c>
+      <c r="B158">
+        <v>7</v>
+      </c>
+      <c r="C158">
+        <v>27</v>
+      </c>
+      <c r="D158" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E158" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F158" s="3">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="G158" s="2">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E159" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F159" s="3">
-        <f>SUM(F2:F156)</f>
-        <v>17370</v>
-      </c>
+      <c r="D159" s="1"/>
+      <c r="E159" s="1"/>
+      <c r="F159" s="3"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E160" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F160" s="2">
-        <f>F159/60</f>
-        <v>289.5</v>
+        <v>6</v>
+      </c>
+      <c r="F160" s="3">
+        <f>SUM(F2:F158)</f>
+        <v>17730</v>
       </c>
     </row>
     <row r="161" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E161" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F161" s="2">
+        <f>F160/60</f>
+        <v>295.5</v>
+      </c>
+    </row>
+    <row r="162" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E162" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F161" s="2">
-        <f>F160/38.5</f>
-        <v>7.5194805194805197</v>
+      <c r="F162" s="2">
+        <f>F161/38.5</f>
+        <v>7.6753246753246751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prepared connection to SQL database
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:H164"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="F160" sqref="F160"/>
+      <selection activeCell="L158" sqref="L158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4394,15 +4394,15 @@
         <v>0.61805555555555558</v>
       </c>
       <c r="E160" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="F160" s="3">
         <f t="shared" si="4"/>
-        <v>69.999999999999915</v>
+        <v>114.99999999999991</v>
       </c>
       <c r="G160" s="2">
         <f t="shared" si="5"/>
-        <v>1.1666666666666652</v>
+        <v>1.9166666666666652</v>
       </c>
     </row>
     <row r="161" spans="4:6" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
       </c>
       <c r="F162" s="3">
         <f>SUM(F2:F160)</f>
-        <v>17875</v>
+        <v>17920</v>
       </c>
     </row>
     <row r="163" spans="4:6" x14ac:dyDescent="0.25">
@@ -4425,7 +4425,7 @@
       </c>
       <c r="F163" s="2">
         <f>F162/60</f>
-        <v>297.91666666666669</v>
+        <v>298.66666666666669</v>
       </c>
     </row>
     <row r="164" spans="4:6" x14ac:dyDescent="0.25">
@@ -4434,7 +4434,7 @@
       </c>
       <c r="F164" s="2">
         <f>F163/38.5</f>
-        <v>7.738095238095239</v>
+        <v>7.7575757575757578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
catch errors which occur if the net is invalid
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H164"/>
+  <dimension ref="A1:H165"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="L158" sqref="L158"/>
+      <selection activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F160" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F161" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G160" si="5">F132/60</f>
+        <f t="shared" ref="G132:G161" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4405,36 +4405,61 @@
         <v>1.9166666666666652</v>
       </c>
     </row>
-    <row r="161" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D161" s="1"/>
-      <c r="E161" s="1"/>
-      <c r="F161" s="3"/>
-    </row>
-    <row r="162" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E162" s="4" t="s">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>2014</v>
+      </c>
+      <c r="B161">
+        <v>7</v>
+      </c>
+      <c r="C161">
+        <v>28</v>
+      </c>
+      <c r="D161" s="1">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E161" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F161" s="3">
+        <f t="shared" si="4"/>
+        <v>209.99999999999997</v>
+      </c>
+      <c r="G161" s="2">
+        <f t="shared" si="5"/>
+        <v>3.4999999999999996</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D162" s="1"/>
+      <c r="E162" s="1"/>
+      <c r="F162" s="3"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E163" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F162" s="3">
-        <f>SUM(F2:F160)</f>
-        <v>17920</v>
-      </c>
-    </row>
-    <row r="163" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E163" s="4" t="s">
+      <c r="F163" s="3">
+        <f>SUM(F2:F161)</f>
+        <v>18130</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E164" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F163" s="2">
-        <f>F162/60</f>
-        <v>298.66666666666669</v>
-      </c>
-    </row>
-    <row r="164" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E164" s="4" t="s">
+      <c r="F164" s="2">
+        <f>F163/60</f>
+        <v>302.16666666666669</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E165" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F164" s="2">
-        <f>F163/38.5</f>
-        <v>7.7575757575757578</v>
+      <c r="F165" s="2">
+        <f>F164/38.5</f>
+        <v>7.8484848484848486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented creation of SQL connection
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H165"/>
+  <dimension ref="A1:H167"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="A162" sqref="A162"/>
+      <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F161" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F162" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G161" si="5">F132/60</f>
+        <f t="shared" ref="G132:G162" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4419,47 +4419,88 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="E161" s="1">
-        <v>0.5</v>
+        <v>0.4375</v>
       </c>
       <c r="F161" s="3">
         <f t="shared" si="4"/>
-        <v>209.99999999999997</v>
+        <v>119.99999999999997</v>
       </c>
       <c r="G161" s="2">
         <f t="shared" si="5"/>
-        <v>3.4999999999999996</v>
+        <v>1.9999999999999996</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D162" s="1"/>
-      <c r="E162" s="1"/>
-      <c r="F162" s="3"/>
+      <c r="A162">
+        <v>2014</v>
+      </c>
+      <c r="B162">
+        <v>7</v>
+      </c>
+      <c r="C162">
+        <v>28</v>
+      </c>
+      <c r="D162" s="1">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E162" s="1">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="F162" s="3">
+        <f t="shared" si="4"/>
+        <v>30.000000000000053</v>
+      </c>
+      <c r="G162" s="2">
+        <f t="shared" si="5"/>
+        <v>0.50000000000000089</v>
+      </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E163" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F163" s="3">
-        <f>SUM(F2:F161)</f>
-        <v>18130</v>
-      </c>
+      <c r="A163">
+        <v>2014</v>
+      </c>
+      <c r="B163">
+        <v>7</v>
+      </c>
+      <c r="C163">
+        <v>28</v>
+      </c>
+      <c r="D163" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E163" s="1"/>
+      <c r="F163" s="3"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E164" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F164" s="2">
-        <f>F163/60</f>
-        <v>302.16666666666669</v>
-      </c>
+      <c r="D164" s="1"/>
+      <c r="E164" s="1"/>
+      <c r="F164" s="3"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E165" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F165" s="3">
+        <f>SUM(F2:F162)</f>
+        <v>18070</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E166" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F166" s="2">
+        <f>F165/60</f>
+        <v>301.16666666666669</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E167" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F165" s="2">
-        <f>F164/38.5</f>
-        <v>7.8484848484848486</v>
+      <c r="F167" s="2">
+        <f>F166/38.5</f>
+        <v>7.8225108225108233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented creation of tables if necessary
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H167"/>
+  <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="E163" sqref="E163"/>
+      <selection activeCell="F164" sqref="F164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F162" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F164" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G162" si="5">F132/60</f>
+        <f t="shared" ref="G132:G164" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4468,39 +4468,73 @@
       <c r="D163" s="1">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E163" s="1"/>
-      <c r="F163" s="3"/>
+      <c r="E163" s="1">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="F163" s="3">
+        <f t="shared" si="4"/>
+        <v>195.00000000000011</v>
+      </c>
+      <c r="G163" s="2">
+        <f t="shared" si="5"/>
+        <v>3.2500000000000018</v>
+      </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D164" s="1"/>
-      <c r="E164" s="1"/>
-      <c r="F164" s="3"/>
+      <c r="A164">
+        <v>2014</v>
+      </c>
+      <c r="B164">
+        <v>7</v>
+      </c>
+      <c r="C164">
+        <v>29</v>
+      </c>
+      <c r="D164" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E164" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F164" s="3">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="G164" s="2">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E165" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F165" s="3">
-        <f>SUM(F2:F162)</f>
-        <v>18070</v>
-      </c>
+      <c r="D165" s="1"/>
+      <c r="E165" s="1"/>
+      <c r="F165" s="3"/>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E166" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F166" s="2">
-        <f>F165/60</f>
-        <v>301.16666666666669</v>
+        <v>6</v>
+      </c>
+      <c r="F166" s="3">
+        <f>SUM(F2:F164)</f>
+        <v>18505</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E167" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F167" s="2">
+        <f>F166/60</f>
+        <v>308.41666666666669</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E168" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F167" s="2">
-        <f>F166/38.5</f>
-        <v>7.8225108225108233</v>
+      <c r="F168" s="2">
+        <f>F167/38.5</f>
+        <v>8.0108225108225106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented update of power net
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H168"/>
+  <dimension ref="A1:H169"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="F164" sqref="F164"/>
+      <selection activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F164" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F165" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G164" si="5">F132/60</f>
+        <f t="shared" ref="G132:G165" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4494,47 +4494,72 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E164" s="1">
-        <v>0.5</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="F164" s="3">
         <f t="shared" si="4"/>
-        <v>240</v>
+        <v>270.00000000000011</v>
       </c>
       <c r="G164" s="2">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>4.5000000000000018</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D165" s="1"/>
-      <c r="E165" s="1"/>
-      <c r="F165" s="3"/>
+      <c r="A165">
+        <v>2014</v>
+      </c>
+      <c r="B165">
+        <v>7</v>
+      </c>
+      <c r="C165">
+        <v>29</v>
+      </c>
+      <c r="D165" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="E165" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F165" s="3">
+        <f t="shared" si="4"/>
+        <v>59.999999999999943</v>
+      </c>
+      <c r="G165" s="2">
+        <f t="shared" si="5"/>
+        <v>0.999999999999999</v>
+      </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E166" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F166" s="3">
-        <f>SUM(F2:F164)</f>
-        <v>18505</v>
-      </c>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
+      <c r="F166" s="3"/>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E167" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F167" s="2">
-        <f>F166/60</f>
-        <v>308.41666666666669</v>
+        <v>6</v>
+      </c>
+      <c r="F167" s="3">
+        <f>SUM(F2:F165)</f>
+        <v>18595</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E168" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F168" s="2">
+        <f>F167/60</f>
+        <v>309.91666666666669</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E169" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F168" s="2">
-        <f>F167/38.5</f>
-        <v>8.0108225108225106</v>
+      <c r="F169" s="2">
+        <f>F168/38.5</f>
+        <v>8.0497835497835499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented reading of generators and transformers
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H169"/>
+  <dimension ref="A1:H170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="F165" sqref="F165"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="E167" sqref="E167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F165" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F166" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G165" si="5">F132/60</f>
+        <f t="shared" ref="G132:G166" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4531,35 +4531,60 @@
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D166" s="1"/>
-      <c r="E166" s="1"/>
-      <c r="F166" s="3"/>
+      <c r="A166">
+        <v>2014</v>
+      </c>
+      <c r="B166">
+        <v>7</v>
+      </c>
+      <c r="C166">
+        <v>29</v>
+      </c>
+      <c r="D166" s="1">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E166" s="1">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="F166" s="3">
+        <f t="shared" si="4"/>
+        <v>109.99999999999993</v>
+      </c>
+      <c r="G166" s="2">
+        <f t="shared" si="5"/>
+        <v>1.8333333333333321</v>
+      </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E167" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F167" s="3">
-        <f>SUM(F2:F165)</f>
-        <v>18595</v>
-      </c>
+      <c r="D167" s="1"/>
+      <c r="E167" s="1"/>
+      <c r="F167" s="3"/>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E168" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F168" s="2">
-        <f>F167/60</f>
-        <v>309.91666666666669</v>
+        <v>6</v>
+      </c>
+      <c r="F168" s="3">
+        <f>SUM(F2:F166)</f>
+        <v>18705</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E169" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F169" s="2">
+        <f>F168/60</f>
+        <v>311.75</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E170" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F169" s="2">
-        <f>F168/38.5</f>
-        <v>8.0497835497835499</v>
+      <c r="F170" s="2">
+        <f>F169/38.5</f>
+        <v>8.0974025974025974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made nodes nullable in the database
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -396,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="E167" sqref="E167"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="N164" sqref="N164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4544,15 +4544,15 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="E166" s="1">
-        <v>0.85416666666666663</v>
+        <v>0.86458333333333337</v>
       </c>
       <c r="F166" s="3">
         <f t="shared" si="4"/>
-        <v>109.99999999999993</v>
+        <v>125.00000000000003</v>
       </c>
       <c r="G166" s="2">
         <f t="shared" si="5"/>
-        <v>1.8333333333333321</v>
+        <v>2.0833333333333339</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -4566,7 +4566,7 @@
       </c>
       <c r="F168" s="3">
         <f>SUM(F2:F166)</f>
-        <v>18705</v>
+        <v>18720</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -4575,7 +4575,7 @@
       </c>
       <c r="F169" s="2">
         <f>F168/60</f>
-        <v>311.75</v>
+        <v>312</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -4584,7 +4584,7 @@
       </c>
       <c r="F170" s="2">
         <f>F169/38.5</f>
-        <v>8.0974025974025974</v>
+        <v>8.103896103896103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented handling of null values in the database
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H170"/>
+  <dimension ref="A1:H171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="N164" sqref="N164"/>
+      <selection activeCell="D168" sqref="D168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F166" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F167" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G166" si="5">F132/60</f>
+        <f t="shared" ref="G132:G167" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4556,35 +4556,60 @@
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D167" s="1"/>
-      <c r="E167" s="1"/>
-      <c r="F167" s="3"/>
+      <c r="A167">
+        <v>2014</v>
+      </c>
+      <c r="B167">
+        <v>7</v>
+      </c>
+      <c r="C167">
+        <v>30</v>
+      </c>
+      <c r="D167" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E167" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F167" s="3">
+        <f t="shared" si="4"/>
+        <v>255.00000000000006</v>
+      </c>
+      <c r="G167" s="2">
+        <f t="shared" si="5"/>
+        <v>4.2500000000000009</v>
+      </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E168" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F168" s="3">
-        <f>SUM(F2:F166)</f>
-        <v>18720</v>
-      </c>
+      <c r="D168" s="1"/>
+      <c r="E168" s="1"/>
+      <c r="F168" s="3"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E169" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F169" s="2">
-        <f>F168/60</f>
-        <v>312</v>
+        <v>6</v>
+      </c>
+      <c r="F169" s="3">
+        <f>SUM(F2:F167)</f>
+        <v>18975</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E170" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F170" s="2">
+        <f>F169/60</f>
+        <v>316.25</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E171" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F170" s="2">
-        <f>F169/38.5</f>
-        <v>8.103896103896103</v>
+      <c r="F171" s="2">
+        <f>F170/38.5</f>
+        <v>8.2142857142857135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up admittance matrix
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H171"/>
+  <dimension ref="A1:H172"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="D168" sqref="D168"/>
+      <selection activeCell="E168" sqref="E168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4581,34 +4581,50 @@
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D168" s="1"/>
+      <c r="A168">
+        <v>2014</v>
+      </c>
+      <c r="B168">
+        <v>7</v>
+      </c>
+      <c r="C168">
+        <v>30</v>
+      </c>
+      <c r="D168" s="1">
+        <v>0.84375</v>
+      </c>
       <c r="E168" s="1"/>
       <c r="F168" s="3"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E169" s="4" t="s">
+      <c r="D169" s="1"/>
+      <c r="E169" s="1"/>
+      <c r="F169" s="3"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E170" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F169" s="3">
+      <c r="F170" s="3">
         <f>SUM(F2:F167)</f>
         <v>18975</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E170" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F170" s="2">
-        <f>F169/60</f>
-        <v>316.25</v>
-      </c>
-    </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E171" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F171" s="2">
+        <f>F170/60</f>
+        <v>316.25</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E172" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F171" s="2">
-        <f>F170/38.5</f>
+      <c r="F172" s="2">
+        <f>F171/38.5</f>
         <v>8.2142857142857135</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added test with transformer with phase shift
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H172"/>
+  <dimension ref="A1:H173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="E169" sqref="E169"/>
+      <selection activeCell="E170" sqref="E170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F168" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F169" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G168" si="5">F132/60</f>
+        <f t="shared" ref="G132:G169" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4606,35 +4606,60 @@
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D169" s="1"/>
-      <c r="E169" s="1"/>
-      <c r="F169" s="3"/>
+      <c r="A169">
+        <v>2014</v>
+      </c>
+      <c r="B169">
+        <v>7</v>
+      </c>
+      <c r="C169">
+        <v>31</v>
+      </c>
+      <c r="D169" s="1">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="E169" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F169" s="3">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="G169" s="2">
+        <f t="shared" si="5"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E170" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F170" s="3">
-        <f>SUM(F2:F168)</f>
-        <v>19095</v>
-      </c>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1"/>
+      <c r="F170" s="3"/>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E171" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F171" s="2">
-        <f>F170/60</f>
-        <v>318.25</v>
+        <v>6</v>
+      </c>
+      <c r="F171" s="3">
+        <f>SUM(F2:F169)</f>
+        <v>19140</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E172" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F172" s="2">
+        <f>F171/60</f>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E173" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F172" s="2">
-        <f>F171/38.5</f>
-        <v>8.2662337662337659</v>
+      <c r="F173" s="2">
+        <f>F172/38.5</f>
+        <v>8.2857142857142865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up single phase node
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H173"/>
+  <dimension ref="A1:H174"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="E170" sqref="E170"/>
+      <selection activeCell="F170" sqref="F170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F169" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F170" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G169" si="5">F132/60</f>
+        <f t="shared" ref="G132:G170" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4619,47 +4619,72 @@
         <v>0.36458333333333331</v>
       </c>
       <c r="E169" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="F169" s="3">
         <f t="shared" si="4"/>
-        <v>45</v>
+        <v>30.000000000000053</v>
       </c>
       <c r="G169" s="2">
         <f t="shared" si="5"/>
+        <v>0.50000000000000089</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>2014</v>
+      </c>
+      <c r="B170">
+        <v>7</v>
+      </c>
+      <c r="C170">
+        <v>31</v>
+      </c>
+      <c r="D170" s="1">
+        <v>0.59375</v>
+      </c>
+      <c r="E170" s="1">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D170" s="1"/>
-      <c r="E170" s="1"/>
-      <c r="F170" s="3"/>
+      <c r="F170" s="3">
+        <f t="shared" si="4"/>
+        <v>225</v>
+      </c>
+      <c r="G170" s="2">
+        <f t="shared" si="5"/>
+        <v>3.75</v>
+      </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E171" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F171" s="3">
-        <f>SUM(F2:F169)</f>
-        <v>19140</v>
-      </c>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="3"/>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E172" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F172" s="2">
-        <f>F171/60</f>
-        <v>319</v>
+        <v>6</v>
+      </c>
+      <c r="F172" s="3">
+        <f>SUM(F2:F170)</f>
+        <v>19350</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E173" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F173" s="2">
+        <f>F172/60</f>
+        <v>322.5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E174" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F173" s="2">
-        <f>F172/38.5</f>
-        <v>8.2857142857142865</v>
+      <c r="F174" s="2">
+        <f>F173/38.5</f>
+        <v>8.3766233766233764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
internal nodes copy the nominal phase shift from their source nodes
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -4644,15 +4644,15 @@
         <v>0.59375</v>
       </c>
       <c r="E170" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="F170" s="3">
         <f t="shared" si="4"/>
-        <v>104.99999999999994</v>
+        <v>165.00000000000006</v>
       </c>
       <c r="G170" s="2">
         <f t="shared" si="5"/>
-        <v>1.7499999999999991</v>
+        <v>2.7500000000000009</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -4666,7 +4666,7 @@
       </c>
       <c r="F172" s="3">
         <f>SUM(F2:F170)</f>
-        <v>19230</v>
+        <v>19290</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -4675,7 +4675,7 @@
       </c>
       <c r="F173" s="2">
         <f>F172/60</f>
-        <v>320.5</v>
+        <v>321.5</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -4684,7 +4684,7 @@
       </c>
       <c r="F174" s="2">
         <f>F173/38.5</f>
-        <v>8.324675324675324</v>
+        <v>8.3506493506493502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved accuracy of current iteration
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H175"/>
+  <dimension ref="A1:H176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A172" sqref="A172"/>
+      <selection activeCell="E173" sqref="E173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F171" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F172" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G171" si="5">F132/60</f>
+        <f t="shared" ref="G132:G172" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4681,35 +4681,60 @@
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D172" s="1"/>
-      <c r="E172" s="1"/>
-      <c r="F172" s="3"/>
+      <c r="A172">
+        <v>2014</v>
+      </c>
+      <c r="B172">
+        <v>8</v>
+      </c>
+      <c r="C172">
+        <v>3</v>
+      </c>
+      <c r="D172" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E172" s="1">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="F172" s="3">
+        <f t="shared" si="4"/>
+        <v>99.999999999999972</v>
+      </c>
+      <c r="G172" s="2">
+        <f t="shared" si="5"/>
+        <v>1.6666666666666663</v>
+      </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E173" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F173" s="3">
-        <f>SUM(F2:F171)</f>
-        <v>19345</v>
-      </c>
+      <c r="D173" s="1"/>
+      <c r="E173" s="1"/>
+      <c r="F173" s="3"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E174" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F174" s="2">
-        <f>F173/60</f>
-        <v>322.41666666666669</v>
+        <v>6</v>
+      </c>
+      <c r="F174" s="3">
+        <f>SUM(F2:F172)</f>
+        <v>19445</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E175" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F175" s="2">
+        <f>F174/60</f>
+        <v>324.08333333333331</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E176" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F175" s="2">
-        <f>F174/38.5</f>
-        <v>8.3744588744588757</v>
+      <c r="F176" s="2">
+        <f>F175/38.5</f>
+        <v>8.4177489177489164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test to verify model of line
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H176"/>
+  <dimension ref="A1:H178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="E172" sqref="E172"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="E174" sqref="E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,11 +3697,11 @@
         <v>0.92708333333333337</v>
       </c>
       <c r="F132" s="3">
-        <f t="shared" ref="F132:F172" si="4">(E132-D132)*24*60</f>
+        <f t="shared" ref="F132:F173" si="4">(E132-D132)*24*60</f>
         <v>120.00000000000006</v>
       </c>
       <c r="G132" s="2">
-        <f t="shared" ref="G132:G172" si="5">F132/60</f>
+        <f t="shared" ref="G132:G173" si="5">F132/60</f>
         <v>2.0000000000000009</v>
       </c>
     </row>
@@ -4706,35 +4706,76 @@
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D173" s="1"/>
-      <c r="E173" s="1"/>
-      <c r="F173" s="3"/>
+      <c r="A173">
+        <v>2014</v>
+      </c>
+      <c r="B173">
+        <v>8</v>
+      </c>
+      <c r="C173">
+        <v>4</v>
+      </c>
+      <c r="D173" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E173" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="F173" s="3">
+        <f t="shared" si="4"/>
+        <v>74.999999999999972</v>
+      </c>
+      <c r="G173" s="2">
+        <f t="shared" si="5"/>
+        <v>1.2499999999999996</v>
+      </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E174" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F174" s="3">
-        <f>SUM(F2:F172)</f>
-        <v>19415</v>
-      </c>
+      <c r="A174">
+        <v>2014</v>
+      </c>
+      <c r="B174">
+        <v>8</v>
+      </c>
+      <c r="C174">
+        <v>4</v>
+      </c>
+      <c r="D174" s="1">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="E174" s="1"/>
+      <c r="F174" s="3"/>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E175" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F175" s="2">
-        <f>F174/60</f>
-        <v>323.58333333333331</v>
-      </c>
+      <c r="D175" s="1"/>
+      <c r="E175" s="1"/>
+      <c r="F175" s="3"/>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E176" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F176" s="3">
+        <f>SUM(F2:F173)</f>
+        <v>19490</v>
+      </c>
+    </row>
+    <row r="177" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E177" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F177" s="2">
+        <f>F176/60</f>
+        <v>324.83333333333331</v>
+      </c>
+    </row>
+    <row r="178" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E178" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F176" s="2">
-        <f>F175/38.5</f>
-        <v>8.4047619047619051</v>
+      <c r="F178" s="2">
+        <f>F177/38.5</f>
+        <v>8.437229437229437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update UI and removed phase shift of transformer
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H179"/>
+  <dimension ref="A1:H180"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="M169" sqref="M169"/>
+      <selection activeCell="I176" sqref="I176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4781,34 +4781,59 @@
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D176" s="1"/>
-      <c r="E176" s="1"/>
-      <c r="F176" s="3"/>
-    </row>
-    <row r="177" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E177" s="4" t="s">
+      <c r="A176">
+        <v>2014</v>
+      </c>
+      <c r="B176">
+        <v>8</v>
+      </c>
+      <c r="C176">
+        <v>5</v>
+      </c>
+      <c r="D176" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E176" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="F176" s="3">
+        <f t="shared" ref="F176" si="6">(E176-D176)*24*60</f>
+        <v>120.00000000000006</v>
+      </c>
+      <c r="G176" s="2">
+        <f t="shared" ref="G176" si="7">F176/60</f>
+        <v>2.0000000000000009</v>
+      </c>
+    </row>
+    <row r="177" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D177" s="1"/>
+      <c r="E177" s="1"/>
+      <c r="F177" s="3"/>
+    </row>
+    <row r="178" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E178" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F177" s="3">
+      <c r="F178" s="3">
         <f>SUM(F2:F175)</f>
         <v>19815</v>
       </c>
     </row>
-    <row r="178" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E178" s="4" t="s">
+    <row r="179" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E179" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F178" s="2">
-        <f>F177/60</f>
+      <c r="F179" s="2">
+        <f>F178/60</f>
         <v>330.25</v>
       </c>
     </row>
-    <row r="179" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E179" s="4" t="s">
+    <row r="180" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E180" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F179" s="2">
-        <f>F178/38.5</f>
+      <c r="F180" s="2">
+        <f>F179/38.5</f>
         <v>8.5779220779220786</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented storage of admittance matrix in the database
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -396,8 +396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="I176" sqref="I176"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="E177" sqref="E177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4794,15 +4794,15 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="E176" s="1">
-        <v>0.875</v>
+        <v>0.88541666666666663</v>
       </c>
       <c r="F176" s="3">
         <f t="shared" ref="F176" si="6">(E176-D176)*24*60</f>
-        <v>120.00000000000006</v>
+        <v>135</v>
       </c>
       <c r="G176" s="2">
         <f t="shared" ref="G176" si="7">F176/60</f>
-        <v>2.0000000000000009</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="177" spans="4:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cleaned up load flow calculator
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H181"/>
+  <dimension ref="A1:H182"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A178" sqref="A178"/>
+      <selection activeCell="A179" sqref="A179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4831,34 +4831,50 @@
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D178" s="1"/>
+      <c r="A178">
+        <v>2014</v>
+      </c>
+      <c r="B178">
+        <v>8</v>
+      </c>
+      <c r="C178">
+        <v>8</v>
+      </c>
+      <c r="D178" s="1">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="E178" s="1"/>
       <c r="F178" s="3"/>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E179" s="4" t="s">
+      <c r="D179" s="1"/>
+      <c r="E179" s="1"/>
+      <c r="F179" s="3"/>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E180" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F179" s="3">
+      <c r="F180" s="3">
         <f>SUM(F2:F175)</f>
         <v>19815</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E180" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F180" s="2">
-        <f>F179/60</f>
-        <v>330.25</v>
-      </c>
-    </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E181" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F181" s="2">
+        <f>F180/60</f>
+        <v>330.25</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E182" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F181" s="2">
-        <f>F180/38.5</f>
+      <c r="F182" s="2">
+        <f>F181/38.5</f>
         <v>8.5779220779220786</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added test for symmetric power net
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H182"/>
+  <dimension ref="A1:H183"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A179" sqref="A179"/>
+      <selection activeCell="E179" sqref="E179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4797,11 +4797,11 @@
         <v>0.88541666666666663</v>
       </c>
       <c r="F176" s="3">
-        <f t="shared" ref="F176:F177" si="6">(E176-D176)*24*60</f>
+        <f t="shared" ref="F176:F178" si="6">(E176-D176)*24*60</f>
         <v>135</v>
       </c>
       <c r="G176" s="2">
-        <f t="shared" ref="G176:G177" si="7">F176/60</f>
+        <f t="shared" ref="G176:G178" si="7">F176/60</f>
         <v>2.25</v>
       </c>
     </row>
@@ -4838,43 +4838,68 @@
         <v>8</v>
       </c>
       <c r="C178">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D178" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E178" s="1"/>
-      <c r="F178" s="3"/>
+      <c r="E178" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="F178" s="3">
+        <f t="shared" si="6"/>
+        <v>59.999999999999943</v>
+      </c>
+      <c r="G178" s="2">
+        <f t="shared" si="7"/>
+        <v>0.999999999999999</v>
+      </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D179" s="1"/>
+      <c r="A179">
+        <v>2014</v>
+      </c>
+      <c r="B179">
+        <v>8</v>
+      </c>
+      <c r="C179">
+        <v>7</v>
+      </c>
+      <c r="D179" s="1">
+        <v>0.65277777777777779</v>
+      </c>
       <c r="E179" s="1"/>
       <c r="F179" s="3"/>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E180" s="4" t="s">
+      <c r="D180" s="1"/>
+      <c r="E180" s="1"/>
+      <c r="F180" s="3"/>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E181" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F180" s="3">
+      <c r="F181" s="3">
         <f>SUM(F2:F175)</f>
         <v>19815</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E181" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F181" s="2">
-        <f>F180/60</f>
-        <v>330.25</v>
-      </c>
-    </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E182" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F182" s="2">
+        <f>F181/60</f>
+        <v>330.25</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E183" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F182" s="2">
-        <f>F181/38.5</f>
+      <c r="F183" s="2">
+        <f>F182/38.5</f>
         <v>8.5779220779220786</v>
       </c>
     </row>

</xml_diff>

<commit_message>
improved interface for detection of voltage collapse
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H183"/>
+  <dimension ref="A1:H185"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="D180" sqref="D180"/>
+      <selection activeCell="E181" sqref="E181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4797,11 +4797,11 @@
         <v>0.88541666666666663</v>
       </c>
       <c r="F176" s="3">
-        <f t="shared" ref="F176:F179" si="6">(E176-D176)*24*60</f>
+        <f t="shared" ref="F176:F180" si="6">(E176-D176)*24*60</f>
         <v>135</v>
       </c>
       <c r="G176" s="2">
-        <f t="shared" ref="G176:G179" si="7">F176/60</f>
+        <f t="shared" ref="G176:G180" si="7">F176/60</f>
         <v>2.25</v>
       </c>
     </row>
@@ -4881,34 +4881,75 @@
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D180" s="1"/>
-      <c r="E180" s="1"/>
-      <c r="F180" s="3"/>
+      <c r="A180">
+        <v>2014</v>
+      </c>
+      <c r="B180">
+        <v>8</v>
+      </c>
+      <c r="C180">
+        <v>11</v>
+      </c>
+      <c r="D180" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="E180" s="1">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="F180" s="3">
+        <f t="shared" si="6"/>
+        <v>59.999999999999943</v>
+      </c>
+      <c r="G180" s="2">
+        <f t="shared" si="7"/>
+        <v>0.999999999999999</v>
+      </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E181" s="4" t="s">
+      <c r="A181">
+        <v>2014</v>
+      </c>
+      <c r="B181">
+        <v>8</v>
+      </c>
+      <c r="C181">
+        <v>11</v>
+      </c>
+      <c r="D181" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E181" s="1"/>
+      <c r="F181" s="3"/>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D182" s="1"/>
+      <c r="E182" s="1"/>
+      <c r="F182" s="3"/>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E183" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F181" s="3">
+      <c r="F183" s="3">
         <f>SUM(F2:F175)</f>
         <v>19815</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E182" s="4" t="s">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E184" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F182" s="2">
-        <f>F181/60</f>
+      <c r="F184" s="2">
+        <f>F183/60</f>
         <v>330.25</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E183" s="4" t="s">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E185" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F183" s="2">
-        <f>F182/38.5</f>
+      <c r="F185" s="2">
+        <f>F184/38.5</f>
         <v>8.5779220779220786</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added chart for convergence
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H185"/>
+  <dimension ref="A1:H189"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="E181" sqref="E181"/>
+      <selection activeCell="C183" sqref="C183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4797,11 +4797,11 @@
         <v>0.88541666666666663</v>
       </c>
       <c r="F176" s="3">
-        <f t="shared" ref="F176:F180" si="6">(E176-D176)*24*60</f>
+        <f t="shared" ref="F176:F184" si="6">(E176-D176)*24*60</f>
         <v>135</v>
       </c>
       <c r="G176" s="2">
-        <f t="shared" ref="G176:G180" si="7">F176/60</f>
+        <f t="shared" ref="G176:G184" si="7">F176/60</f>
         <v>2.25</v>
       </c>
     </row>
@@ -4918,38 +4918,138 @@
       <c r="D181" s="1">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E181" s="1"/>
-      <c r="F181" s="3"/>
+      <c r="E181" s="1">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="F181" s="3">
+        <f t="shared" si="6"/>
+        <v>135</v>
+      </c>
+      <c r="G181" s="2">
+        <f t="shared" si="7"/>
+        <v>2.25</v>
+      </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D182" s="1"/>
-      <c r="E182" s="1"/>
-      <c r="F182" s="3"/>
+      <c r="A182">
+        <v>2014</v>
+      </c>
+      <c r="B182">
+        <v>8</v>
+      </c>
+      <c r="C182" s="3">
+        <v>12</v>
+      </c>
+      <c r="D182" s="1">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="E182" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F182" s="3">
+        <f t="shared" si="6"/>
+        <v>20.000000000000007</v>
+      </c>
+      <c r="G182" s="2">
+        <f t="shared" si="7"/>
+        <v>0.33333333333333343</v>
+      </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E183" s="4" t="s">
+      <c r="A183">
+        <v>2014</v>
+      </c>
+      <c r="B183">
+        <v>8</v>
+      </c>
+      <c r="C183" s="3">
+        <v>12</v>
+      </c>
+      <c r="D183" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E183" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F183" s="3">
+        <f t="shared" si="6"/>
+        <v>74.999999999999886</v>
+      </c>
+      <c r="G183" s="2">
+        <f t="shared" si="7"/>
+        <v>1.249999999999998</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>2014</v>
+      </c>
+      <c r="B184">
+        <v>8</v>
+      </c>
+      <c r="C184" s="3">
+        <v>13</v>
+      </c>
+      <c r="D184" s="1">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="E184" s="1">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="F184" s="3">
+        <f t="shared" si="6"/>
+        <v>180.00000000000009</v>
+      </c>
+      <c r="G184" s="2">
+        <f t="shared" si="7"/>
+        <v>3.0000000000000013</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>2014</v>
+      </c>
+      <c r="B185">
+        <v>8</v>
+      </c>
+      <c r="C185" s="3">
+        <v>14</v>
+      </c>
+      <c r="D185" s="1">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E185" s="1"/>
+      <c r="F185" s="3"/>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D186" s="1"/>
+      <c r="E186" s="1"/>
+      <c r="F186" s="3"/>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E187" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F183" s="3">
+      <c r="F187" s="3">
         <f>SUM(F2:F175)</f>
         <v>19815</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E184" s="4" t="s">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E188" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F184" s="2">
-        <f>F183/60</f>
+      <c r="F188" s="2">
+        <f>F187/60</f>
         <v>330.25</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E185" s="4" t="s">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E189" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F185" s="2">
-        <f>F184/38.5</f>
+      <c r="F189" s="2">
+        <f>F188/38.5</f>
         <v>8.5779220779220786</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added flag for less accurate model of a connection
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H185"/>
+  <dimension ref="A1:H186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="E181" sqref="E181"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="E182" sqref="E182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4922,34 +4922,50 @@
       <c r="F181" s="3"/>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D182" s="1"/>
+      <c r="A182">
+        <v>2014</v>
+      </c>
+      <c r="B182">
+        <v>8</v>
+      </c>
+      <c r="C182">
+        <v>18</v>
+      </c>
+      <c r="D182" s="1">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="E182" s="1"/>
       <c r="F182" s="3"/>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E183" s="4" t="s">
+      <c r="D183" s="1"/>
+      <c r="E183" s="1"/>
+      <c r="F183" s="3"/>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E184" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F183" s="3">
+      <c r="F184" s="3">
         <f>SUM(F2:F175)</f>
         <v>19815</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E184" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F184" s="2">
-        <f>F183/60</f>
-        <v>330.25</v>
-      </c>
-    </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E185" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F185" s="2">
+        <f>F184/60</f>
+        <v>330.25</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E186" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F185" s="2">
-        <f>F184/38.5</f>
+      <c r="F186" s="2">
+        <f>F185/38.5</f>
         <v>8.5779220779220786</v>
       </c>
     </row>

</xml_diff>

<commit_message>
exported charts from excel sheet
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H189"/>
+  <dimension ref="A1:H191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="E186" sqref="E186"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="E187" sqref="E187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4797,11 +4797,11 @@
         <v>0.88541666666666663</v>
       </c>
       <c r="F176" s="3">
-        <f t="shared" ref="F176:F185" si="6">(E176-D176)*24*60</f>
+        <f t="shared" ref="F176:F186" si="6">(E176-D176)*24*60</f>
         <v>135</v>
       </c>
       <c r="G176" s="2">
-        <f t="shared" ref="G176:G185" si="7">F176/60</f>
+        <f t="shared" ref="G176:G186" si="7">F176/60</f>
         <v>2.25</v>
       </c>
     </row>
@@ -5031,35 +5031,76 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D186" s="1"/>
-      <c r="E186" s="1"/>
-      <c r="F186" s="3"/>
+      <c r="A186">
+        <v>2014</v>
+      </c>
+      <c r="B186">
+        <v>8</v>
+      </c>
+      <c r="C186" s="3">
+        <v>18</v>
+      </c>
+      <c r="D186" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E186" s="1">
+        <v>0.71875</v>
+      </c>
+      <c r="F186" s="3">
+        <f t="shared" si="6"/>
+        <v>165.00000000000006</v>
+      </c>
+      <c r="G186" s="2">
+        <f t="shared" si="7"/>
+        <v>2.7500000000000009</v>
+      </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E187" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F187" s="3">
-        <f>SUM(F2:F185)</f>
-        <v>20860</v>
-      </c>
+      <c r="A187">
+        <v>2014</v>
+      </c>
+      <c r="B187">
+        <v>8</v>
+      </c>
+      <c r="C187" s="3">
+        <v>18</v>
+      </c>
+      <c r="D187" s="1">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="E187" s="1"/>
+      <c r="F187" s="3"/>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E188" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F188" s="2">
-        <f>F187/60</f>
-        <v>347.66666666666669</v>
-      </c>
+      <c r="D188" s="1"/>
+      <c r="E188" s="1"/>
+      <c r="F188" s="3"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E189" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F189" s="3">
+        <f>SUM(F2:F186)</f>
+        <v>21025</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E190" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F190" s="2">
+        <f>F189/60</f>
+        <v>350.41666666666669</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E191" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F189" s="2">
-        <f>F188/38.5</f>
-        <v>9.0303030303030312</v>
+      <c r="F191" s="2">
+        <f>F190/38.5</f>
+        <v>9.1017316017316023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added experiment to test the capabilities if the power net is close to voltage collapse
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H191"/>
+  <dimension ref="A1:H192"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="E187" sqref="E187"/>
+      <selection activeCell="E188" sqref="E188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4797,11 +4797,11 @@
         <v>0.88541666666666663</v>
       </c>
       <c r="F176" s="3">
-        <f t="shared" ref="F176:F186" si="6">(E176-D176)*24*60</f>
+        <f t="shared" ref="F176:F187" si="6">(E176-D176)*24*60</f>
         <v>135</v>
       </c>
       <c r="G176" s="2">
-        <f t="shared" ref="G176:G186" si="7">F176/60</f>
+        <f t="shared" ref="G176:G187" si="7">F176/60</f>
         <v>2.25</v>
       </c>
     </row>
@@ -5068,39 +5068,64 @@
       <c r="D187" s="1">
         <v>0.84027777777777779</v>
       </c>
-      <c r="E187" s="1"/>
-      <c r="F187" s="3"/>
+      <c r="E187" s="1">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="F187" s="3">
+        <f t="shared" si="6"/>
+        <v>125.00000000000003</v>
+      </c>
+      <c r="G187" s="2">
+        <f t="shared" si="7"/>
+        <v>2.0833333333333339</v>
+      </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D188" s="1"/>
+      <c r="A188">
+        <v>2014</v>
+      </c>
+      <c r="B188">
+        <v>8</v>
+      </c>
+      <c r="C188" s="3">
+        <v>19</v>
+      </c>
+      <c r="D188" s="1">
+        <v>0.40625</v>
+      </c>
       <c r="E188" s="1"/>
       <c r="F188" s="3"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E189" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F189" s="3">
-        <f>SUM(F2:F186)</f>
-        <v>21025</v>
-      </c>
+      <c r="D189" s="1"/>
+      <c r="E189" s="1"/>
+      <c r="F189" s="3"/>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E190" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F190" s="2">
-        <f>F189/60</f>
-        <v>350.41666666666669</v>
+        <v>6</v>
+      </c>
+      <c r="F190" s="3">
+        <f>SUM(F2:F187)</f>
+        <v>21150</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E191" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F191" s="2">
+        <f>F190/60</f>
+        <v>352.5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E192" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F191" s="2">
-        <f>F190/38.5</f>
-        <v>9.1017316017316023</v>
+      <c r="F192" s="2">
+        <f>F191/38.5</f>
+        <v>9.1558441558441555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added transmission equation model to the database
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H192"/>
+  <dimension ref="A1:H193"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="I188" sqref="I188"/>
+      <selection activeCell="H190" sqref="H190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5097,34 +5097,50 @@
       <c r="F188" s="3"/>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D189" s="1"/>
+      <c r="A189">
+        <v>2014</v>
+      </c>
+      <c r="B189">
+        <v>8</v>
+      </c>
+      <c r="C189" s="3">
+        <v>20</v>
+      </c>
+      <c r="D189" s="1">
+        <v>0.34027777777777773</v>
+      </c>
       <c r="E189" s="1"/>
       <c r="F189" s="3"/>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E190" s="4" t="s">
+      <c r="D190" s="1"/>
+      <c r="E190" s="1"/>
+      <c r="F190" s="3"/>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E191" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F190" s="3">
+      <c r="F191" s="3">
         <f>SUM(F2:F187)</f>
         <v>21150</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E191" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F191" s="2">
-        <f>F190/60</f>
-        <v>352.5</v>
-      </c>
-    </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E192" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F192" s="2">
+        <f>F191/60</f>
+        <v>352.5</v>
+      </c>
+    </row>
+    <row r="193" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E193" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F192" s="2">
-        <f>F191/38.5</f>
+      <c r="F193" s="2">
+        <f>F192/38.5</f>
         <v>9.1558441558441555</v>
       </c>
     </row>

</xml_diff>

<commit_message>
improved selection unit in ui
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -397,7 +397,7 @@
   <dimension ref="A1:H189"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183"/>
+      <selection activeCell="E186" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4797,11 +4797,11 @@
         <v>0.88541666666666663</v>
       </c>
       <c r="F176" s="3">
-        <f t="shared" ref="F176:F184" si="6">(E176-D176)*24*60</f>
+        <f t="shared" ref="F176:F185" si="6">(E176-D176)*24*60</f>
         <v>135</v>
       </c>
       <c r="G176" s="2">
-        <f t="shared" ref="G176:G184" si="7">F176/60</f>
+        <f t="shared" ref="G176:G185" si="7">F176/60</f>
         <v>2.25</v>
       </c>
     </row>
@@ -5018,8 +5018,17 @@
       <c r="D185" s="1">
         <v>0.3888888888888889</v>
       </c>
-      <c r="E185" s="1"/>
-      <c r="F185" s="3"/>
+      <c r="E185" s="1">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="F185" s="3">
+        <f t="shared" si="6"/>
+        <v>135</v>
+      </c>
+      <c r="G185" s="2">
+        <f t="shared" si="7"/>
+        <v>2.25</v>
+      </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D186" s="1"/>
@@ -5031,8 +5040,8 @@
         <v>6</v>
       </c>
       <c r="F187" s="3">
-        <f>SUM(F2:F175)</f>
-        <v>19815</v>
+        <f>SUM(F2:F185)</f>
+        <v>20860</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
@@ -5041,7 +5050,7 @@
       </c>
       <c r="F188" s="2">
         <f>F187/60</f>
-        <v>330.25</v>
+        <v>347.66666666666669</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -5050,7 +5059,7 @@
       </c>
       <c r="F189" s="2">
         <f>F188/38.5</f>
-        <v>8.5779220779220786</v>
+        <v>9.0303030303030312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added power point presentation
</commit_message>
<xml_diff>
--- a/documents/working_hours.xlsx
+++ b/documents/working_hours.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H193"/>
+  <dimension ref="A1:H194"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="K191" sqref="K191"/>
+      <selection activeCell="F190" sqref="F190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5097,11 +5097,11 @@
         <v>0.4375</v>
       </c>
       <c r="F188" s="3">
-        <f t="shared" ref="F188:F189" si="8">(E188-D188)*24*60</f>
+        <f t="shared" ref="F188:F190" si="8">(E188-D188)*24*60</f>
         <v>45</v>
       </c>
       <c r="G188" s="2">
-        <f t="shared" ref="G188:G189" si="9">F188/60</f>
+        <f t="shared" ref="G188:G190" si="9">F188/60</f>
         <v>0.75</v>
       </c>
     </row>
@@ -5131,34 +5131,59 @@
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D190" s="1"/>
-      <c r="E190" s="1"/>
-      <c r="F190" s="3"/>
+      <c r="A190">
+        <v>2014</v>
+      </c>
+      <c r="B190">
+        <v>9</v>
+      </c>
+      <c r="C190" s="3">
+        <v>8</v>
+      </c>
+      <c r="D190" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="E190" s="1">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F190" s="3">
+        <f t="shared" si="8"/>
+        <v>74.999999999999972</v>
+      </c>
+      <c r="G190" s="2">
+        <f t="shared" si="9"/>
+        <v>1.2499999999999996</v>
+      </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E191" s="4" t="s">
+      <c r="D191" s="1"/>
+      <c r="E191" s="1"/>
+      <c r="F191" s="3"/>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E192" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F191" s="3">
+      <c r="F192" s="3">
         <f>SUM(F2:F187)</f>
         <v>21150</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E192" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F192" s="2">
-        <f>F191/60</f>
-        <v>352.5</v>
-      </c>
-    </row>
     <row r="193" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E193" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F193" s="2">
+        <f>F192/60</f>
+        <v>352.5</v>
+      </c>
+    </row>
+    <row r="194" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E194" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F193" s="2">
-        <f>F192/38.5</f>
+      <c r="F194" s="2">
+        <f>F193/38.5</f>
         <v>9.1558441558441555</v>
       </c>
     </row>

</xml_diff>